<commit_message>
Year, Months and Weeks headers added
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -26,18 +26,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFA500"/>
-        <bgColor rgb="00FFA500"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,36 +422,156 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n"/>
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="B2" s="1" t="n"/>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="D4" s="1" t="n"/>
-      <c r="E4" s="1" t="n"/>
-    </row>
-    <row r="5">
-      <c r="E5" s="1" t="n"/>
-    </row>
-    <row r="6">
-      <c r="E6" s="1" t="n"/>
-      <c r="F6" s="1" t="n"/>
-    </row>
-    <row r="7">
-      <c r="F7" s="1" t="n"/>
-      <c r="G7" s="1" t="n"/>
-    </row>
-    <row r="8">
-      <c r="G8" s="1" t="n"/>
-      <c r="H8" s="1" t="n"/>
-      <c r="I8" s="1" t="n"/>
-      <c r="J8" s="1" t="n"/>
-      <c r="K8" s="1" t="n"/>
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Weeks with and without input
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,13 +25,34 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000070c0"/>
+        <bgColor rgb="000070c0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000070C0"/>
+        <bgColor rgb="000070C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFA500"/>
+        <bgColor rgb="00FFA500"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +67,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,167 +441,103 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="B1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr"/>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>_</t>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>_</t>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Week 1</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Week 2</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Week 3</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Week 4</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Week 5</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>Week 6</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Week 7</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>Week 8</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>Week 9</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
+      <c r="B3" s="3" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="C4" s="3" t="n"/>
+    </row>
+    <row r="5">
+      <c r="D5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="E6" s="3" t="n"/>
+    </row>
+    <row r="7">
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="I8" s="3" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:J1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added start date end date
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:L9"/>
+  <dimension ref="B1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,9 @@
     <col width="15" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="15" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -474,9 +477,19 @@
           <t>Tasks</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>End Date</t>
+        </is>
+      </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2022</t>
         </is>
       </c>
     </row>
@@ -491,6 +504,11 @@
           <t>Month 2</t>
         </is>
       </c>
+      <c r="N2" s="3" t="inlineStr">
+        <is>
+          <t>Month 3</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="F3" s="4" t="inlineStr">
@@ -526,6 +544,21 @@
       <c r="L3" s="4" t="inlineStr">
         <is>
           <t>Week 7</t>
+        </is>
+      </c>
+      <c r="M3" s="4" t="inlineStr">
+        <is>
+          <t>Week 8</t>
+        </is>
+      </c>
+      <c r="N3" s="4" t="inlineStr">
+        <is>
+          <t>Week 9</t>
+        </is>
+      </c>
+      <c r="O3" s="4" t="inlineStr">
+        <is>
+          <t>Week 10</t>
         </is>
       </c>
     </row>
@@ -563,14 +596,37 @@
       <c r="B9" t="n">
         <v>6</v>
       </c>
+      <c r="J9" s="5" t="n"/>
       <c r="K9" s="5" t="n"/>
     </row>
+    <row r="10">
+      <c r="B10" t="n">
+        <v>7</v>
+      </c>
+      <c r="L10" s="5" t="n"/>
+      <c r="M10" s="5" t="n"/>
+    </row>
+    <row r="11">
+      <c r="B11" t="n">
+        <v>8</v>
+      </c>
+      <c r="M11" s="5" t="n"/>
+    </row>
+    <row r="12">
+      <c r="B12" t="n">
+        <v>9</v>
+      </c>
+      <c r="N12" s="5" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="F1:O1"/>
     <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update added task names
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:J7"/>
+  <dimension ref="B1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,8 +462,6 @@
     <col width="15" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -496,39 +494,24 @@
     <row r="2">
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>December</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>January</t>
+          <t>Month 1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>26/Dec - 01/Jan</t>
+          <t>Week 1</t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t>02/Jan - 08/Jan</t>
+          <t>Week 2</t>
         </is>
       </c>
       <c r="H3" s="4" t="inlineStr">
         <is>
-          <t>09/Jan - 15/Jan</t>
-        </is>
-      </c>
-      <c r="I3" s="4" t="inlineStr">
-        <is>
-          <t>16/Jan - 22/Jan</t>
-        </is>
-      </c>
-      <c r="J3" s="4" t="inlineStr">
-        <is>
-          <t>23/Jan - 29/Jan</t>
+          <t>Week 3</t>
         </is>
       </c>
     </row>
@@ -539,16 +522,6 @@
       <c r="C4" t="inlineStr">
         <is>
           <t>demo</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>12/26</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>01/01</t>
         </is>
       </c>
       <c r="F4" s="5" t="n"/>
@@ -562,58 +535,15 @@
           <t>init</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>01/02</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>01/08</t>
-        </is>
-      </c>
       <c r="G5" s="5" t="n"/>
     </row>
-    <row r="6">
-      <c r="B6" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>01/09</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>01/15</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="n"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>01/16</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>01/22</t>
-        </is>
-      </c>
-      <c r="I7" s="5" t="n"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed February Leap Dates
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -33,7 +33,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -44,12 +44,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="000070C0"/>
         <bgColor rgb="000070C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="000070c0"/>
-        <bgColor rgb="000070c0"/>
       </patternFill>
     </fill>
     <fill>
@@ -71,7 +65,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
@@ -79,16 +73,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -454,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:K8"/>
+  <dimension ref="B1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,6 +463,11 @@
     <col width="18" customWidth="1" min="9" max="9"/>
     <col width="18" customWidth="1" min="10" max="10"/>
     <col width="18" customWidth="1" min="11" max="11"/>
+    <col width="18" customWidth="1" min="12" max="12"/>
+    <col width="18" customWidth="1" min="13" max="13"/>
+    <col width="18" customWidth="1" min="14" max="14"/>
+    <col width="18" customWidth="1" min="15" max="15"/>
+    <col width="18" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -504,160 +500,256 @@
     <row r="2">
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>February</t>
         </is>
       </c>
       <c r="K2" s="3" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="O2" s="3" t="inlineStr">
+        <is>
+          <t>April</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>01/May - 07/May</t>
-        </is>
-      </c>
-      <c r="G3" s="4" t="inlineStr">
-        <is>
-          <t>08/May - 14/May</t>
-        </is>
-      </c>
-      <c r="H3" s="4" t="inlineStr">
-        <is>
-          <t>15/May - 21/May</t>
-        </is>
-      </c>
-      <c r="I3" s="4" t="inlineStr">
-        <is>
-          <t>22/May - 28/May</t>
-        </is>
-      </c>
-      <c r="J3" s="4" t="inlineStr">
-        <is>
-          <t>29/May - 04/Jun</t>
-        </is>
-      </c>
-      <c r="K3" s="4" t="inlineStr">
-        <is>
-          <t>05/Jun - 11/Jun</t>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>01/Feb - 07/Feb</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>08/Feb - 14/Feb</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>15/Feb - 21/Feb</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>22/Feb - 28/Feb</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>29/Feb - 06/Mar</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>07/Mar - 13/Mar</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>14/Mar - 20/Mar</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>21/Mar - 27/Mar</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>28/Mar - 03/Apr</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>04/Apr - 10/Apr</t>
+        </is>
+      </c>
+      <c r="P3" s="3" t="inlineStr">
+        <is>
+          <t>11/Apr - 17/Apr</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>Demo</t>
-        </is>
-      </c>
+      <c r="C4" s="4" t="n"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05/01</t>
+          <t>02/01</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>05/07</t>
-        </is>
-      </c>
-      <c r="F4" s="6" t="n"/>
+          <t>02/07</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>Meeting</t>
-        </is>
-      </c>
+      <c r="C5" s="4" t="n"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>05/08</t>
+          <t>02/08</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>05/14</t>
-        </is>
-      </c>
-      <c r="G5" s="6" t="n"/>
+          <t>02/14</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>KickOff</t>
-        </is>
-      </c>
+      <c r="C6" s="4" t="n"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>05/15</t>
+          <t>02/15</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>05/21</t>
-        </is>
-      </c>
-      <c r="H6" s="6" t="n"/>
+          <t>02/21</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Implement</t>
-        </is>
-      </c>
+      <c r="C7" s="4" t="n"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>05/22</t>
+          <t>02/22</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>05/28</t>
-        </is>
-      </c>
-      <c r="I7" s="6" t="n"/>
+          <t>02/28</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
+      <c r="C8" s="4" t="n"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>05/29</t>
+          <t>02/29</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>06/04</t>
-        </is>
-      </c>
-      <c r="J8" s="6" t="n"/>
+          <t>03/06</t>
+        </is>
+      </c>
+      <c r="J8" s="5" t="n"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="n"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>03/07</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>03/13</t>
+        </is>
+      </c>
+      <c r="K9" s="5" t="n"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>03/14</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>03/20</t>
+        </is>
+      </c>
+      <c r="L10" s="5" t="n"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="n"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>03/21</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>03/27</t>
+        </is>
+      </c>
+      <c r="M11" s="5" t="n"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="n"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>03/28</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>04/03</t>
+        </is>
+      </c>
+      <c r="N12" s="5" t="n"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="n"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>04/04</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>04/10</t>
+        </is>
+      </c>
+      <c r="O13" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="F1:P1"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="K2:N2"/>
     <mergeCell ref="E1:E3"/>
-    <mergeCell ref="K2"/>
     <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix year range headers
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -493,81 +493,86 @@
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023-2024</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="F2" s="3" t="inlineStr">
         <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>January</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="inlineStr">
+        <is>
           <t>February</t>
         </is>
       </c>
-      <c r="K2" s="3" t="inlineStr">
+      <c r="P2" s="3" t="inlineStr">
         <is>
           <t>March</t>
-        </is>
-      </c>
-      <c r="O2" s="3" t="inlineStr">
-        <is>
-          <t>April</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>01/Feb - 07/Feb</t>
+          <t>25/Dec - 31/Dec</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>08/Feb - 14/Feb</t>
+          <t>01/Jan - 07/Jan</t>
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>15/Feb - 21/Feb</t>
+          <t>08/Jan - 14/Jan</t>
         </is>
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>22/Feb - 28/Feb</t>
+          <t>15/Jan - 21/Jan</t>
         </is>
       </c>
       <c r="J3" s="3" t="inlineStr">
         <is>
-          <t>29/Feb - 06/Mar</t>
+          <t>22/Jan - 28/Jan</t>
         </is>
       </c>
       <c r="K3" s="3" t="inlineStr">
         <is>
-          <t>07/Mar - 13/Mar</t>
+          <t>29/Jan - 04/Feb</t>
         </is>
       </c>
       <c r="L3" s="3" t="inlineStr">
         <is>
-          <t>14/Mar - 20/Mar</t>
+          <t>05/Feb - 11/Feb</t>
         </is>
       </c>
       <c r="M3" s="3" t="inlineStr">
         <is>
-          <t>21/Mar - 27/Mar</t>
+          <t>12/Feb - 18/Feb</t>
         </is>
       </c>
       <c r="N3" s="3" t="inlineStr">
         <is>
-          <t>28/Mar - 03/Apr</t>
+          <t>19/Feb - 25/Feb</t>
         </is>
       </c>
       <c r="O3" s="3" t="inlineStr">
         <is>
-          <t>04/Apr - 10/Apr</t>
+          <t>26/Feb - 03/Mar</t>
         </is>
       </c>
       <c r="P3" s="3" t="inlineStr">
         <is>
-          <t>11/Apr - 17/Apr</t>
+          <t>04/Mar - 10/Mar</t>
         </is>
       </c>
     </row>
@@ -578,12 +583,12 @@
       <c r="C4" s="4" t="n"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>02/01</t>
+          <t>12/25</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>02/07</t>
+          <t>12/31</t>
         </is>
       </c>
       <c r="F4" s="5" t="n"/>
@@ -595,12 +600,12 @@
       <c r="C5" s="4" t="n"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>02/08</t>
+          <t>01/01</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>02/14</t>
+          <t>01/07</t>
         </is>
       </c>
       <c r="G5" s="5" t="n"/>
@@ -612,12 +617,12 @@
       <c r="C6" s="4" t="n"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>02/15</t>
+          <t>01/08</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>02/21</t>
+          <t>01/14</t>
         </is>
       </c>
       <c r="H6" s="5" t="n"/>
@@ -629,12 +634,12 @@
       <c r="C7" s="4" t="n"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>02/22</t>
+          <t>01/15</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>02/28</t>
+          <t>01/21</t>
         </is>
       </c>
       <c r="I7" s="5" t="n"/>
@@ -646,12 +651,12 @@
       <c r="C8" s="4" t="n"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>02/29</t>
+          <t>01/22</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>03/06</t>
+          <t>01/28</t>
         </is>
       </c>
       <c r="J8" s="5" t="n"/>
@@ -663,12 +668,12 @@
       <c r="C9" s="4" t="n"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>03/07</t>
+          <t>01/29</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>03/13</t>
+          <t>02/04</t>
         </is>
       </c>
       <c r="K9" s="5" t="n"/>
@@ -680,12 +685,12 @@
       <c r="C10" s="4" t="n"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>03/14</t>
+          <t>02/05</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>03/20</t>
+          <t>02/11</t>
         </is>
       </c>
       <c r="L10" s="5" t="n"/>
@@ -697,12 +702,12 @@
       <c r="C11" s="4" t="n"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>03/21</t>
+          <t>02/12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>03/27</t>
+          <t>02/18</t>
         </is>
       </c>
       <c r="M11" s="5" t="n"/>
@@ -714,12 +719,12 @@
       <c r="C12" s="4" t="n"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>03/28</t>
+          <t>02/19</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>04/03</t>
+          <t>02/25</t>
         </is>
       </c>
       <c r="N12" s="5" t="n"/>
@@ -731,26 +736,27 @@
       <c r="C13" s="4" t="n"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>04/04</t>
+          <t>02/26</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>04/10</t>
+          <t>03/04</t>
         </is>
       </c>
       <c r="O13" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="F1:P1"/>
-    <mergeCell ref="O2:P2"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2"/>
     <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed empty input start week case
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -65,7 +65,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
@@ -76,6 +76,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -445,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:Q13"/>
+  <dimension ref="B1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +469,6 @@
     <col width="20" customWidth="1" min="14" max="14"/>
     <col width="20" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -497,277 +497,161 @@
           <t>2024</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>December</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-      <c r="L2" s="3" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
-      <c r="P2" s="3" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
+          <t>Month 1</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>Month 2</t>
+        </is>
+      </c>
+      <c r="N2" s="3" t="inlineStr">
+        <is>
+          <t>Month 3</t>
+        </is>
+      </c>
+      <c r="P2" s="4" t="n"/>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>25/Dec - 31/Dec</t>
+          <t>Week 1</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>01/Jan - 07/Jan</t>
+          <t>Week 2</t>
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>08/Jan - 14/Jan</t>
+          <t>Week 3</t>
         </is>
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>15/Jan - 21/Jan</t>
+          <t>Week 4</t>
         </is>
       </c>
       <c r="J3" s="3" t="inlineStr">
         <is>
-          <t>22/Jan - 28/Jan</t>
+          <t>Week 5</t>
         </is>
       </c>
       <c r="K3" s="3" t="inlineStr">
         <is>
-          <t>29/Jan - 04/Feb</t>
+          <t>Week 6</t>
         </is>
       </c>
       <c r="L3" s="3" t="inlineStr">
         <is>
-          <t>05/Feb - 11/Feb</t>
+          <t>Week 7</t>
         </is>
       </c>
       <c r="M3" s="3" t="inlineStr">
         <is>
-          <t>12/Feb - 18/Feb</t>
+          <t>Week 8</t>
         </is>
       </c>
       <c r="N3" s="3" t="inlineStr">
         <is>
-          <t>19/Feb - 25/Feb</t>
+          <t>Week 9</t>
         </is>
       </c>
       <c r="O3" s="3" t="inlineStr">
         <is>
-          <t>26/Feb - 04/Mar</t>
+          <t>Week 10</t>
         </is>
       </c>
       <c r="P3" s="3" t="inlineStr">
         <is>
-          <t>05/Mar - 11/Mar</t>
-        </is>
-      </c>
-      <c r="Q3" s="3" t="inlineStr">
-        <is>
-          <t>12/Mar - 18/Mar</t>
+          <t>Week 11</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>12/25</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>12/31</t>
-        </is>
-      </c>
-      <c r="F4" s="5" t="n"/>
+      <c r="C4" s="5" t="n"/>
+      <c r="F4" s="6" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>01/01</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>01/07</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="n"/>
+      <c r="C5" s="5" t="n"/>
+      <c r="G5" s="6" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>01/08</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>01/14</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="n"/>
+      <c r="C6" s="5" t="n"/>
+      <c r="H6" s="6" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>01/15</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>01/21</t>
-        </is>
-      </c>
-      <c r="I7" s="5" t="n"/>
+      <c r="C7" s="5" t="n"/>
+      <c r="I7" s="6" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>01/22</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>01/28</t>
-        </is>
-      </c>
-      <c r="J8" s="5" t="n"/>
+      <c r="C8" s="5" t="n"/>
+      <c r="J8" s="6" t="n"/>
     </row>
     <row r="9">
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>01/29</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>02/04</t>
-        </is>
-      </c>
-      <c r="K9" s="5" t="n"/>
+      <c r="C9" s="5" t="n"/>
+      <c r="K9" s="6" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>02/05</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>02/11</t>
-        </is>
-      </c>
-      <c r="L10" s="5" t="n"/>
+      <c r="C10" s="5" t="n"/>
+      <c r="L10" s="6" t="n"/>
     </row>
     <row r="11">
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="n"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>02/12</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>02/18</t>
-        </is>
-      </c>
-      <c r="M11" s="5" t="n"/>
+      <c r="C11" s="5" t="n"/>
+      <c r="M11" s="6" t="n"/>
     </row>
     <row r="12">
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="C12" s="4" t="n"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>02/19</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>02/25</t>
-        </is>
-      </c>
-      <c r="N12" s="5" t="n"/>
+      <c r="C12" s="5" t="n"/>
+      <c r="N12" s="6" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="4" t="n">
+      <c r="B13" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="C13" s="4" t="n"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>02/26</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>03/04</t>
-        </is>
-      </c>
-      <c r="O13" s="5" t="n"/>
+      <c r="C13" s="5" t="n"/>
+      <c r="O13" s="6" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="F1"/>
+  <mergeCells count="8">
+    <mergeCell ref="F1:P1"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="J2:M2"/>
     <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Validation input task hours fix
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:P13"/>
+  <dimension ref="B1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,15 +460,6 @@
     <col width="10" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -504,17 +495,7 @@
           <t>Month 1</t>
         </is>
       </c>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>Month 2</t>
-        </is>
-      </c>
-      <c r="N2" s="3" t="inlineStr">
-        <is>
-          <t>Month 3</t>
-        </is>
-      </c>
-      <c r="P2" s="4" t="n"/>
+      <c r="G2" s="4" t="n"/>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
@@ -525,51 +506,6 @@
       <c r="G3" s="3" t="inlineStr">
         <is>
           <t>Week 2</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>Week 3</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t>Week 4</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>Week 5</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="inlineStr">
-        <is>
-          <t>Week 6</t>
-        </is>
-      </c>
-      <c r="L3" s="3" t="inlineStr">
-        <is>
-          <t>Week 7</t>
-        </is>
-      </c>
-      <c r="M3" s="3" t="inlineStr">
-        <is>
-          <t>Week 8</t>
-        </is>
-      </c>
-      <c r="N3" s="3" t="inlineStr">
-        <is>
-          <t>Week 9</t>
-        </is>
-      </c>
-      <c r="O3" s="3" t="inlineStr">
-        <is>
-          <t>Week 10</t>
-        </is>
-      </c>
-      <c r="P3" s="3" t="inlineStr">
-        <is>
-          <t>Week 11</t>
         </is>
       </c>
     </row>
@@ -580,79 +516,14 @@
       <c r="C4" s="5" t="n"/>
       <c r="F4" s="6" t="n"/>
     </row>
-    <row r="5">
-      <c r="B5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="n"/>
-      <c r="G5" s="6" t="n"/>
-    </row>
-    <row r="6">
-      <c r="B6" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5" t="n"/>
-      <c r="H6" s="6" t="n"/>
-    </row>
-    <row r="7">
-      <c r="B7" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="n"/>
-      <c r="I7" s="6" t="n"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5" t="n"/>
-      <c r="J8" s="6" t="n"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5" t="n"/>
-      <c r="K9" s="6" t="n"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="n"/>
-      <c r="L10" s="6" t="n"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="C11" s="5" t="n"/>
-      <c r="M11" s="6" t="n"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5" t="n"/>
-      <c r="N12" s="6" t="n"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="C13" s="5" t="n"/>
-      <c r="O13" s="6" t="n"/>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F1:P1"/>
+  <mergeCells count="6">
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="F2"/>
     <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix activity input whitespace issue
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -65,7 +65,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
@@ -76,7 +76,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -446,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:G4"/>
+  <dimension ref="B1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,10 +455,21 @@
   <cols>
     <col width="5" customWidth="1" min="2" max="2"/>
     <col width="30" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -488,42 +498,358 @@
           <t>2024</t>
         </is>
       </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>Month 1</t>
-        </is>
-      </c>
-      <c r="G2" s="4" t="n"/>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>January</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="inlineStr">
+        <is>
+          <t>February</t>
+        </is>
+      </c>
+      <c r="P2" s="3" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>Week 1</t>
+          <t>25/Dec - 31/Dec</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>Week 2</t>
+          <t>01/Jan - 07/Jan</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>08/Jan - 14/Jan</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>15/Jan - 21/Jan</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>22/Jan - 28/Jan</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>29/Jan - 04/Feb</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>05/Feb - 11/Feb</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>12/Feb - 18/Feb</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>19/Feb - 25/Feb</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>26/Feb - 04/Mar</t>
+        </is>
+      </c>
+      <c r="P3" s="3" t="inlineStr">
+        <is>
+          <t>05/Mar - 11/Mar</t>
+        </is>
+      </c>
+      <c r="Q3" s="3" t="inlineStr">
+        <is>
+          <t>12/Mar - 18/Mar</t>
+        </is>
+      </c>
+      <c r="R3" s="3" t="inlineStr">
+        <is>
+          <t>19/Mar - 25/Mar</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="n"/>
-      <c r="F4" s="6" t="n"/>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Kick Off</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>12/25</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>12/31</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="n"/>
+    </row>
+    <row r="5">
+      <c r="B5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>01/01</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>01/07</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="n"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>01/08</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>01/14</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="n"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>01/15</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>02/04</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="n"/>
+      <c r="J7" s="5" t="n"/>
+      <c r="K7" s="5" t="n"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>02/05</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>03/04</t>
+        </is>
+      </c>
+      <c r="L8" s="5" t="n"/>
+      <c r="M8" s="5" t="n"/>
+      <c r="N8" s="5" t="n"/>
+      <c r="O8" s="5" t="n"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>03/05</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>03/11</t>
+        </is>
+      </c>
+      <c r="P9" s="5" t="n"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>Demo</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>03/05</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>03/11</t>
+        </is>
+      </c>
+      <c r="P10" s="5" t="n"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>03/12</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>03/18</t>
+        </is>
+      </c>
+      <c r="Q11" s="5" t="n"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>Prod</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>03/12</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>03/18</t>
+        </is>
+      </c>
+      <c r="Q12" s="5" t="n"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="n"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>03/12</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>03/18</t>
+        </is>
+      </c>
+      <c r="Q13" s="5" t="n"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="n"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>03/12</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>03/18</t>
+        </is>
+      </c>
+      <c r="Q14" s="5" t="n"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="n"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>03/12</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>03/18</t>
+        </is>
+      </c>
+      <c r="Q15" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="F1"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
+    <mergeCell ref="G1:R1"/>
     <mergeCell ref="F2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:O2"/>
     <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix issue month header length when no start week input
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:R15"/>
+  <dimension ref="B1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,12 +464,6 @@
     <col width="20" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
     <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
-    <col width="20" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -520,16 +514,11 @@
           <t>February</t>
         </is>
       </c>
-      <c r="P2" s="3" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>25/Dec - 31/Dec</t>
+          <t>26/Dec - 31/Dec</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -560,36 +549,6 @@
       <c r="L3" s="3" t="inlineStr">
         <is>
           <t>05/Feb - 11/Feb</t>
-        </is>
-      </c>
-      <c r="M3" s="3" t="inlineStr">
-        <is>
-          <t>12/Feb - 18/Feb</t>
-        </is>
-      </c>
-      <c r="N3" s="3" t="inlineStr">
-        <is>
-          <t>19/Feb - 25/Feb</t>
-        </is>
-      </c>
-      <c r="O3" s="3" t="inlineStr">
-        <is>
-          <t>26/Feb - 04/Mar</t>
-        </is>
-      </c>
-      <c r="P3" s="3" t="inlineStr">
-        <is>
-          <t>05/Mar - 11/Mar</t>
-        </is>
-      </c>
-      <c r="Q3" s="3" t="inlineStr">
-        <is>
-          <t>12/Mar - 18/Mar</t>
-        </is>
-      </c>
-      <c r="R3" s="3" t="inlineStr">
-        <is>
-          <t>19/Mar - 25/Mar</t>
         </is>
       </c>
     </row>
@@ -597,14 +556,10 @@
       <c r="B4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Kick Off</t>
-        </is>
-      </c>
+      <c r="C4" s="4" t="n"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12/25</t>
+          <t>12/26</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -618,11 +573,7 @@
       <c r="B5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+      <c r="C5" s="4" t="n"/>
       <c r="D5" t="inlineStr">
         <is>
           <t>01/01</t>
@@ -639,11 +590,7 @@
       <c r="B6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
+      <c r="C6" s="4" t="n"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>01/08</t>
@@ -660,11 +607,7 @@
       <c r="B7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
+      <c r="C7" s="4" t="n"/>
       <c r="D7" t="inlineStr">
         <is>
           <t>01/15</t>
@@ -672,183 +615,38 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>02/04</t>
+          <t>01/21</t>
         </is>
       </c>
       <c r="I7" s="5" t="n"/>
-      <c r="J7" s="5" t="n"/>
-      <c r="K7" s="5" t="n"/>
     </row>
     <row r="8">
       <c r="B8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
+      <c r="C8" s="4" t="n"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>02/05</t>
+          <t>01/22</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>03/04</t>
-        </is>
-      </c>
-      <c r="L8" s="5" t="n"/>
-      <c r="M8" s="5" t="n"/>
-      <c r="N8" s="5" t="n"/>
-      <c r="O8" s="5" t="n"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>03/05</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>03/11</t>
-        </is>
-      </c>
-      <c r="P9" s="5" t="n"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>Demo</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>03/05</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>03/11</t>
-        </is>
-      </c>
-      <c r="P10" s="5" t="n"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>03/12</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>03/18</t>
-        </is>
-      </c>
-      <c r="Q11" s="5" t="n"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="C12" s="4" t="inlineStr">
-        <is>
-          <t>Prod</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>03/12</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>03/18</t>
-        </is>
-      </c>
-      <c r="Q12" s="5" t="n"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="n"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>03/12</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>03/18</t>
-        </is>
-      </c>
-      <c r="Q13" s="5" t="n"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>03/12</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>03/18</t>
-        </is>
-      </c>
-      <c r="Q14" s="5" t="n"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>03/12</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>03/18</t>
-        </is>
-      </c>
-      <c r="Q15" s="5" t="n"/>
+          <t>01/28</t>
+        </is>
+      </c>
+      <c r="J8" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
+    <mergeCell ref="G1:L1"/>
     <mergeCell ref="F1"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="G1:R1"/>
     <mergeCell ref="F2"/>
-    <mergeCell ref="P2:R2"/>
     <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="L2"/>
     <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Tasks Separated by milestones
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:L8"/>
+  <dimension ref="B1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,9 +461,6 @@
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -492,162 +489,90 @@
           <t>2024</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>December</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-      <c r="L2" s="3" t="inlineStr">
-        <is>
-          <t>February</t>
+          <t>Month 1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>26/Dec - 31/Dec</t>
+          <t>Week 1</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>01/Jan - 07/Jan</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>08/Jan - 14/Jan</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t>15/Jan - 21/Jan</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>22/Jan - 28/Jan</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="inlineStr">
-        <is>
-          <t>29/Jan - 04/Feb</t>
-        </is>
-      </c>
-      <c r="L3" s="3" t="inlineStr">
-        <is>
-          <t>05/Feb - 11/Feb</t>
+          <t>Week 2</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>12/26</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>12/31</t>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Task 1</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>ML1 - T1</t>
         </is>
       </c>
       <c r="F4" s="5" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" s="4" t="n">
-        <v>2</v>
-      </c>
+      <c r="B5" s="4" t="n"/>
       <c r="C5" s="4" t="n"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>01/01</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>01/07</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>01/08</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>01/14</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="n"/>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Task 2</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>ML2 - X1</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>01/15</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>01/21</t>
-        </is>
-      </c>
-      <c r="I7" s="5" t="n"/>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Task 3</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>ML2 - X2</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>01/22</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>01/28</t>
-        </is>
-      </c>
-      <c r="J8" s="5" t="n"/>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Task 4</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>ML2 - X3</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="F1"/>
+  <mergeCells count="6">
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed get_week_dates, still week header bug milestones
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:I8"/>
+  <dimension ref="B1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,8 +459,6 @@
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -493,84 +491,128 @@
     <row r="2">
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>Month 1</t>
+          <t>January</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>Week 1</t>
+          <t>01/Jan - 07/Jan</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>Week 2</t>
+          <t>08/Jan - 14/Jan</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Task 1</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>ML1 - T1</t>
-        </is>
-      </c>
-      <c r="F4" s="5" t="n"/>
+      <c r="B4" s="4" t="n"/>
+      <c r="C4" s="4" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" s="4" t="n"/>
-      <c r="C5" s="4" t="n"/>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Task 1.1</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>M1 - T1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>01/01</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>01/07</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>Task 2</t>
+          <t>Task 1.2</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>ML2 - X1</t>
-        </is>
-      </c>
-      <c r="F6" s="5" t="n"/>
+          <t>M1 - T2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>01/08</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>01/14</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Task 3</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>ML2 - X2</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="n"/>
+      <c r="B7" s="4" t="n"/>
+      <c r="C7" s="4" t="n"/>
     </row>
     <row r="8">
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>Task 4</t>
+          <t>Task 2.1</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>ML2 - X3</t>
-        </is>
-      </c>
-      <c r="H8" s="5" t="n"/>
+          <t>M2 - X1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>01/15</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>01/21</t>
+        </is>
+      </c>
+      <c r="F8" s="5" t="n"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Task 2.2</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>M2 - X2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>01/22</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>01/28</t>
+        </is>
+      </c>
+      <c r="G9" s="5" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F2:I2"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Fix week headers multiple milestones
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -42,14 +42,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000070C0"/>
-        <bgColor rgb="000070C0"/>
+        <fgColor rgb="00FFA500"/>
+        <bgColor rgb="00FFA500"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFA500"/>
-        <bgColor rgb="00FFA500"/>
+        <fgColor rgb="000070C0"/>
+        <bgColor rgb="000070C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -67,19 +67,19 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:G9"/>
+  <dimension ref="B1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,8 +457,8 @@
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -506,6 +506,16 @@
           <t>08/Jan - 14/Jan</t>
         </is>
       </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>15/Jan - 21/Jan</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>22/Jan - 28/Jan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="4" t="n"/>
@@ -592,7 +602,7 @@
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>M2 - X2</t>
+          <t>M2 - X@</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -609,12 +619,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="F2:G2"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="C1:C3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adding debugging for checking weeks
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:I9"/>
+  <dimension ref="B1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,8 @@
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="16" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
+    <col width="16" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -494,6 +496,11 @@
           <t>January</t>
         </is>
       </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>February</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
@@ -514,6 +521,26 @@
       <c r="I3" s="3" t="inlineStr">
         <is>
           <t>22/Jan - 28/Jan</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>29/Jan - 04/Feb</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>05/Feb - 11/Feb</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>12/Feb - 18/Feb</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>19/Feb - 25/Feb</t>
         </is>
       </c>
     </row>
@@ -529,7 +556,7 @@
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>M1 - T1</t>
+          <t>M - A</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -552,7 +579,7 @@
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>M1 - T2</t>
+          <t>M - B</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -579,20 +606,20 @@
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>M2 - X1</t>
+          <t>N - C</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>01/15</t>
+          <t>02/12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>01/21</t>
-        </is>
-      </c>
-      <c r="F8" s="5" t="n"/>
+          <t>02/18</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="n"/>
     </row>
     <row r="9">
       <c r="B9" s="4" t="inlineStr">
@@ -602,29 +629,30 @@
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>M2 - X@</t>
+          <t>N - D</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>01/22</t>
+          <t>02/19</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>01/28</t>
-        </is>
-      </c>
-      <c r="G9" s="5" t="n"/>
+          <t>02/25</t>
+        </is>
+      </c>
+      <c r="I9" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B1:B3"/>
     <mergeCell ref="D1:D3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="F1:I1"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F2:I2"/>
     <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed col dates, task cell fills, week headers
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:M9"/>
+  <dimension ref="B1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,11 +496,6 @@
           <t>January</t>
         </is>
       </c>
-      <c r="K2" s="3" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
@@ -521,26 +516,6 @@
       <c r="I3" s="3" t="inlineStr">
         <is>
           <t>22/Jan - 28/Jan</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>29/Jan - 04/Feb</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="inlineStr">
-        <is>
-          <t>05/Feb - 11/Feb</t>
-        </is>
-      </c>
-      <c r="L3" s="3" t="inlineStr">
-        <is>
-          <t>12/Feb - 18/Feb</t>
-        </is>
-      </c>
-      <c r="M3" s="3" t="inlineStr">
-        <is>
-          <t>19/Feb - 25/Feb</t>
         </is>
       </c>
     </row>
@@ -611,12 +586,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>02/12</t>
+          <t>01/15</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>02/18</t>
+          <t>01/21</t>
         </is>
       </c>
       <c r="H8" s="5" t="n"/>
@@ -634,25 +609,24 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>02/19</t>
+          <t>01/22</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>02/25</t>
+          <t>01/28</t>
         </is>
       </c>
       <c r="I9" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="K2:M2"/>
+  <mergeCells count="6">
+    <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="C1:C3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added milestone task number and activity name
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -42,14 +42,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFA500"/>
-        <bgColor rgb="00FFA500"/>
+        <fgColor rgb="000070C0"/>
+        <bgColor rgb="000070C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000070C0"/>
-        <bgColor rgb="000070C0"/>
+        <fgColor rgb="00FFA500"/>
+        <bgColor rgb="00FFA500"/>
       </patternFill>
     </fill>
   </fills>
@@ -65,21 +65,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -445,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:I9"/>
+  <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,27 +527,16 @@
       <c r="C4" s="4" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Task 1.1</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>M - A</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>01/01</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>01/07</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="n"/>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Task 1</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="4" t="inlineStr">
@@ -554,79 +546,114 @@
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>M - B</t>
+          <t>M1 - A</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>01/01</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>01/07</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="n"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Task 1.1</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>M1 - B</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>01/08</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>01/14</t>
         </is>
       </c>
-      <c r="G6" s="5" t="n"/>
-    </row>
-    <row r="7">
-      <c r="B7" s="4" t="n"/>
-      <c r="C7" s="4" t="n"/>
+      <c r="G7" s="6" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>Task 2.1</t>
-        </is>
-      </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>N - C</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>01/15</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>01/21</t>
-        </is>
-      </c>
-      <c r="H8" s="5" t="n"/>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>Task 2</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>M2</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="4" t="inlineStr">
         <is>
+          <t>Task 2.1</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>M2 - C</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>01/15</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>01/21</t>
+        </is>
+      </c>
+      <c r="H9" s="6" t="n"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4" t="inlineStr">
+        <is>
           <t>Task 2.2</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>N - D</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>M2 - D</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>01/22</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>01/28</t>
         </is>
       </c>
-      <c r="I9" s="5" t="n"/>
+      <c r="I10" s="6" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="D1:D3"/>
+  <mergeCells count="10">
+    <mergeCell ref="B8"/>
+    <mergeCell ref="C8"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="E1:E3"/>
+    <mergeCell ref="B5"/>
+    <mergeCell ref="C5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added milestone start end dates
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -534,7 +534,17 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>01/01</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>01/14</t>
         </is>
       </c>
     </row>
@@ -546,7 +556,7 @@
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>M1 - A</t>
+          <t>M - A</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -569,7 +579,7 @@
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>M1 - B</t>
+          <t>M - B</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -592,7 +602,17 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>01/15</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>01/28</t>
         </is>
       </c>
     </row>
@@ -604,7 +624,7 @@
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>M2 - C</t>
+          <t>N - C</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -627,7 +647,7 @@
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>M2 - D</t>
+          <t>N - D</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">

</xml_diff>

<commit_message>
added task fills for milestones
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -534,7 +534,7 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -547,6 +547,8 @@
           <t>01/14</t>
         </is>
       </c>
+      <c r="F5" s="6" t="n"/>
+      <c r="G5" s="6" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="4" t="inlineStr">
@@ -556,7 +558,7 @@
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>M - A</t>
+          <t>M1 - A</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -579,7 +581,7 @@
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>M - B</t>
+          <t>M1 - B</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -602,7 +604,7 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -615,6 +617,8 @@
           <t>01/28</t>
         </is>
       </c>
+      <c r="H8" s="6" t="n"/>
+      <c r="I8" s="6" t="n"/>
     </row>
     <row r="9">
       <c r="B9" s="4" t="inlineStr">
@@ -624,7 +628,7 @@
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>N - C</t>
+          <t>M2 - C</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -647,7 +651,7 @@
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>N - D</t>
+          <t>M2 - D</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">

</xml_diff>

<commit_message>
Fixed for empty start week input
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,9 @@
     <col width="16" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
     <col width="16" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="16" customWidth="1" min="13" max="13"/>
+    <col width="16" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -538,6 +541,21 @@
           <t>05/Feb - 11/Feb</t>
         </is>
       </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>12/Feb - 18/Feb</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>19/Feb - 25/Feb</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>26/Feb - 03/Mar</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="4" t="n"/>
@@ -731,14 +749,110 @@
       </c>
       <c r="K12" s="6" t="n"/>
     </row>
+    <row r="13">
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Task 3</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>02/12</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>03/03</t>
+        </is>
+      </c>
+      <c r="L13" s="6" t="n"/>
+      <c r="M13" s="6" t="n"/>
+      <c r="N13" s="6" t="n"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>Task 3.4</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>M3 - G</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>02/12</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>02/18</t>
+        </is>
+      </c>
+      <c r="L14" s="6" t="n"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>Task 3.4</t>
+        </is>
+      </c>
+      <c r="C15" s="4" t="inlineStr">
+        <is>
+          <t>M3 - H</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>02/19</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>02/25</t>
+        </is>
+      </c>
+      <c r="M15" s="6" t="n"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>Task 3.4</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="inlineStr">
+        <is>
+          <t>M3 - I</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>02/26</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>03/03</t>
+        </is>
+      </c>
+      <c r="N16" s="6" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="B9"/>
+    <mergeCell ref="B13"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="K2"/>
-    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C13"/>
+    <mergeCell ref="F1:N1"/>
+    <mergeCell ref="K2:N2"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="B5"/>
     <mergeCell ref="C5"/>

</xml_diff>

<commit_message>
Fixed months weeks header when empty input week start date
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:I10"/>
+  <dimension ref="B1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,10 @@
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="16" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -499,6 +503,11 @@
           <t>January</t>
         </is>
       </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>February</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
@@ -519,6 +528,26 @@
       <c r="I3" s="3" t="inlineStr">
         <is>
           <t>22/Jan - 28/Jan</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>29/Jan - 04/Feb</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>05/Feb - 11/Feb</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>12/Feb - 18/Feb</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>19/Feb - 25/Feb</t>
         </is>
       </c>
     </row>
@@ -537,6 +566,19 @@
           <t>M1</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>01/01</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>01/21</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="n"/>
+      <c r="G5" s="6" t="n"/>
+      <c r="H5" s="6" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="4" t="inlineStr">
@@ -549,6 +591,16 @@
           <t>M1 - A</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>01/01</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>01/07</t>
+        </is>
+      </c>
       <c r="F6" s="6" t="n"/>
     </row>
     <row r="7">
@@ -562,58 +614,220 @@
           <t>M1 - B</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>01/08</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>01/14</t>
+        </is>
+      </c>
       <c r="G7" s="6" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>M1 - C</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>01/15</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>01/21</t>
+        </is>
+      </c>
+      <c r="H8" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>Task 2</t>
         </is>
       </c>
-      <c r="C8" s="5" t="inlineStr">
+      <c r="C9" s="5" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>2.1</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>M2 - C</t>
-        </is>
-      </c>
-      <c r="H9" s="6" t="n"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>01/22</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>02/11</t>
+        </is>
+      </c>
+      <c r="I9" s="6" t="n"/>
+      <c r="J9" s="6" t="n"/>
+      <c r="K9" s="6" t="n"/>
     </row>
     <row r="10">
       <c r="B10" s="4" t="inlineStr">
         <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>M2 - D</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>01/22</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>01/28</t>
+        </is>
+      </c>
+      <c r="I10" s="6" t="n"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="4" t="inlineStr">
+        <is>
           <t>2.2</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>M2 - D</t>
-        </is>
-      </c>
-      <c r="I10" s="6" t="n"/>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>M2 - E</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>01/29</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>02/04</t>
+        </is>
+      </c>
+      <c r="J11" s="6" t="n"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>2.3</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>M2 - F</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>02/05</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>02/11</t>
+        </is>
+      </c>
+      <c r="K12" s="6" t="n"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Task 3</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>02/12</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>02/25</t>
+        </is>
+      </c>
+      <c r="L13" s="6" t="n"/>
+      <c r="M13" s="6" t="n"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>3.1</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>M3 - G</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>02/12</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>02/18</t>
+        </is>
+      </c>
+      <c r="L14" s="6" t="n"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>3.2</t>
+        </is>
+      </c>
+      <c r="C15" s="4" t="inlineStr">
+        <is>
+          <t>M3 - H</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>02/19</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>02/25</t>
+        </is>
+      </c>
+      <c r="M15" s="6" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B8"/>
-    <mergeCell ref="C8"/>
+  <mergeCells count="13">
+    <mergeCell ref="K2:M2"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B9"/>
+    <mergeCell ref="B13"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
-    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="C13"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="B5"/>
     <mergeCell ref="C5"/>
+    <mergeCell ref="C9"/>
+    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
bold font on corresponding cells
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -17,13 +17,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00000000"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
     <font>
       <b val="1"/>
@@ -42,14 +49,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000070C0"/>
-        <bgColor rgb="000070C0"/>
+        <fgColor rgb="00FFA500"/>
+        <bgColor rgb="00FFA500"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFA500"/>
-        <bgColor rgb="00FFA500"/>
+        <fgColor rgb="000070C0"/>
+        <bgColor rgb="000070C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -65,24 +72,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -448,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:O18"/>
+  <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +464,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="5" customWidth="1" min="2" max="2"/>
+    <col width="7" customWidth="1" min="2" max="2"/>
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
@@ -464,12 +472,6 @@
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
-    <col width="16" customWidth="1" min="10" max="10"/>
-    <col width="16" customWidth="1" min="11" max="11"/>
-    <col width="16" customWidth="1" min="12" max="12"/>
-    <col width="16" customWidth="1" min="13" max="13"/>
-    <col width="16" customWidth="1" min="14" max="14"/>
-    <col width="16" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -505,16 +507,6 @@
           <t>January</t>
         </is>
       </c>
-      <c r="K2" s="3" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
-      <c r="O2" s="3" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="F3" s="3" t="inlineStr">
@@ -535,36 +527,6 @@
       <c r="I3" s="3" t="inlineStr">
         <is>
           <t>22/Jan - 28/Jan</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>29/Jan - 04/Feb</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="inlineStr">
-        <is>
-          <t>05/Feb - 11/Feb</t>
-        </is>
-      </c>
-      <c r="L3" s="3" t="inlineStr">
-        <is>
-          <t>12/Feb - 18/Feb</t>
-        </is>
-      </c>
-      <c r="M3" s="3" t="inlineStr">
-        <is>
-          <t>19/Feb - 25/Feb</t>
-        </is>
-      </c>
-      <c r="N3" s="3" t="inlineStr">
-        <is>
-          <t>26/Feb - 03/Mar</t>
-        </is>
-      </c>
-      <c r="O3" s="3" t="inlineStr">
-        <is>
-          <t>04/Mar - 10/Mar</t>
         </is>
       </c>
     </row>
@@ -580,23 +542,21 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>M1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
         <is>
           <t>01/01</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>01/28</t>
-        </is>
-      </c>
-      <c r="F5" s="6" t="n"/>
-      <c r="G5" s="6" t="n"/>
-      <c r="H5" s="6" t="n"/>
-      <c r="I5" s="6" t="n"/>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>01/14</t>
+        </is>
+      </c>
+      <c r="F5" s="7" t="n"/>
+      <c r="G5" s="7" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="4" t="inlineStr">
@@ -606,7 +566,7 @@
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>M1 - A</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -619,7 +579,7 @@
           <t>01/07</t>
         </is>
       </c>
-      <c r="F6" s="6" t="n"/>
+      <c r="F6" s="7" t="n"/>
     </row>
     <row r="7">
       <c r="B7" s="4" t="inlineStr">
@@ -629,7 +589,7 @@
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>M1 - B</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -642,282 +602,90 @@
           <t>01/14</t>
         </is>
       </c>
-      <c r="G7" s="6" t="n"/>
+      <c r="G7" s="7" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>1.3</t>
-        </is>
-      </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>M1 - C</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>Task 2</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D8" s="6" t="inlineStr">
         <is>
           <t>01/15</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>01/21</t>
-        </is>
-      </c>
-      <c r="H8" s="6" t="n"/>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>01/28</t>
+        </is>
+      </c>
+      <c r="H8" s="7" t="n"/>
+      <c r="I8" s="7" t="n"/>
     </row>
     <row r="9">
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>2.1</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>M1 - D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>01/15</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>01/21</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="n"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>2.2</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>01/22</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>01/28</t>
         </is>
       </c>
-      <c r="I9" s="6" t="n"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="5" t="inlineStr">
-        <is>
-          <t>Task 2</t>
-        </is>
-      </c>
-      <c r="C10" s="5" t="inlineStr">
-        <is>
-          <t>M2</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>01/29</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>02/18</t>
-        </is>
-      </c>
-      <c r="J10" s="6" t="n"/>
-      <c r="K10" s="6" t="n"/>
-      <c r="L10" s="6" t="n"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>2.1</t>
-        </is>
-      </c>
-      <c r="C11" s="4" t="inlineStr">
-        <is>
-          <t>M2 - E</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>01/29</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>02/04</t>
-        </is>
-      </c>
-      <c r="J11" s="6" t="n"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>2.2</t>
-        </is>
-      </c>
-      <c r="C12" s="4" t="inlineStr">
-        <is>
-          <t>M2 - F</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>02/05</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>02/11</t>
-        </is>
-      </c>
-      <c r="K12" s="6" t="n"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>2.3</t>
-        </is>
-      </c>
-      <c r="C13" s="4" t="inlineStr">
-        <is>
-          <t>M2 - G</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>02/12</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>02/18</t>
-        </is>
-      </c>
-      <c r="L13" s="6" t="n"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="5" t="inlineStr">
-        <is>
-          <t>Task 3</t>
-        </is>
-      </c>
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>02/19</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>03/03</t>
-        </is>
-      </c>
-      <c r="M14" s="6" t="n"/>
-      <c r="N14" s="6" t="n"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="C15" s="4" t="inlineStr">
-        <is>
-          <t>M3 - H</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>02/19</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>02/25</t>
-        </is>
-      </c>
-      <c r="M15" s="6" t="n"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>3.2</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>M3 - I</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>02/26</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>03/03</t>
-        </is>
-      </c>
-      <c r="N16" s="6" t="n"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="5" t="inlineStr">
-        <is>
-          <t>Task 4</t>
-        </is>
-      </c>
-      <c r="C17" s="5" t="inlineStr">
-        <is>
-          <t>M4</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>03/04</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>03/10</t>
-        </is>
-      </c>
-      <c r="O17" s="6" t="n"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="4" t="inlineStr">
-        <is>
-          <t>4.1</t>
-        </is>
-      </c>
-      <c r="C18" s="4" t="inlineStr">
-        <is>
-          <t>M4 - J</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>03/04</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>03/10</t>
-        </is>
-      </c>
-      <c r="O18" s="6" t="n"/>
+      <c r="I10" s="7" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="10">
+    <mergeCell ref="B8"/>
+    <mergeCell ref="C8"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
-    <mergeCell ref="B17"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C14"/>
-    <mergeCell ref="C17"/>
-    <mergeCell ref="F1:O1"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="O2"/>
-    <mergeCell ref="C10"/>
-    <mergeCell ref="B10"/>
-    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="B5"/>
-    <mergeCell ref="B14"/>
     <mergeCell ref="C5"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix start week dates issue
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -40,7 +40,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -55,12 +55,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="0032a852"/>
+        <bgColor rgb="0032a852"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="000070C0"/>
         <bgColor rgb="000070C0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -68,28 +74,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -542,7 +555,7 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="D5" s="6" t="inlineStr">
@@ -579,7 +592,7 @@
           <t>01/07</t>
         </is>
       </c>
-      <c r="F6" s="7" t="n"/>
+      <c r="F6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="B7" s="4" t="inlineStr">
@@ -602,7 +615,7 @@
           <t>01/14</t>
         </is>
       </c>
-      <c r="G7" s="7" t="n"/>
+      <c r="G7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="B8" s="5" t="inlineStr">
@@ -612,7 +625,7 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -649,7 +662,7 @@
           <t>01/21</t>
         </is>
       </c>
-      <c r="H9" s="7" t="n"/>
+      <c r="H9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="B10" s="4" t="inlineStr">
@@ -672,7 +685,7 @@
           <t>01/28</t>
         </is>
       </c>
-      <c r="I10" s="7" t="n"/>
+      <c r="I10" s="8" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Fix dates milestone issue
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -614,7 +614,12 @@
       <c r="A2" s="1" t="n"/>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>February</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>March</t>
         </is>
       </c>
       <c r="J2" s="1" t="n"/>
@@ -663,22 +668,22 @@
       <c r="A3" s="1" t="n"/>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>05/Apr - 11/Apr</t>
+          <t>25/Feb - 02/Mar</t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t>12/Apr - 18/Apr</t>
+          <t>03/Mar - 09/Mar</t>
         </is>
       </c>
       <c r="H3" s="4" t="inlineStr">
         <is>
-          <t>19/Apr - 25/Apr</t>
+          <t>10/Mar - 16/Mar</t>
         </is>
       </c>
       <c r="I3" s="4" t="inlineStr">
         <is>
-          <t>26/Apr - 02/May</t>
+          <t>17/Mar - 23/Mar</t>
         </is>
       </c>
       <c r="J3" s="1" t="n"/>
@@ -789,12 +794,12 @@
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
-          <t>04/05</t>
+          <t>02/25</t>
         </is>
       </c>
       <c r="E5" s="7" t="inlineStr">
         <is>
-          <t>04/18</t>
+          <t>03/09</t>
         </is>
       </c>
       <c r="F5" s="8" t="n"/>
@@ -857,12 +862,12 @@
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>04/05</t>
+          <t>02/25</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>04/11</t>
+          <t>03/02</t>
         </is>
       </c>
       <c r="F6" s="9" t="n"/>
@@ -925,12 +930,12 @@
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>04/12</t>
+          <t>03/03</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>04/18</t>
+          <t>03/09</t>
         </is>
       </c>
       <c r="F7" s="1" t="n"/>
@@ -993,12 +998,12 @@
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
-          <t>04/19</t>
+          <t>03/10</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>05/02</t>
+          <t>03/23</t>
         </is>
       </c>
       <c r="F8" s="1" t="n"/>
@@ -1061,12 +1066,12 @@
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>04/19</t>
+          <t>03/10</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>04/25</t>
+          <t>03/16</t>
         </is>
       </c>
       <c r="F9" s="1" t="n"/>
@@ -1129,12 +1134,12 @@
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>04/26</t>
+          <t>03/17</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>05/02</t>
+          <t>03/23</t>
         </is>
       </c>
       <c r="F10" s="1" t="n"/>
@@ -5864,14 +5869,15 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="B8"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="C8"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
-    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F2"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="B5"/>
     <mergeCell ref="C5"/>

</xml_diff>

<commit_message>
Fix dates issue for weeks and tasks
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -614,11 +614,6 @@
       <c r="A2" s="1" t="n"/>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t>February</t>
-        </is>
-      </c>
-      <c r="G2" s="4" t="inlineStr">
-        <is>
           <t>March</t>
         </is>
       </c>
@@ -668,22 +663,22 @@
       <c r="A3" s="1" t="n"/>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>25/Feb - 02/Mar</t>
+          <t>10/Mar - 16/Mar</t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t>03/Mar - 09/Mar</t>
+          <t>17/Mar - 23/Mar</t>
         </is>
       </c>
       <c r="H3" s="4" t="inlineStr">
         <is>
-          <t>10/Mar - 16/Mar</t>
+          <t>24/Mar - 30/Mar</t>
         </is>
       </c>
       <c r="I3" s="4" t="inlineStr">
         <is>
-          <t>17/Mar - 23/Mar</t>
+          <t>31/Mar - 06/Apr</t>
         </is>
       </c>
       <c r="J3" s="1" t="n"/>
@@ -794,12 +789,12 @@
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
-          <t>02/25</t>
+          <t>03/10</t>
         </is>
       </c>
       <c r="E5" s="7" t="inlineStr">
         <is>
-          <t>03/09</t>
+          <t>03/23</t>
         </is>
       </c>
       <c r="F5" s="8" t="n"/>
@@ -862,12 +857,12 @@
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>02/25</t>
+          <t>03/10</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>03/02</t>
+          <t>03/16</t>
         </is>
       </c>
       <c r="F6" s="9" t="n"/>
@@ -930,12 +925,12 @@
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>03/03</t>
+          <t>03/17</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>03/09</t>
+          <t>03/23</t>
         </is>
       </c>
       <c r="F7" s="1" t="n"/>
@@ -998,18 +993,18 @@
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
-          <t>03/10</t>
+          <t>03/24</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>03/23</t>
+          <t>03/30</t>
         </is>
       </c>
       <c r="F8" s="1" t="n"/>
       <c r="G8" s="1" t="n"/>
       <c r="H8" s="8" t="n"/>
-      <c r="I8" s="8" t="n"/>
+      <c r="I8" s="1" t="n"/>
       <c r="J8" s="1" t="n"/>
       <c r="K8" s="1" t="n"/>
       <c r="L8" s="1" t="n"/>
@@ -1066,12 +1061,12 @@
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>03/10</t>
+          <t>03/24</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>03/16</t>
+          <t>03/30</t>
         </is>
       </c>
       <c r="F9" s="1" t="n"/>
@@ -1134,18 +1129,18 @@
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>03/17</t>
+          <t>03/24</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>03/23</t>
+          <t>03/30</t>
         </is>
       </c>
       <c r="F10" s="1" t="n"/>
       <c r="G10" s="1" t="n"/>
-      <c r="H10" s="1" t="n"/>
-      <c r="I10" s="9" t="n"/>
+      <c r="H10" s="9" t="n"/>
+      <c r="I10" s="1" t="n"/>
       <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
       <c r="L10" s="1" t="n"/>
@@ -1190,14 +1185,30 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="5" t="n"/>
-      <c r="C11" s="5" t="n"/>
-      <c r="D11" s="1" t="n"/>
-      <c r="E11" s="1" t="n"/>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>Task 3</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>03/31</t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="inlineStr">
+        <is>
+          <t>04/06</t>
+        </is>
+      </c>
       <c r="F11" s="1" t="n"/>
       <c r="G11" s="1" t="n"/>
       <c r="H11" s="1" t="n"/>
-      <c r="I11" s="1" t="n"/>
+      <c r="I11" s="8" t="n"/>
       <c r="J11" s="1" t="n"/>
       <c r="K11" s="1" t="n"/>
       <c r="L11" s="1" t="n"/>
@@ -1242,14 +1253,30 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="5" t="n"/>
-      <c r="C12" s="5" t="n"/>
-      <c r="D12" s="1" t="n"/>
-      <c r="E12" s="1" t="n"/>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>3.1</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>03/31</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>04/06</t>
+        </is>
+      </c>
       <c r="F12" s="1" t="n"/>
       <c r="G12" s="1" t="n"/>
       <c r="H12" s="1" t="n"/>
-      <c r="I12" s="1" t="n"/>
+      <c r="I12" s="9" t="n"/>
       <c r="J12" s="1" t="n"/>
       <c r="K12" s="1" t="n"/>
       <c r="L12" s="1" t="n"/>
@@ -1294,14 +1321,30 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="1" t="n"/>
-      <c r="E13" s="1" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>3.2</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>03/31</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>04/06</t>
+        </is>
+      </c>
       <c r="F13" s="1" t="n"/>
       <c r="G13" s="1" t="n"/>
       <c r="H13" s="1" t="n"/>
-      <c r="I13" s="1" t="n"/>
+      <c r="I13" s="9" t="n"/>
       <c r="J13" s="1" t="n"/>
       <c r="K13" s="1" t="n"/>
       <c r="L13" s="1" t="n"/>
@@ -5869,15 +5912,16 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="B8"/>
-    <mergeCell ref="G2:I2"/>
     <mergeCell ref="C8"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
-    <mergeCell ref="F2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B11"/>
+    <mergeCell ref="C11"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="B5"/>
     <mergeCell ref="C5"/>

</xml_diff>

<commit_message>
Fix month gantt chart
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -97,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -110,11 +110,17 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -490,51 +496,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
+    <col width="7" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
-    <col width="20" customWidth="1" min="18" max="18"/>
-    <col width="20" customWidth="1" min="19" max="19"/>
-    <col width="20" customWidth="1" min="20" max="20"/>
-    <col width="20" customWidth="1" min="21" max="21"/>
-    <col width="20" customWidth="1" min="22" max="22"/>
-    <col width="20" customWidth="1" min="23" max="23"/>
-    <col width="20" customWidth="1" min="24" max="24"/>
-    <col width="20" customWidth="1" min="25" max="25"/>
-    <col width="20" customWidth="1" min="26" max="26"/>
-    <col width="20" customWidth="1" min="27" max="27"/>
-    <col width="20" customWidth="1" min="28" max="28"/>
-    <col width="20" customWidth="1" min="29" max="29"/>
-    <col width="20" customWidth="1" min="30" max="30"/>
-    <col width="20" customWidth="1" min="31" max="31"/>
-    <col width="20" customWidth="1" min="32" max="32"/>
-    <col width="20" customWidth="1" min="33" max="33"/>
-    <col width="20" customWidth="1" min="34" max="34"/>
-    <col width="20" customWidth="1" min="35" max="35"/>
-    <col width="20" customWidth="1" min="36" max="36"/>
-    <col width="20" customWidth="1" min="37" max="37"/>
-    <col width="20" customWidth="1" min="38" max="38"/>
-    <col width="20" customWidth="1" min="39" max="39"/>
-    <col width="20" customWidth="1" min="40" max="40"/>
-    <col width="20" customWidth="1" min="41" max="41"/>
-    <col width="20" customWidth="1" min="42" max="42"/>
-    <col width="20" customWidth="1" min="43" max="43"/>
-    <col width="20" customWidth="1" min="44" max="44"/>
-    <col width="20" customWidth="1" min="45" max="45"/>
-    <col width="20" customWidth="1" min="46" max="46"/>
-    <col width="20" customWidth="1" min="47" max="47"/>
-    <col width="20" customWidth="1" min="48" max="48"/>
-    <col width="20" customWidth="1" min="49" max="49"/>
-    <col width="20" customWidth="1" min="50" max="50"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -615,6 +584,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n"/>
+      <c r="B2" s="4" t="n"/>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="4" t="n"/>
+      <c r="E2" s="4" t="n"/>
       <c r="F2" s="5" t="inlineStr">
         <is>
           <t>December</t>
@@ -671,6 +644,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
+      <c r="B3" s="4" t="n"/>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="4" t="n"/>
+      <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
           <t>20/Dec - 26/Dec</t>
@@ -735,8 +712,8 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="n"/>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="6" t="n"/>
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
@@ -787,28 +764,28 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>Task 1</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" s="7" t="inlineStr">
         <is>
           <t>M1</t>
         </is>
       </c>
-      <c r="D5" s="7" t="inlineStr">
+      <c r="D5" s="8" t="inlineStr">
         <is>
           <t>20-Dec</t>
         </is>
       </c>
-      <c r="E5" s="7" t="inlineStr">
+      <c r="E5" s="8" t="inlineStr">
         <is>
           <t>02-Jan</t>
         </is>
       </c>
-      <c r="F5" s="8" t="n"/>
-      <c r="G5" s="8" t="n"/>
+      <c r="F5" s="9" t="n"/>
+      <c r="G5" s="9" t="n"/>
       <c r="H5" s="1" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
@@ -855,27 +832,27 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B6" s="10" t="inlineStr">
         <is>
           <t>1.1</t>
         </is>
       </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="C6" s="10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
+      <c r="D6" s="11" t="inlineStr">
         <is>
           <t>20-Dec</t>
         </is>
       </c>
-      <c r="E6" s="9" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>26-Dec</t>
         </is>
       </c>
-      <c r="F6" s="10" t="n"/>
+      <c r="F6" s="12" t="n"/>
       <c r="G6" s="1" t="n"/>
       <c r="H6" s="1" t="n"/>
       <c r="I6" s="1" t="n"/>
@@ -923,28 +900,28 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="10" t="inlineStr">
         <is>
           <t>1.2</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="C7" s="10" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
+      <c r="D7" s="11" t="inlineStr">
         <is>
           <t>27-Dec</t>
         </is>
       </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
           <t>02-Jan</t>
         </is>
       </c>
       <c r="F7" s="1" t="n"/>
-      <c r="G7" s="10" t="n"/>
+      <c r="G7" s="12" t="n"/>
       <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n"/>
       <c r="J7" s="1" t="n"/>
@@ -991,30 +968,30 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="6" t="inlineStr">
+      <c r="B8" s="7" t="inlineStr">
         <is>
           <t>Task 2</t>
         </is>
       </c>
-      <c r="C8" s="6" t="inlineStr">
+      <c r="C8" s="7" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
-      <c r="D8" s="7" t="inlineStr">
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t>03-Jan</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr">
+      <c r="E8" s="8" t="inlineStr">
         <is>
           <t>16-Jan</t>
         </is>
       </c>
       <c r="F8" s="1" t="n"/>
       <c r="G8" s="1" t="n"/>
-      <c r="H8" s="8" t="n"/>
-      <c r="I8" s="8" t="n"/>
+      <c r="H8" s="9" t="n"/>
+      <c r="I8" s="9" t="n"/>
       <c r="J8" s="1" t="n"/>
       <c r="K8" s="1" t="n"/>
       <c r="L8" s="1" t="n"/>
@@ -1059,29 +1036,29 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="10" t="inlineStr">
         <is>
           <t>2.1</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="C9" s="10" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D9" s="9" t="inlineStr">
+      <c r="D9" s="11" t="inlineStr">
         <is>
           <t>03-Jan</t>
         </is>
       </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="E9" s="11" t="inlineStr">
         <is>
           <t>09-Jan</t>
         </is>
       </c>
       <c r="F9" s="1" t="n"/>
       <c r="G9" s="1" t="n"/>
-      <c r="H9" s="10" t="n"/>
+      <c r="H9" s="12" t="n"/>
       <c r="I9" s="1" t="n"/>
       <c r="J9" s="1" t="n"/>
       <c r="K9" s="1" t="n"/>
@@ -1127,22 +1104,22 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="10" t="inlineStr">
         <is>
           <t>2.2</t>
         </is>
       </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C10" s="10" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="D10" s="9" t="inlineStr">
+      <c r="D10" s="11" t="inlineStr">
         <is>
           <t>10-Jan</t>
         </is>
       </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="E10" s="11" t="inlineStr">
         <is>
           <t>16-Jan</t>
         </is>
@@ -1150,7 +1127,7 @@
       <c r="F10" s="1" t="n"/>
       <c r="G10" s="1" t="n"/>
       <c r="H10" s="1" t="n"/>
-      <c r="I10" s="10" t="n"/>
+      <c r="I10" s="12" t="n"/>
       <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
       <c r="L10" s="1" t="n"/>
@@ -1195,8 +1172,8 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="n"/>
+      <c r="B11" s="6" t="n"/>
+      <c r="C11" s="6" t="n"/>
       <c r="D11" s="1" t="n"/>
       <c r="E11" s="1" t="n"/>
       <c r="F11" s="1" t="n"/>
@@ -1247,8 +1224,8 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="1" t="n"/>
-      <c r="C12" s="1" t="n"/>
+      <c r="B12" s="6" t="n"/>
+      <c r="C12" s="6" t="n"/>
       <c r="D12" s="1" t="n"/>
       <c r="E12" s="1" t="n"/>
       <c r="F12" s="1" t="n"/>
@@ -1299,8 +1276,8 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="1" t="n"/>
-      <c r="C13" s="1" t="n"/>
+      <c r="B13" s="6" t="n"/>
+      <c r="C13" s="6" t="n"/>
       <c r="D13" s="1" t="n"/>
       <c r="E13" s="1" t="n"/>
       <c r="F13" s="1" t="n"/>
@@ -1351,8 +1328,8 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="1" t="n"/>
-      <c r="C14" s="1" t="n"/>
+      <c r="B14" s="6" t="n"/>
+      <c r="C14" s="6" t="n"/>
       <c r="D14" s="1" t="n"/>
       <c r="E14" s="1" t="n"/>
       <c r="F14" s="1" t="n"/>
@@ -1403,8 +1380,8 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="n"/>
+      <c r="B15" s="6" t="n"/>
+      <c r="C15" s="6" t="n"/>
       <c r="D15" s="1" t="n"/>
       <c r="E15" s="1" t="n"/>
       <c r="F15" s="1" t="n"/>
@@ -1455,8 +1432,8 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
-      <c r="B16" s="1" t="n"/>
-      <c r="C16" s="1" t="n"/>
+      <c r="B16" s="6" t="n"/>
+      <c r="C16" s="6" t="n"/>
       <c r="D16" s="1" t="n"/>
       <c r="E16" s="1" t="n"/>
       <c r="F16" s="1" t="n"/>
@@ -1507,8 +1484,8 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="1" t="n"/>
-      <c r="C17" s="1" t="n"/>
+      <c r="B17" s="6" t="n"/>
+      <c r="C17" s="6" t="n"/>
       <c r="D17" s="1" t="n"/>
       <c r="E17" s="1" t="n"/>
       <c r="F17" s="1" t="n"/>
@@ -1559,8 +1536,8 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="n"/>
+      <c r="B18" s="6" t="n"/>
+      <c r="C18" s="6" t="n"/>
       <c r="D18" s="1" t="n"/>
       <c r="E18" s="1" t="n"/>
       <c r="F18" s="1" t="n"/>
@@ -1611,8 +1588,8 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="n"/>
+      <c r="B19" s="6" t="n"/>
+      <c r="C19" s="6" t="n"/>
       <c r="D19" s="1" t="n"/>
       <c r="E19" s="1" t="n"/>
       <c r="F19" s="1" t="n"/>
@@ -1663,8 +1640,8 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="n"/>
+      <c r="B20" s="6" t="n"/>
+      <c r="C20" s="6" t="n"/>
       <c r="D20" s="1" t="n"/>
       <c r="E20" s="1" t="n"/>
       <c r="F20" s="1" t="n"/>
@@ -1715,8 +1692,8 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="1" t="n"/>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
       <c r="D21" s="1" t="n"/>
       <c r="E21" s="1" t="n"/>
       <c r="F21" s="1" t="n"/>
@@ -1767,8 +1744,8 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="1" t="n"/>
-      <c r="C22" s="1" t="n"/>
+      <c r="B22" s="6" t="n"/>
+      <c r="C22" s="6" t="n"/>
       <c r="D22" s="1" t="n"/>
       <c r="E22" s="1" t="n"/>
       <c r="F22" s="1" t="n"/>
@@ -1819,8 +1796,8 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="n"/>
-      <c r="C23" s="1" t="n"/>
+      <c r="B23" s="6" t="n"/>
+      <c r="C23" s="6" t="n"/>
       <c r="D23" s="1" t="n"/>
       <c r="E23" s="1" t="n"/>
       <c r="F23" s="1" t="n"/>
@@ -1871,8 +1848,8 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="1" t="n"/>
-      <c r="C24" s="1" t="n"/>
+      <c r="B24" s="6" t="n"/>
+      <c r="C24" s="6" t="n"/>
       <c r="D24" s="1" t="n"/>
       <c r="E24" s="1" t="n"/>
       <c r="F24" s="1" t="n"/>
@@ -1923,8 +1900,8 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="n"/>
+      <c r="B25" s="6" t="n"/>
+      <c r="C25" s="6" t="n"/>
       <c r="D25" s="1" t="n"/>
       <c r="E25" s="1" t="n"/>
       <c r="F25" s="1" t="n"/>
@@ -1975,8 +1952,8 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="n"/>
+      <c r="B26" s="6" t="n"/>
+      <c r="C26" s="6" t="n"/>
       <c r="D26" s="1" t="n"/>
       <c r="E26" s="1" t="n"/>
       <c r="F26" s="1" t="n"/>
@@ -2027,8 +2004,8 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="n"/>
-      <c r="C27" s="1" t="n"/>
+      <c r="B27" s="6" t="n"/>
+      <c r="C27" s="6" t="n"/>
       <c r="D27" s="1" t="n"/>
       <c r="E27" s="1" t="n"/>
       <c r="F27" s="1" t="n"/>
@@ -2079,8 +2056,8 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="1" t="n"/>
-      <c r="C28" s="1" t="n"/>
+      <c r="B28" s="6" t="n"/>
+      <c r="C28" s="6" t="n"/>
       <c r="D28" s="1" t="n"/>
       <c r="E28" s="1" t="n"/>
       <c r="F28" s="1" t="n"/>
@@ -2131,8 +2108,8 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
-      <c r="B29" s="1" t="n"/>
-      <c r="C29" s="1" t="n"/>
+      <c r="B29" s="6" t="n"/>
+      <c r="C29" s="6" t="n"/>
       <c r="D29" s="1" t="n"/>
       <c r="E29" s="1" t="n"/>
       <c r="F29" s="1" t="n"/>
@@ -2183,8 +2160,8 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
-      <c r="B30" s="1" t="n"/>
-      <c r="C30" s="1" t="n"/>
+      <c r="B30" s="6" t="n"/>
+      <c r="C30" s="6" t="n"/>
       <c r="D30" s="1" t="n"/>
       <c r="E30" s="1" t="n"/>
       <c r="F30" s="1" t="n"/>
@@ -2235,8 +2212,8 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
-      <c r="B31" s="1" t="n"/>
-      <c r="C31" s="1" t="n"/>
+      <c r="B31" s="6" t="n"/>
+      <c r="C31" s="6" t="n"/>
       <c r="D31" s="1" t="n"/>
       <c r="E31" s="1" t="n"/>
       <c r="F31" s="1" t="n"/>
@@ -2287,8 +2264,8 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="n"/>
-      <c r="C32" s="1" t="n"/>
+      <c r="B32" s="6" t="n"/>
+      <c r="C32" s="6" t="n"/>
       <c r="D32" s="1" t="n"/>
       <c r="E32" s="1" t="n"/>
       <c r="F32" s="1" t="n"/>
@@ -2339,8 +2316,8 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
-      <c r="B33" s="1" t="n"/>
-      <c r="C33" s="1" t="n"/>
+      <c r="B33" s="6" t="n"/>
+      <c r="C33" s="6" t="n"/>
       <c r="D33" s="1" t="n"/>
       <c r="E33" s="1" t="n"/>
       <c r="F33" s="1" t="n"/>
@@ -2391,8 +2368,8 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
-      <c r="B34" s="1" t="n"/>
-      <c r="C34" s="1" t="n"/>
+      <c r="B34" s="6" t="n"/>
+      <c r="C34" s="6" t="n"/>
       <c r="D34" s="1" t="n"/>
       <c r="E34" s="1" t="n"/>
       <c r="F34" s="1" t="n"/>
@@ -2443,8 +2420,8 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
-      <c r="B35" s="1" t="n"/>
-      <c r="C35" s="1" t="n"/>
+      <c r="B35" s="6" t="n"/>
+      <c r="C35" s="6" t="n"/>
       <c r="D35" s="1" t="n"/>
       <c r="E35" s="1" t="n"/>
       <c r="F35" s="1" t="n"/>
@@ -2495,8 +2472,8 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
-      <c r="B36" s="1" t="n"/>
-      <c r="C36" s="1" t="n"/>
+      <c r="B36" s="6" t="n"/>
+      <c r="C36" s="6" t="n"/>
       <c r="D36" s="1" t="n"/>
       <c r="E36" s="1" t="n"/>
       <c r="F36" s="1" t="n"/>
@@ -2547,8 +2524,8 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
-      <c r="B37" s="1" t="n"/>
-      <c r="C37" s="1" t="n"/>
+      <c r="B37" s="6" t="n"/>
+      <c r="C37" s="6" t="n"/>
       <c r="D37" s="1" t="n"/>
       <c r="E37" s="1" t="n"/>
       <c r="F37" s="1" t="n"/>
@@ -2599,8 +2576,8 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
-      <c r="B38" s="1" t="n"/>
-      <c r="C38" s="1" t="n"/>
+      <c r="B38" s="6" t="n"/>
+      <c r="C38" s="6" t="n"/>
       <c r="D38" s="1" t="n"/>
       <c r="E38" s="1" t="n"/>
       <c r="F38" s="1" t="n"/>
@@ -2651,8 +2628,8 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
-      <c r="B39" s="1" t="n"/>
-      <c r="C39" s="1" t="n"/>
+      <c r="B39" s="6" t="n"/>
+      <c r="C39" s="6" t="n"/>
       <c r="D39" s="1" t="n"/>
       <c r="E39" s="1" t="n"/>
       <c r="F39" s="1" t="n"/>
@@ -2703,8 +2680,8 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
-      <c r="B40" s="1" t="n"/>
-      <c r="C40" s="1" t="n"/>
+      <c r="B40" s="6" t="n"/>
+      <c r="C40" s="6" t="n"/>
       <c r="D40" s="1" t="n"/>
       <c r="E40" s="1" t="n"/>
       <c r="F40" s="1" t="n"/>
@@ -2755,8 +2732,8 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="n"/>
-      <c r="C41" s="1" t="n"/>
+      <c r="B41" s="6" t="n"/>
+      <c r="C41" s="6" t="n"/>
       <c r="D41" s="1" t="n"/>
       <c r="E41" s="1" t="n"/>
       <c r="F41" s="1" t="n"/>
@@ -2807,8 +2784,8 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="n"/>
-      <c r="C42" s="1" t="n"/>
+      <c r="B42" s="6" t="n"/>
+      <c r="C42" s="6" t="n"/>
       <c r="D42" s="1" t="n"/>
       <c r="E42" s="1" t="n"/>
       <c r="F42" s="1" t="n"/>
@@ -2859,8 +2836,8 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
-      <c r="B43" s="1" t="n"/>
-      <c r="C43" s="1" t="n"/>
+      <c r="B43" s="6" t="n"/>
+      <c r="C43" s="6" t="n"/>
       <c r="D43" s="1" t="n"/>
       <c r="E43" s="1" t="n"/>
       <c r="F43" s="1" t="n"/>
@@ -2911,8 +2888,8 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
-      <c r="B44" s="1" t="n"/>
-      <c r="C44" s="1" t="n"/>
+      <c r="B44" s="6" t="n"/>
+      <c r="C44" s="6" t="n"/>
       <c r="D44" s="1" t="n"/>
       <c r="E44" s="1" t="n"/>
       <c r="F44" s="1" t="n"/>
@@ -2963,8 +2940,8 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
-      <c r="B45" s="1" t="n"/>
-      <c r="C45" s="1" t="n"/>
+      <c r="B45" s="6" t="n"/>
+      <c r="C45" s="6" t="n"/>
       <c r="D45" s="1" t="n"/>
       <c r="E45" s="1" t="n"/>
       <c r="F45" s="1" t="n"/>
@@ -3015,8 +2992,8 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
-      <c r="B46" s="1" t="n"/>
-      <c r="C46" s="1" t="n"/>
+      <c r="B46" s="6" t="n"/>
+      <c r="C46" s="6" t="n"/>
       <c r="D46" s="1" t="n"/>
       <c r="E46" s="1" t="n"/>
       <c r="F46" s="1" t="n"/>
@@ -3067,8 +3044,8 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n"/>
-      <c r="B47" s="1" t="n"/>
-      <c r="C47" s="1" t="n"/>
+      <c r="B47" s="6" t="n"/>
+      <c r="C47" s="6" t="n"/>
       <c r="D47" s="1" t="n"/>
       <c r="E47" s="1" t="n"/>
       <c r="F47" s="1" t="n"/>
@@ -3119,8 +3096,8 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
-      <c r="B48" s="1" t="n"/>
-      <c r="C48" s="1" t="n"/>
+      <c r="B48" s="6" t="n"/>
+      <c r="C48" s="6" t="n"/>
       <c r="D48" s="1" t="n"/>
       <c r="E48" s="1" t="n"/>
       <c r="F48" s="1" t="n"/>
@@ -3171,8 +3148,8 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
-      <c r="B49" s="1" t="n"/>
-      <c r="C49" s="1" t="n"/>
+      <c r="B49" s="6" t="n"/>
+      <c r="C49" s="6" t="n"/>
       <c r="D49" s="1" t="n"/>
       <c r="E49" s="1" t="n"/>
       <c r="F49" s="1" t="n"/>
@@ -3223,8 +3200,8 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
-      <c r="B50" s="1" t="n"/>
-      <c r="C50" s="1" t="n"/>
+      <c r="B50" s="6" t="n"/>
+      <c r="C50" s="6" t="n"/>
       <c r="D50" s="1" t="n"/>
       <c r="E50" s="1" t="n"/>
       <c r="F50" s="1" t="n"/>
@@ -3275,8 +3252,8 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n"/>
-      <c r="B51" s="1" t="n"/>
-      <c r="C51" s="1" t="n"/>
+      <c r="B51" s="6" t="n"/>
+      <c r="C51" s="6" t="n"/>
       <c r="D51" s="1" t="n"/>
       <c r="E51" s="1" t="n"/>
       <c r="F51" s="1" t="n"/>
@@ -3327,8 +3304,8 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
-      <c r="B52" s="1" t="n"/>
-      <c r="C52" s="1" t="n"/>
+      <c r="B52" s="6" t="n"/>
+      <c r="C52" s="6" t="n"/>
       <c r="D52" s="1" t="n"/>
       <c r="E52" s="1" t="n"/>
       <c r="F52" s="1" t="n"/>
@@ -3379,8 +3356,8 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n"/>
-      <c r="B53" s="1" t="n"/>
-      <c r="C53" s="1" t="n"/>
+      <c r="B53" s="6" t="n"/>
+      <c r="C53" s="6" t="n"/>
       <c r="D53" s="1" t="n"/>
       <c r="E53" s="1" t="n"/>
       <c r="F53" s="1" t="n"/>
@@ -3431,8 +3408,8 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n"/>
-      <c r="B54" s="1" t="n"/>
-      <c r="C54" s="1" t="n"/>
+      <c r="B54" s="6" t="n"/>
+      <c r="C54" s="6" t="n"/>
       <c r="D54" s="1" t="n"/>
       <c r="E54" s="1" t="n"/>
       <c r="F54" s="1" t="n"/>
@@ -3483,8 +3460,8 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
-      <c r="B55" s="1" t="n"/>
-      <c r="C55" s="1" t="n"/>
+      <c r="B55" s="6" t="n"/>
+      <c r="C55" s="6" t="n"/>
       <c r="D55" s="1" t="n"/>
       <c r="E55" s="1" t="n"/>
       <c r="F55" s="1" t="n"/>
@@ -3535,8 +3512,8 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n"/>
-      <c r="B56" s="1" t="n"/>
-      <c r="C56" s="1" t="n"/>
+      <c r="B56" s="6" t="n"/>
+      <c r="C56" s="6" t="n"/>
       <c r="D56" s="1" t="n"/>
       <c r="E56" s="1" t="n"/>
       <c r="F56" s="1" t="n"/>
@@ -3587,8 +3564,8 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="n"/>
-      <c r="C57" s="1" t="n"/>
+      <c r="B57" s="6" t="n"/>
+      <c r="C57" s="6" t="n"/>
       <c r="D57" s="1" t="n"/>
       <c r="E57" s="1" t="n"/>
       <c r="F57" s="1" t="n"/>
@@ -3639,8 +3616,8 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n"/>
-      <c r="B58" s="1" t="n"/>
-      <c r="C58" s="1" t="n"/>
+      <c r="B58" s="6" t="n"/>
+      <c r="C58" s="6" t="n"/>
       <c r="D58" s="1" t="n"/>
       <c r="E58" s="1" t="n"/>
       <c r="F58" s="1" t="n"/>
@@ -3691,8 +3668,8 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n"/>
-      <c r="B59" s="1" t="n"/>
-      <c r="C59" s="1" t="n"/>
+      <c r="B59" s="6" t="n"/>
+      <c r="C59" s="6" t="n"/>
       <c r="D59" s="1" t="n"/>
       <c r="E59" s="1" t="n"/>
       <c r="F59" s="1" t="n"/>
@@ -3743,8 +3720,8 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
-      <c r="B60" s="1" t="n"/>
-      <c r="C60" s="1" t="n"/>
+      <c r="B60" s="6" t="n"/>
+      <c r="C60" s="6" t="n"/>
       <c r="D60" s="1" t="n"/>
       <c r="E60" s="1" t="n"/>
       <c r="F60" s="1" t="n"/>
@@ -3795,8 +3772,8 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
-      <c r="B61" s="1" t="n"/>
-      <c r="C61" s="1" t="n"/>
+      <c r="B61" s="6" t="n"/>
+      <c r="C61" s="6" t="n"/>
       <c r="D61" s="1" t="n"/>
       <c r="E61" s="1" t="n"/>
       <c r="F61" s="1" t="n"/>
@@ -3847,8 +3824,8 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n"/>
-      <c r="B62" s="1" t="n"/>
-      <c r="C62" s="1" t="n"/>
+      <c r="B62" s="6" t="n"/>
+      <c r="C62" s="6" t="n"/>
       <c r="D62" s="1" t="n"/>
       <c r="E62" s="1" t="n"/>
       <c r="F62" s="1" t="n"/>
@@ -3899,8 +3876,8 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n"/>
-      <c r="B63" s="1" t="n"/>
-      <c r="C63" s="1" t="n"/>
+      <c r="B63" s="6" t="n"/>
+      <c r="C63" s="6" t="n"/>
       <c r="D63" s="1" t="n"/>
       <c r="E63" s="1" t="n"/>
       <c r="F63" s="1" t="n"/>
@@ -3951,8 +3928,8 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n"/>
-      <c r="B64" s="1" t="n"/>
-      <c r="C64" s="1" t="n"/>
+      <c r="B64" s="6" t="n"/>
+      <c r="C64" s="6" t="n"/>
       <c r="D64" s="1" t="n"/>
       <c r="E64" s="1" t="n"/>
       <c r="F64" s="1" t="n"/>
@@ -4003,8 +3980,8 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
-      <c r="B65" s="1" t="n"/>
-      <c r="C65" s="1" t="n"/>
+      <c r="B65" s="6" t="n"/>
+      <c r="C65" s="6" t="n"/>
       <c r="D65" s="1" t="n"/>
       <c r="E65" s="1" t="n"/>
       <c r="F65" s="1" t="n"/>
@@ -4055,8 +4032,8 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
-      <c r="B66" s="1" t="n"/>
-      <c r="C66" s="1" t="n"/>
+      <c r="B66" s="6" t="n"/>
+      <c r="C66" s="6" t="n"/>
       <c r="D66" s="1" t="n"/>
       <c r="E66" s="1" t="n"/>
       <c r="F66" s="1" t="n"/>
@@ -4107,8 +4084,8 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
-      <c r="B67" s="1" t="n"/>
-      <c r="C67" s="1" t="n"/>
+      <c r="B67" s="6" t="n"/>
+      <c r="C67" s="6" t="n"/>
       <c r="D67" s="1" t="n"/>
       <c r="E67" s="1" t="n"/>
       <c r="F67" s="1" t="n"/>
@@ -4159,8 +4136,8 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
-      <c r="B68" s="1" t="n"/>
-      <c r="C68" s="1" t="n"/>
+      <c r="B68" s="6" t="n"/>
+      <c r="C68" s="6" t="n"/>
       <c r="D68" s="1" t="n"/>
       <c r="E68" s="1" t="n"/>
       <c r="F68" s="1" t="n"/>
@@ -4211,8 +4188,8 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
-      <c r="B69" s="1" t="n"/>
-      <c r="C69" s="1" t="n"/>
+      <c r="B69" s="6" t="n"/>
+      <c r="C69" s="6" t="n"/>
       <c r="D69" s="1" t="n"/>
       <c r="E69" s="1" t="n"/>
       <c r="F69" s="1" t="n"/>
@@ -4263,8 +4240,8 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
-      <c r="B70" s="1" t="n"/>
-      <c r="C70" s="1" t="n"/>
+      <c r="B70" s="6" t="n"/>
+      <c r="C70" s="6" t="n"/>
       <c r="D70" s="1" t="n"/>
       <c r="E70" s="1" t="n"/>
       <c r="F70" s="1" t="n"/>
@@ -4315,8 +4292,8 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
-      <c r="B71" s="1" t="n"/>
-      <c r="C71" s="1" t="n"/>
+      <c r="B71" s="6" t="n"/>
+      <c r="C71" s="6" t="n"/>
       <c r="D71" s="1" t="n"/>
       <c r="E71" s="1" t="n"/>
       <c r="F71" s="1" t="n"/>
@@ -4367,8 +4344,8 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>
-      <c r="B72" s="1" t="n"/>
-      <c r="C72" s="1" t="n"/>
+      <c r="B72" s="6" t="n"/>
+      <c r="C72" s="6" t="n"/>
       <c r="D72" s="1" t="n"/>
       <c r="E72" s="1" t="n"/>
       <c r="F72" s="1" t="n"/>
@@ -4419,8 +4396,8 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
-      <c r="B73" s="1" t="n"/>
-      <c r="C73" s="1" t="n"/>
+      <c r="B73" s="6" t="n"/>
+      <c r="C73" s="6" t="n"/>
       <c r="D73" s="1" t="n"/>
       <c r="E73" s="1" t="n"/>
       <c r="F73" s="1" t="n"/>
@@ -4471,8 +4448,8 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
-      <c r="B74" s="1" t="n"/>
-      <c r="C74" s="1" t="n"/>
+      <c r="B74" s="6" t="n"/>
+      <c r="C74" s="6" t="n"/>
       <c r="D74" s="1" t="n"/>
       <c r="E74" s="1" t="n"/>
       <c r="F74" s="1" t="n"/>
@@ -4523,8 +4500,8 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
-      <c r="B75" s="1" t="n"/>
-      <c r="C75" s="1" t="n"/>
+      <c r="B75" s="6" t="n"/>
+      <c r="C75" s="6" t="n"/>
       <c r="D75" s="1" t="n"/>
       <c r="E75" s="1" t="n"/>
       <c r="F75" s="1" t="n"/>
@@ -4575,8 +4552,8 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
-      <c r="B76" s="1" t="n"/>
-      <c r="C76" s="1" t="n"/>
+      <c r="B76" s="6" t="n"/>
+      <c r="C76" s="6" t="n"/>
       <c r="D76" s="1" t="n"/>
       <c r="E76" s="1" t="n"/>
       <c r="F76" s="1" t="n"/>
@@ -4627,8 +4604,8 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n"/>
-      <c r="B77" s="1" t="n"/>
-      <c r="C77" s="1" t="n"/>
+      <c r="B77" s="6" t="n"/>
+      <c r="C77" s="6" t="n"/>
       <c r="D77" s="1" t="n"/>
       <c r="E77" s="1" t="n"/>
       <c r="F77" s="1" t="n"/>
@@ -4679,8 +4656,8 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
-      <c r="B78" s="1" t="n"/>
-      <c r="C78" s="1" t="n"/>
+      <c r="B78" s="6" t="n"/>
+      <c r="C78" s="6" t="n"/>
       <c r="D78" s="1" t="n"/>
       <c r="E78" s="1" t="n"/>
       <c r="F78" s="1" t="n"/>
@@ -4731,8 +4708,8 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n"/>
-      <c r="B79" s="1" t="n"/>
-      <c r="C79" s="1" t="n"/>
+      <c r="B79" s="6" t="n"/>
+      <c r="C79" s="6" t="n"/>
       <c r="D79" s="1" t="n"/>
       <c r="E79" s="1" t="n"/>
       <c r="F79" s="1" t="n"/>
@@ -4783,8 +4760,8 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n"/>
-      <c r="B80" s="1" t="n"/>
-      <c r="C80" s="1" t="n"/>
+      <c r="B80" s="6" t="n"/>
+      <c r="C80" s="6" t="n"/>
       <c r="D80" s="1" t="n"/>
       <c r="E80" s="1" t="n"/>
       <c r="F80" s="1" t="n"/>
@@ -4835,8 +4812,8 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
-      <c r="B81" s="1" t="n"/>
-      <c r="C81" s="1" t="n"/>
+      <c r="B81" s="6" t="n"/>
+      <c r="C81" s="6" t="n"/>
       <c r="D81" s="1" t="n"/>
       <c r="E81" s="1" t="n"/>
       <c r="F81" s="1" t="n"/>
@@ -4887,8 +4864,8 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
-      <c r="B82" s="1" t="n"/>
-      <c r="C82" s="1" t="n"/>
+      <c r="B82" s="6" t="n"/>
+      <c r="C82" s="6" t="n"/>
       <c r="D82" s="1" t="n"/>
       <c r="E82" s="1" t="n"/>
       <c r="F82" s="1" t="n"/>
@@ -4939,8 +4916,8 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n"/>
-      <c r="B83" s="1" t="n"/>
-      <c r="C83" s="1" t="n"/>
+      <c r="B83" s="6" t="n"/>
+      <c r="C83" s="6" t="n"/>
       <c r="D83" s="1" t="n"/>
       <c r="E83" s="1" t="n"/>
       <c r="F83" s="1" t="n"/>
@@ -4991,8 +4968,8 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
-      <c r="B84" s="1" t="n"/>
-      <c r="C84" s="1" t="n"/>
+      <c r="B84" s="6" t="n"/>
+      <c r="C84" s="6" t="n"/>
       <c r="D84" s="1" t="n"/>
       <c r="E84" s="1" t="n"/>
       <c r="F84" s="1" t="n"/>
@@ -5043,8 +5020,8 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
-      <c r="B85" s="1" t="n"/>
-      <c r="C85" s="1" t="n"/>
+      <c r="B85" s="6" t="n"/>
+      <c r="C85" s="6" t="n"/>
       <c r="D85" s="1" t="n"/>
       <c r="E85" s="1" t="n"/>
       <c r="F85" s="1" t="n"/>
@@ -5095,8 +5072,8 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n"/>
-      <c r="B86" s="1" t="n"/>
-      <c r="C86" s="1" t="n"/>
+      <c r="B86" s="6" t="n"/>
+      <c r="C86" s="6" t="n"/>
       <c r="D86" s="1" t="n"/>
       <c r="E86" s="1" t="n"/>
       <c r="F86" s="1" t="n"/>
@@ -5147,8 +5124,8 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
-      <c r="B87" s="1" t="n"/>
-      <c r="C87" s="1" t="n"/>
+      <c r="B87" s="6" t="n"/>
+      <c r="C87" s="6" t="n"/>
       <c r="D87" s="1" t="n"/>
       <c r="E87" s="1" t="n"/>
       <c r="F87" s="1" t="n"/>
@@ -5199,8 +5176,8 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
-      <c r="B88" s="1" t="n"/>
-      <c r="C88" s="1" t="n"/>
+      <c r="B88" s="6" t="n"/>
+      <c r="C88" s="6" t="n"/>
       <c r="D88" s="1" t="n"/>
       <c r="E88" s="1" t="n"/>
       <c r="F88" s="1" t="n"/>
@@ -5251,8 +5228,8 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
-      <c r="B89" s="1" t="n"/>
-      <c r="C89" s="1" t="n"/>
+      <c r="B89" s="6" t="n"/>
+      <c r="C89" s="6" t="n"/>
       <c r="D89" s="1" t="n"/>
       <c r="E89" s="1" t="n"/>
       <c r="F89" s="1" t="n"/>
@@ -5303,8 +5280,8 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
-      <c r="B90" s="1" t="n"/>
-      <c r="C90" s="1" t="n"/>
+      <c r="B90" s="6" t="n"/>
+      <c r="C90" s="6" t="n"/>
       <c r="D90" s="1" t="n"/>
       <c r="E90" s="1" t="n"/>
       <c r="F90" s="1" t="n"/>
@@ -5355,8 +5332,8 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n"/>
-      <c r="B91" s="1" t="n"/>
-      <c r="C91" s="1" t="n"/>
+      <c r="B91" s="6" t="n"/>
+      <c r="C91" s="6" t="n"/>
       <c r="D91" s="1" t="n"/>
       <c r="E91" s="1" t="n"/>
       <c r="F91" s="1" t="n"/>
@@ -5407,8 +5384,8 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n"/>
-      <c r="B92" s="1" t="n"/>
-      <c r="C92" s="1" t="n"/>
+      <c r="B92" s="6" t="n"/>
+      <c r="C92" s="6" t="n"/>
       <c r="D92" s="1" t="n"/>
       <c r="E92" s="1" t="n"/>
       <c r="F92" s="1" t="n"/>
@@ -5459,8 +5436,8 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n"/>
-      <c r="B93" s="1" t="n"/>
-      <c r="C93" s="1" t="n"/>
+      <c r="B93" s="6" t="n"/>
+      <c r="C93" s="6" t="n"/>
       <c r="D93" s="1" t="n"/>
       <c r="E93" s="1" t="n"/>
       <c r="F93" s="1" t="n"/>
@@ -5511,8 +5488,8 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
-      <c r="B94" s="1" t="n"/>
-      <c r="C94" s="1" t="n"/>
+      <c r="B94" s="6" t="n"/>
+      <c r="C94" s="6" t="n"/>
       <c r="D94" s="1" t="n"/>
       <c r="E94" s="1" t="n"/>
       <c r="F94" s="1" t="n"/>
@@ -5563,8 +5540,8 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
-      <c r="B95" s="1" t="n"/>
-      <c r="C95" s="1" t="n"/>
+      <c r="B95" s="6" t="n"/>
+      <c r="C95" s="6" t="n"/>
       <c r="D95" s="1" t="n"/>
       <c r="E95" s="1" t="n"/>
       <c r="F95" s="1" t="n"/>
@@ -5615,8 +5592,8 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
-      <c r="B96" s="1" t="n"/>
-      <c r="C96" s="1" t="n"/>
+      <c r="B96" s="6" t="n"/>
+      <c r="C96" s="6" t="n"/>
       <c r="D96" s="1" t="n"/>
       <c r="E96" s="1" t="n"/>
       <c r="F96" s="1" t="n"/>
@@ -5667,8 +5644,8 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
-      <c r="B97" s="1" t="n"/>
-      <c r="C97" s="1" t="n"/>
+      <c r="B97" s="6" t="n"/>
+      <c r="C97" s="6" t="n"/>
       <c r="D97" s="1" t="n"/>
       <c r="E97" s="1" t="n"/>
       <c r="F97" s="1" t="n"/>
@@ -5719,8 +5696,8 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n"/>
-      <c r="B98" s="1" t="n"/>
-      <c r="C98" s="1" t="n"/>
+      <c r="B98" s="6" t="n"/>
+      <c r="C98" s="6" t="n"/>
       <c r="D98" s="1" t="n"/>
       <c r="E98" s="1" t="n"/>
       <c r="F98" s="1" t="n"/>
@@ -5771,8 +5748,8 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
-      <c r="B99" s="1" t="n"/>
-      <c r="C99" s="1" t="n"/>
+      <c r="B99" s="6" t="n"/>
+      <c r="C99" s="6" t="n"/>
       <c r="D99" s="1" t="n"/>
       <c r="E99" s="1" t="n"/>
       <c r="F99" s="1" t="n"/>
@@ -5823,8 +5800,8 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n"/>
-      <c r="B100" s="1" t="n"/>
-      <c r="C100" s="1" t="n"/>
+      <c r="B100" s="6" t="n"/>
+      <c r="C100" s="6" t="n"/>
       <c r="D100" s="1" t="n"/>
       <c r="E100" s="1" t="n"/>
       <c r="F100" s="1" t="n"/>
@@ -5905,6 +5882,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="7" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n"/>
@@ -5984,6 +5971,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n"/>
+      <c r="B2" s="4" t="n"/>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="4" t="n"/>
+      <c r="E2" s="4" t="n"/>
       <c r="F2" s="5" t="inlineStr">
         <is>
           <t>December</t>
@@ -6040,6 +6031,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
+      <c r="B3" s="4" t="n"/>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="4" t="n"/>
+      <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
           <t>20/Dec - 26/Dec</t>
@@ -6104,8 +6099,8 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="n"/>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="6" t="n"/>
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
@@ -6156,28 +6151,28 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>Task 1</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
+      <c r="C5" s="10" t="inlineStr">
         <is>
           <t>M1</t>
         </is>
       </c>
-      <c r="D5" s="9" t="inlineStr">
+      <c r="D5" s="11" t="inlineStr">
         <is>
           <t>20-Dec</t>
         </is>
       </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>02-Jan</t>
         </is>
       </c>
-      <c r="F5" s="8" t="n"/>
-      <c r="G5" s="8" t="n"/>
+      <c r="F5" s="9" t="n"/>
+      <c r="G5" s="9" t="n"/>
       <c r="H5" s="1" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
@@ -6224,8 +6219,8 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="n"/>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="6" t="n"/>
       <c r="D6" s="1" t="n"/>
       <c r="E6" s="1" t="n"/>
       <c r="F6" s="1" t="n"/>
@@ -6276,8 +6271,8 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="6" t="n"/>
       <c r="D7" s="1" t="n"/>
       <c r="E7" s="1" t="n"/>
       <c r="F7" s="1" t="n"/>
@@ -6328,30 +6323,30 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="10" t="inlineStr">
         <is>
           <t>Task 2</t>
         </is>
       </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="C8" s="10" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
+      <c r="D8" s="11" t="inlineStr">
         <is>
           <t>03-Jan</t>
         </is>
       </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="E8" s="11" t="inlineStr">
         <is>
           <t>16-Jan</t>
         </is>
       </c>
       <c r="F8" s="1" t="n"/>
       <c r="G8" s="1" t="n"/>
-      <c r="H8" s="8" t="n"/>
-      <c r="I8" s="8" t="n"/>
+      <c r="H8" s="9" t="n"/>
+      <c r="I8" s="9" t="n"/>
       <c r="J8" s="1" t="n"/>
       <c r="K8" s="1" t="n"/>
       <c r="L8" s="1" t="n"/>
@@ -6396,8 +6391,8 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="n"/>
+      <c r="B9" s="6" t="n"/>
+      <c r="C9" s="6" t="n"/>
       <c r="D9" s="1" t="n"/>
       <c r="E9" s="1" t="n"/>
       <c r="F9" s="1" t="n"/>
@@ -6448,8 +6443,8 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="n"/>
+      <c r="B10" s="6" t="n"/>
+      <c r="C10" s="6" t="n"/>
       <c r="D10" s="1" t="n"/>
       <c r="E10" s="1" t="n"/>
       <c r="F10" s="1" t="n"/>
@@ -6500,8 +6495,8 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="n"/>
+      <c r="B11" s="6" t="n"/>
+      <c r="C11" s="6" t="n"/>
       <c r="D11" s="1" t="n"/>
       <c r="E11" s="1" t="n"/>
       <c r="F11" s="1" t="n"/>
@@ -6552,8 +6547,8 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="1" t="n"/>
-      <c r="C12" s="1" t="n"/>
+      <c r="B12" s="6" t="n"/>
+      <c r="C12" s="6" t="n"/>
       <c r="D12" s="1" t="n"/>
       <c r="E12" s="1" t="n"/>
       <c r="F12" s="1" t="n"/>
@@ -6604,8 +6599,8 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="1" t="n"/>
-      <c r="C13" s="1" t="n"/>
+      <c r="B13" s="6" t="n"/>
+      <c r="C13" s="6" t="n"/>
       <c r="D13" s="1" t="n"/>
       <c r="E13" s="1" t="n"/>
       <c r="F13" s="1" t="n"/>
@@ -6656,8 +6651,8 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="1" t="n"/>
-      <c r="C14" s="1" t="n"/>
+      <c r="B14" s="6" t="n"/>
+      <c r="C14" s="6" t="n"/>
       <c r="D14" s="1" t="n"/>
       <c r="E14" s="1" t="n"/>
       <c r="F14" s="1" t="n"/>
@@ -6708,8 +6703,8 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="n"/>
+      <c r="B15" s="6" t="n"/>
+      <c r="C15" s="6" t="n"/>
       <c r="D15" s="1" t="n"/>
       <c r="E15" s="1" t="n"/>
       <c r="F15" s="1" t="n"/>
@@ -6760,8 +6755,8 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
-      <c r="B16" s="1" t="n"/>
-      <c r="C16" s="1" t="n"/>
+      <c r="B16" s="6" t="n"/>
+      <c r="C16" s="6" t="n"/>
       <c r="D16" s="1" t="n"/>
       <c r="E16" s="1" t="n"/>
       <c r="F16" s="1" t="n"/>
@@ -6812,8 +6807,8 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="1" t="n"/>
-      <c r="C17" s="1" t="n"/>
+      <c r="B17" s="6" t="n"/>
+      <c r="C17" s="6" t="n"/>
       <c r="D17" s="1" t="n"/>
       <c r="E17" s="1" t="n"/>
       <c r="F17" s="1" t="n"/>
@@ -6864,8 +6859,8 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="n"/>
+      <c r="B18" s="6" t="n"/>
+      <c r="C18" s="6" t="n"/>
       <c r="D18" s="1" t="n"/>
       <c r="E18" s="1" t="n"/>
       <c r="F18" s="1" t="n"/>
@@ -6916,8 +6911,8 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="n"/>
+      <c r="B19" s="6" t="n"/>
+      <c r="C19" s="6" t="n"/>
       <c r="D19" s="1" t="n"/>
       <c r="E19" s="1" t="n"/>
       <c r="F19" s="1" t="n"/>
@@ -6968,8 +6963,8 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="n"/>
+      <c r="B20" s="6" t="n"/>
+      <c r="C20" s="6" t="n"/>
       <c r="D20" s="1" t="n"/>
       <c r="E20" s="1" t="n"/>
       <c r="F20" s="1" t="n"/>
@@ -7020,8 +7015,8 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="1" t="n"/>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
       <c r="D21" s="1" t="n"/>
       <c r="E21" s="1" t="n"/>
       <c r="F21" s="1" t="n"/>
@@ -7072,8 +7067,8 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="1" t="n"/>
-      <c r="C22" s="1" t="n"/>
+      <c r="B22" s="6" t="n"/>
+      <c r="C22" s="6" t="n"/>
       <c r="D22" s="1" t="n"/>
       <c r="E22" s="1" t="n"/>
       <c r="F22" s="1" t="n"/>
@@ -7124,8 +7119,8 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="n"/>
-      <c r="C23" s="1" t="n"/>
+      <c r="B23" s="6" t="n"/>
+      <c r="C23" s="6" t="n"/>
       <c r="D23" s="1" t="n"/>
       <c r="E23" s="1" t="n"/>
       <c r="F23" s="1" t="n"/>
@@ -7176,8 +7171,8 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="1" t="n"/>
-      <c r="C24" s="1" t="n"/>
+      <c r="B24" s="6" t="n"/>
+      <c r="C24" s="6" t="n"/>
       <c r="D24" s="1" t="n"/>
       <c r="E24" s="1" t="n"/>
       <c r="F24" s="1" t="n"/>
@@ -7228,8 +7223,8 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="n"/>
+      <c r="B25" s="6" t="n"/>
+      <c r="C25" s="6" t="n"/>
       <c r="D25" s="1" t="n"/>
       <c r="E25" s="1" t="n"/>
       <c r="F25" s="1" t="n"/>
@@ -7280,8 +7275,8 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="n"/>
+      <c r="B26" s="6" t="n"/>
+      <c r="C26" s="6" t="n"/>
       <c r="D26" s="1" t="n"/>
       <c r="E26" s="1" t="n"/>
       <c r="F26" s="1" t="n"/>
@@ -7332,8 +7327,8 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="n"/>
-      <c r="C27" s="1" t="n"/>
+      <c r="B27" s="6" t="n"/>
+      <c r="C27" s="6" t="n"/>
       <c r="D27" s="1" t="n"/>
       <c r="E27" s="1" t="n"/>
       <c r="F27" s="1" t="n"/>
@@ -7384,8 +7379,8 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="1" t="n"/>
-      <c r="C28" s="1" t="n"/>
+      <c r="B28" s="6" t="n"/>
+      <c r="C28" s="6" t="n"/>
       <c r="D28" s="1" t="n"/>
       <c r="E28" s="1" t="n"/>
       <c r="F28" s="1" t="n"/>
@@ -7436,8 +7431,8 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
-      <c r="B29" s="1" t="n"/>
-      <c r="C29" s="1" t="n"/>
+      <c r="B29" s="6" t="n"/>
+      <c r="C29" s="6" t="n"/>
       <c r="D29" s="1" t="n"/>
       <c r="E29" s="1" t="n"/>
       <c r="F29" s="1" t="n"/>
@@ -7488,8 +7483,8 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
-      <c r="B30" s="1" t="n"/>
-      <c r="C30" s="1" t="n"/>
+      <c r="B30" s="6" t="n"/>
+      <c r="C30" s="6" t="n"/>
       <c r="D30" s="1" t="n"/>
       <c r="E30" s="1" t="n"/>
       <c r="F30" s="1" t="n"/>
@@ -7540,8 +7535,8 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
-      <c r="B31" s="1" t="n"/>
-      <c r="C31" s="1" t="n"/>
+      <c r="B31" s="6" t="n"/>
+      <c r="C31" s="6" t="n"/>
       <c r="D31" s="1" t="n"/>
       <c r="E31" s="1" t="n"/>
       <c r="F31" s="1" t="n"/>
@@ -7592,8 +7587,8 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="n"/>
-      <c r="C32" s="1" t="n"/>
+      <c r="B32" s="6" t="n"/>
+      <c r="C32" s="6" t="n"/>
       <c r="D32" s="1" t="n"/>
       <c r="E32" s="1" t="n"/>
       <c r="F32" s="1" t="n"/>
@@ -7644,8 +7639,8 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
-      <c r="B33" s="1" t="n"/>
-      <c r="C33" s="1" t="n"/>
+      <c r="B33" s="6" t="n"/>
+      <c r="C33" s="6" t="n"/>
       <c r="D33" s="1" t="n"/>
       <c r="E33" s="1" t="n"/>
       <c r="F33" s="1" t="n"/>
@@ -7696,8 +7691,8 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
-      <c r="B34" s="1" t="n"/>
-      <c r="C34" s="1" t="n"/>
+      <c r="B34" s="6" t="n"/>
+      <c r="C34" s="6" t="n"/>
       <c r="D34" s="1" t="n"/>
       <c r="E34" s="1" t="n"/>
       <c r="F34" s="1" t="n"/>
@@ -7748,8 +7743,8 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
-      <c r="B35" s="1" t="n"/>
-      <c r="C35" s="1" t="n"/>
+      <c r="B35" s="6" t="n"/>
+      <c r="C35" s="6" t="n"/>
       <c r="D35" s="1" t="n"/>
       <c r="E35" s="1" t="n"/>
       <c r="F35" s="1" t="n"/>
@@ -7800,8 +7795,8 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
-      <c r="B36" s="1" t="n"/>
-      <c r="C36" s="1" t="n"/>
+      <c r="B36" s="6" t="n"/>
+      <c r="C36" s="6" t="n"/>
       <c r="D36" s="1" t="n"/>
       <c r="E36" s="1" t="n"/>
       <c r="F36" s="1" t="n"/>
@@ -7852,8 +7847,8 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
-      <c r="B37" s="1" t="n"/>
-      <c r="C37" s="1" t="n"/>
+      <c r="B37" s="6" t="n"/>
+      <c r="C37" s="6" t="n"/>
       <c r="D37" s="1" t="n"/>
       <c r="E37" s="1" t="n"/>
       <c r="F37" s="1" t="n"/>
@@ -7904,8 +7899,8 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
-      <c r="B38" s="1" t="n"/>
-      <c r="C38" s="1" t="n"/>
+      <c r="B38" s="6" t="n"/>
+      <c r="C38" s="6" t="n"/>
       <c r="D38" s="1" t="n"/>
       <c r="E38" s="1" t="n"/>
       <c r="F38" s="1" t="n"/>
@@ -7956,8 +7951,8 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
-      <c r="B39" s="1" t="n"/>
-      <c r="C39" s="1" t="n"/>
+      <c r="B39" s="6" t="n"/>
+      <c r="C39" s="6" t="n"/>
       <c r="D39" s="1" t="n"/>
       <c r="E39" s="1" t="n"/>
       <c r="F39" s="1" t="n"/>
@@ -8008,8 +8003,8 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
-      <c r="B40" s="1" t="n"/>
-      <c r="C40" s="1" t="n"/>
+      <c r="B40" s="6" t="n"/>
+      <c r="C40" s="6" t="n"/>
       <c r="D40" s="1" t="n"/>
       <c r="E40" s="1" t="n"/>
       <c r="F40" s="1" t="n"/>
@@ -8060,8 +8055,8 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="n"/>
-      <c r="C41" s="1" t="n"/>
+      <c r="B41" s="6" t="n"/>
+      <c r="C41" s="6" t="n"/>
       <c r="D41" s="1" t="n"/>
       <c r="E41" s="1" t="n"/>
       <c r="F41" s="1" t="n"/>
@@ -8112,8 +8107,8 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="n"/>
-      <c r="C42" s="1" t="n"/>
+      <c r="B42" s="6" t="n"/>
+      <c r="C42" s="6" t="n"/>
       <c r="D42" s="1" t="n"/>
       <c r="E42" s="1" t="n"/>
       <c r="F42" s="1" t="n"/>
@@ -8164,8 +8159,8 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
-      <c r="B43" s="1" t="n"/>
-      <c r="C43" s="1" t="n"/>
+      <c r="B43" s="6" t="n"/>
+      <c r="C43" s="6" t="n"/>
       <c r="D43" s="1" t="n"/>
       <c r="E43" s="1" t="n"/>
       <c r="F43" s="1" t="n"/>
@@ -8216,8 +8211,8 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
-      <c r="B44" s="1" t="n"/>
-      <c r="C44" s="1" t="n"/>
+      <c r="B44" s="6" t="n"/>
+      <c r="C44" s="6" t="n"/>
       <c r="D44" s="1" t="n"/>
       <c r="E44" s="1" t="n"/>
       <c r="F44" s="1" t="n"/>
@@ -8268,8 +8263,8 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
-      <c r="B45" s="1" t="n"/>
-      <c r="C45" s="1" t="n"/>
+      <c r="B45" s="6" t="n"/>
+      <c r="C45" s="6" t="n"/>
       <c r="D45" s="1" t="n"/>
       <c r="E45" s="1" t="n"/>
       <c r="F45" s="1" t="n"/>
@@ -8320,8 +8315,8 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
-      <c r="B46" s="1" t="n"/>
-      <c r="C46" s="1" t="n"/>
+      <c r="B46" s="6" t="n"/>
+      <c r="C46" s="6" t="n"/>
       <c r="D46" s="1" t="n"/>
       <c r="E46" s="1" t="n"/>
       <c r="F46" s="1" t="n"/>
@@ -8372,8 +8367,8 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n"/>
-      <c r="B47" s="1" t="n"/>
-      <c r="C47" s="1" t="n"/>
+      <c r="B47" s="6" t="n"/>
+      <c r="C47" s="6" t="n"/>
       <c r="D47" s="1" t="n"/>
       <c r="E47" s="1" t="n"/>
       <c r="F47" s="1" t="n"/>
@@ -8424,8 +8419,8 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
-      <c r="B48" s="1" t="n"/>
-      <c r="C48" s="1" t="n"/>
+      <c r="B48" s="6" t="n"/>
+      <c r="C48" s="6" t="n"/>
       <c r="D48" s="1" t="n"/>
       <c r="E48" s="1" t="n"/>
       <c r="F48" s="1" t="n"/>
@@ -8476,8 +8471,8 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
-      <c r="B49" s="1" t="n"/>
-      <c r="C49" s="1" t="n"/>
+      <c r="B49" s="6" t="n"/>
+      <c r="C49" s="6" t="n"/>
       <c r="D49" s="1" t="n"/>
       <c r="E49" s="1" t="n"/>
       <c r="F49" s="1" t="n"/>
@@ -8528,8 +8523,8 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
-      <c r="B50" s="1" t="n"/>
-      <c r="C50" s="1" t="n"/>
+      <c r="B50" s="6" t="n"/>
+      <c r="C50" s="6" t="n"/>
       <c r="D50" s="1" t="n"/>
       <c r="E50" s="1" t="n"/>
       <c r="F50" s="1" t="n"/>
@@ -8580,8 +8575,8 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n"/>
-      <c r="B51" s="1" t="n"/>
-      <c r="C51" s="1" t="n"/>
+      <c r="B51" s="6" t="n"/>
+      <c r="C51" s="6" t="n"/>
       <c r="D51" s="1" t="n"/>
       <c r="E51" s="1" t="n"/>
       <c r="F51" s="1" t="n"/>
@@ -8632,8 +8627,8 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
-      <c r="B52" s="1" t="n"/>
-      <c r="C52" s="1" t="n"/>
+      <c r="B52" s="6" t="n"/>
+      <c r="C52" s="6" t="n"/>
       <c r="D52" s="1" t="n"/>
       <c r="E52" s="1" t="n"/>
       <c r="F52" s="1" t="n"/>
@@ -8684,8 +8679,8 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n"/>
-      <c r="B53" s="1" t="n"/>
-      <c r="C53" s="1" t="n"/>
+      <c r="B53" s="6" t="n"/>
+      <c r="C53" s="6" t="n"/>
       <c r="D53" s="1" t="n"/>
       <c r="E53" s="1" t="n"/>
       <c r="F53" s="1" t="n"/>
@@ -8736,8 +8731,8 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n"/>
-      <c r="B54" s="1" t="n"/>
-      <c r="C54" s="1" t="n"/>
+      <c r="B54" s="6" t="n"/>
+      <c r="C54" s="6" t="n"/>
       <c r="D54" s="1" t="n"/>
       <c r="E54" s="1" t="n"/>
       <c r="F54" s="1" t="n"/>
@@ -8788,8 +8783,8 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
-      <c r="B55" s="1" t="n"/>
-      <c r="C55" s="1" t="n"/>
+      <c r="B55" s="6" t="n"/>
+      <c r="C55" s="6" t="n"/>
       <c r="D55" s="1" t="n"/>
       <c r="E55" s="1" t="n"/>
       <c r="F55" s="1" t="n"/>
@@ -8840,8 +8835,8 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n"/>
-      <c r="B56" s="1" t="n"/>
-      <c r="C56" s="1" t="n"/>
+      <c r="B56" s="6" t="n"/>
+      <c r="C56" s="6" t="n"/>
       <c r="D56" s="1" t="n"/>
       <c r="E56" s="1" t="n"/>
       <c r="F56" s="1" t="n"/>
@@ -8892,8 +8887,8 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="n"/>
-      <c r="C57" s="1" t="n"/>
+      <c r="B57" s="6" t="n"/>
+      <c r="C57" s="6" t="n"/>
       <c r="D57" s="1" t="n"/>
       <c r="E57" s="1" t="n"/>
       <c r="F57" s="1" t="n"/>
@@ -8944,8 +8939,8 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n"/>
-      <c r="B58" s="1" t="n"/>
-      <c r="C58" s="1" t="n"/>
+      <c r="B58" s="6" t="n"/>
+      <c r="C58" s="6" t="n"/>
       <c r="D58" s="1" t="n"/>
       <c r="E58" s="1" t="n"/>
       <c r="F58" s="1" t="n"/>
@@ -8996,8 +8991,8 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n"/>
-      <c r="B59" s="1" t="n"/>
-      <c r="C59" s="1" t="n"/>
+      <c r="B59" s="6" t="n"/>
+      <c r="C59" s="6" t="n"/>
       <c r="D59" s="1" t="n"/>
       <c r="E59" s="1" t="n"/>
       <c r="F59" s="1" t="n"/>
@@ -9048,8 +9043,8 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
-      <c r="B60" s="1" t="n"/>
-      <c r="C60" s="1" t="n"/>
+      <c r="B60" s="6" t="n"/>
+      <c r="C60" s="6" t="n"/>
       <c r="D60" s="1" t="n"/>
       <c r="E60" s="1" t="n"/>
       <c r="F60" s="1" t="n"/>
@@ -9100,8 +9095,8 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
-      <c r="B61" s="1" t="n"/>
-      <c r="C61" s="1" t="n"/>
+      <c r="B61" s="6" t="n"/>
+      <c r="C61" s="6" t="n"/>
       <c r="D61" s="1" t="n"/>
       <c r="E61" s="1" t="n"/>
       <c r="F61" s="1" t="n"/>
@@ -9152,8 +9147,8 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n"/>
-      <c r="B62" s="1" t="n"/>
-      <c r="C62" s="1" t="n"/>
+      <c r="B62" s="6" t="n"/>
+      <c r="C62" s="6" t="n"/>
       <c r="D62" s="1" t="n"/>
       <c r="E62" s="1" t="n"/>
       <c r="F62" s="1" t="n"/>
@@ -9204,8 +9199,8 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n"/>
-      <c r="B63" s="1" t="n"/>
-      <c r="C63" s="1" t="n"/>
+      <c r="B63" s="6" t="n"/>
+      <c r="C63" s="6" t="n"/>
       <c r="D63" s="1" t="n"/>
       <c r="E63" s="1" t="n"/>
       <c r="F63" s="1" t="n"/>
@@ -9256,8 +9251,8 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n"/>
-      <c r="B64" s="1" t="n"/>
-      <c r="C64" s="1" t="n"/>
+      <c r="B64" s="6" t="n"/>
+      <c r="C64" s="6" t="n"/>
       <c r="D64" s="1" t="n"/>
       <c r="E64" s="1" t="n"/>
       <c r="F64" s="1" t="n"/>
@@ -9308,8 +9303,8 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
-      <c r="B65" s="1" t="n"/>
-      <c r="C65" s="1" t="n"/>
+      <c r="B65" s="6" t="n"/>
+      <c r="C65" s="6" t="n"/>
       <c r="D65" s="1" t="n"/>
       <c r="E65" s="1" t="n"/>
       <c r="F65" s="1" t="n"/>
@@ -9360,8 +9355,8 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
-      <c r="B66" s="1" t="n"/>
-      <c r="C66" s="1" t="n"/>
+      <c r="B66" s="6" t="n"/>
+      <c r="C66" s="6" t="n"/>
       <c r="D66" s="1" t="n"/>
       <c r="E66" s="1" t="n"/>
       <c r="F66" s="1" t="n"/>
@@ -9412,8 +9407,8 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
-      <c r="B67" s="1" t="n"/>
-      <c r="C67" s="1" t="n"/>
+      <c r="B67" s="6" t="n"/>
+      <c r="C67" s="6" t="n"/>
       <c r="D67" s="1" t="n"/>
       <c r="E67" s="1" t="n"/>
       <c r="F67" s="1" t="n"/>
@@ -9464,8 +9459,8 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
-      <c r="B68" s="1" t="n"/>
-      <c r="C68" s="1" t="n"/>
+      <c r="B68" s="6" t="n"/>
+      <c r="C68" s="6" t="n"/>
       <c r="D68" s="1" t="n"/>
       <c r="E68" s="1" t="n"/>
       <c r="F68" s="1" t="n"/>
@@ -9516,8 +9511,8 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
-      <c r="B69" s="1" t="n"/>
-      <c r="C69" s="1" t="n"/>
+      <c r="B69" s="6" t="n"/>
+      <c r="C69" s="6" t="n"/>
       <c r="D69" s="1" t="n"/>
       <c r="E69" s="1" t="n"/>
       <c r="F69" s="1" t="n"/>
@@ -9568,8 +9563,8 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
-      <c r="B70" s="1" t="n"/>
-      <c r="C70" s="1" t="n"/>
+      <c r="B70" s="6" t="n"/>
+      <c r="C70" s="6" t="n"/>
       <c r="D70" s="1" t="n"/>
       <c r="E70" s="1" t="n"/>
       <c r="F70" s="1" t="n"/>
@@ -9620,8 +9615,8 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
-      <c r="B71" s="1" t="n"/>
-      <c r="C71" s="1" t="n"/>
+      <c r="B71" s="6" t="n"/>
+      <c r="C71" s="6" t="n"/>
       <c r="D71" s="1" t="n"/>
       <c r="E71" s="1" t="n"/>
       <c r="F71" s="1" t="n"/>
@@ -9672,8 +9667,8 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>
-      <c r="B72" s="1" t="n"/>
-      <c r="C72" s="1" t="n"/>
+      <c r="B72" s="6" t="n"/>
+      <c r="C72" s="6" t="n"/>
       <c r="D72" s="1" t="n"/>
       <c r="E72" s="1" t="n"/>
       <c r="F72" s="1" t="n"/>
@@ -9724,8 +9719,8 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
-      <c r="B73" s="1" t="n"/>
-      <c r="C73" s="1" t="n"/>
+      <c r="B73" s="6" t="n"/>
+      <c r="C73" s="6" t="n"/>
       <c r="D73" s="1" t="n"/>
       <c r="E73" s="1" t="n"/>
       <c r="F73" s="1" t="n"/>
@@ -9776,8 +9771,8 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
-      <c r="B74" s="1" t="n"/>
-      <c r="C74" s="1" t="n"/>
+      <c r="B74" s="6" t="n"/>
+      <c r="C74" s="6" t="n"/>
       <c r="D74" s="1" t="n"/>
       <c r="E74" s="1" t="n"/>
       <c r="F74" s="1" t="n"/>
@@ -9828,8 +9823,8 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
-      <c r="B75" s="1" t="n"/>
-      <c r="C75" s="1" t="n"/>
+      <c r="B75" s="6" t="n"/>
+      <c r="C75" s="6" t="n"/>
       <c r="D75" s="1" t="n"/>
       <c r="E75" s="1" t="n"/>
       <c r="F75" s="1" t="n"/>
@@ -9880,8 +9875,8 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
-      <c r="B76" s="1" t="n"/>
-      <c r="C76" s="1" t="n"/>
+      <c r="B76" s="6" t="n"/>
+      <c r="C76" s="6" t="n"/>
       <c r="D76" s="1" t="n"/>
       <c r="E76" s="1" t="n"/>
       <c r="F76" s="1" t="n"/>
@@ -9932,8 +9927,8 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n"/>
-      <c r="B77" s="1" t="n"/>
-      <c r="C77" s="1" t="n"/>
+      <c r="B77" s="6" t="n"/>
+      <c r="C77" s="6" t="n"/>
       <c r="D77" s="1" t="n"/>
       <c r="E77" s="1" t="n"/>
       <c r="F77" s="1" t="n"/>
@@ -9984,8 +9979,8 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
-      <c r="B78" s="1" t="n"/>
-      <c r="C78" s="1" t="n"/>
+      <c r="B78" s="6" t="n"/>
+      <c r="C78" s="6" t="n"/>
       <c r="D78" s="1" t="n"/>
       <c r="E78" s="1" t="n"/>
       <c r="F78" s="1" t="n"/>
@@ -10036,8 +10031,8 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n"/>
-      <c r="B79" s="1" t="n"/>
-      <c r="C79" s="1" t="n"/>
+      <c r="B79" s="6" t="n"/>
+      <c r="C79" s="6" t="n"/>
       <c r="D79" s="1" t="n"/>
       <c r="E79" s="1" t="n"/>
       <c r="F79" s="1" t="n"/>
@@ -10088,8 +10083,8 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n"/>
-      <c r="B80" s="1" t="n"/>
-      <c r="C80" s="1" t="n"/>
+      <c r="B80" s="6" t="n"/>
+      <c r="C80" s="6" t="n"/>
       <c r="D80" s="1" t="n"/>
       <c r="E80" s="1" t="n"/>
       <c r="F80" s="1" t="n"/>
@@ -10140,8 +10135,8 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
-      <c r="B81" s="1" t="n"/>
-      <c r="C81" s="1" t="n"/>
+      <c r="B81" s="6" t="n"/>
+      <c r="C81" s="6" t="n"/>
       <c r="D81" s="1" t="n"/>
       <c r="E81" s="1" t="n"/>
       <c r="F81" s="1" t="n"/>
@@ -10192,8 +10187,8 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
-      <c r="B82" s="1" t="n"/>
-      <c r="C82" s="1" t="n"/>
+      <c r="B82" s="6" t="n"/>
+      <c r="C82" s="6" t="n"/>
       <c r="D82" s="1" t="n"/>
       <c r="E82" s="1" t="n"/>
       <c r="F82" s="1" t="n"/>
@@ -10244,8 +10239,8 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n"/>
-      <c r="B83" s="1" t="n"/>
-      <c r="C83" s="1" t="n"/>
+      <c r="B83" s="6" t="n"/>
+      <c r="C83" s="6" t="n"/>
       <c r="D83" s="1" t="n"/>
       <c r="E83" s="1" t="n"/>
       <c r="F83" s="1" t="n"/>
@@ -10296,8 +10291,8 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
-      <c r="B84" s="1" t="n"/>
-      <c r="C84" s="1" t="n"/>
+      <c r="B84" s="6" t="n"/>
+      <c r="C84" s="6" t="n"/>
       <c r="D84" s="1" t="n"/>
       <c r="E84" s="1" t="n"/>
       <c r="F84" s="1" t="n"/>
@@ -10348,8 +10343,8 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
-      <c r="B85" s="1" t="n"/>
-      <c r="C85" s="1" t="n"/>
+      <c r="B85" s="6" t="n"/>
+      <c r="C85" s="6" t="n"/>
       <c r="D85" s="1" t="n"/>
       <c r="E85" s="1" t="n"/>
       <c r="F85" s="1" t="n"/>
@@ -10400,8 +10395,8 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n"/>
-      <c r="B86" s="1" t="n"/>
-      <c r="C86" s="1" t="n"/>
+      <c r="B86" s="6" t="n"/>
+      <c r="C86" s="6" t="n"/>
       <c r="D86" s="1" t="n"/>
       <c r="E86" s="1" t="n"/>
       <c r="F86" s="1" t="n"/>
@@ -10452,8 +10447,8 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
-      <c r="B87" s="1" t="n"/>
-      <c r="C87" s="1" t="n"/>
+      <c r="B87" s="6" t="n"/>
+      <c r="C87" s="6" t="n"/>
       <c r="D87" s="1" t="n"/>
       <c r="E87" s="1" t="n"/>
       <c r="F87" s="1" t="n"/>
@@ -10504,8 +10499,8 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
-      <c r="B88" s="1" t="n"/>
-      <c r="C88" s="1" t="n"/>
+      <c r="B88" s="6" t="n"/>
+      <c r="C88" s="6" t="n"/>
       <c r="D88" s="1" t="n"/>
       <c r="E88" s="1" t="n"/>
       <c r="F88" s="1" t="n"/>
@@ -10556,8 +10551,8 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
-      <c r="B89" s="1" t="n"/>
-      <c r="C89" s="1" t="n"/>
+      <c r="B89" s="6" t="n"/>
+      <c r="C89" s="6" t="n"/>
       <c r="D89" s="1" t="n"/>
       <c r="E89" s="1" t="n"/>
       <c r="F89" s="1" t="n"/>
@@ -10608,8 +10603,8 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
-      <c r="B90" s="1" t="n"/>
-      <c r="C90" s="1" t="n"/>
+      <c r="B90" s="6" t="n"/>
+      <c r="C90" s="6" t="n"/>
       <c r="D90" s="1" t="n"/>
       <c r="E90" s="1" t="n"/>
       <c r="F90" s="1" t="n"/>
@@ -10660,8 +10655,8 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n"/>
-      <c r="B91" s="1" t="n"/>
-      <c r="C91" s="1" t="n"/>
+      <c r="B91" s="6" t="n"/>
+      <c r="C91" s="6" t="n"/>
       <c r="D91" s="1" t="n"/>
       <c r="E91" s="1" t="n"/>
       <c r="F91" s="1" t="n"/>
@@ -10712,8 +10707,8 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n"/>
-      <c r="B92" s="1" t="n"/>
-      <c r="C92" s="1" t="n"/>
+      <c r="B92" s="6" t="n"/>
+      <c r="C92" s="6" t="n"/>
       <c r="D92" s="1" t="n"/>
       <c r="E92" s="1" t="n"/>
       <c r="F92" s="1" t="n"/>
@@ -10764,8 +10759,8 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n"/>
-      <c r="B93" s="1" t="n"/>
-      <c r="C93" s="1" t="n"/>
+      <c r="B93" s="6" t="n"/>
+      <c r="C93" s="6" t="n"/>
       <c r="D93" s="1" t="n"/>
       <c r="E93" s="1" t="n"/>
       <c r="F93" s="1" t="n"/>
@@ -10816,8 +10811,8 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
-      <c r="B94" s="1" t="n"/>
-      <c r="C94" s="1" t="n"/>
+      <c r="B94" s="6" t="n"/>
+      <c r="C94" s="6" t="n"/>
       <c r="D94" s="1" t="n"/>
       <c r="E94" s="1" t="n"/>
       <c r="F94" s="1" t="n"/>
@@ -10868,8 +10863,8 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
-      <c r="B95" s="1" t="n"/>
-      <c r="C95" s="1" t="n"/>
+      <c r="B95" s="6" t="n"/>
+      <c r="C95" s="6" t="n"/>
       <c r="D95" s="1" t="n"/>
       <c r="E95" s="1" t="n"/>
       <c r="F95" s="1" t="n"/>
@@ -10920,8 +10915,8 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
-      <c r="B96" s="1" t="n"/>
-      <c r="C96" s="1" t="n"/>
+      <c r="B96" s="6" t="n"/>
+      <c r="C96" s="6" t="n"/>
       <c r="D96" s="1" t="n"/>
       <c r="E96" s="1" t="n"/>
       <c r="F96" s="1" t="n"/>
@@ -10972,8 +10967,8 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
-      <c r="B97" s="1" t="n"/>
-      <c r="C97" s="1" t="n"/>
+      <c r="B97" s="6" t="n"/>
+      <c r="C97" s="6" t="n"/>
       <c r="D97" s="1" t="n"/>
       <c r="E97" s="1" t="n"/>
       <c r="F97" s="1" t="n"/>
@@ -11024,8 +11019,8 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n"/>
-      <c r="B98" s="1" t="n"/>
-      <c r="C98" s="1" t="n"/>
+      <c r="B98" s="6" t="n"/>
+      <c r="C98" s="6" t="n"/>
       <c r="D98" s="1" t="n"/>
       <c r="E98" s="1" t="n"/>
       <c r="F98" s="1" t="n"/>
@@ -11076,8 +11071,8 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
-      <c r="B99" s="1" t="n"/>
-      <c r="C99" s="1" t="n"/>
+      <c r="B99" s="6" t="n"/>
+      <c r="C99" s="6" t="n"/>
       <c r="D99" s="1" t="n"/>
       <c r="E99" s="1" t="n"/>
       <c r="F99" s="1" t="n"/>
@@ -11128,8 +11123,8 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n"/>
-      <c r="B100" s="1" t="n"/>
-      <c r="C100" s="1" t="n"/>
+      <c r="B100" s="6" t="n"/>
+      <c r="C100" s="6" t="n"/>
       <c r="D100" s="1" t="n"/>
       <c r="E100" s="1" t="n"/>
       <c r="F100" s="1" t="n"/>

</xml_diff>

<commit_message>
Fix to use floats and ints
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -505,16 +505,6 @@
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -545,16 +535,16 @@
         </is>
       </c>
       <c r="G1" s="4" t="n"/>
-      <c r="H1" s="4" t="n"/>
-      <c r="I1" s="4" t="n"/>
-      <c r="J1" s="4" t="n"/>
-      <c r="K1" s="4" t="n"/>
-      <c r="L1" s="4" t="n"/>
-      <c r="M1" s="4" t="n"/>
-      <c r="N1" s="4" t="n"/>
-      <c r="O1" s="4" t="n"/>
-      <c r="P1" s="4" t="n"/>
-      <c r="Q1" s="4" t="n"/>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
       <c r="R1" s="1" t="n"/>
       <c r="S1" s="1" t="n"/>
       <c r="T1" s="1" t="n"/>
@@ -597,32 +587,20 @@
       <c r="E2" s="4" t="n"/>
       <c r="F2" s="5" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>December</t>
         </is>
       </c>
       <c r="G2" s="4" t="n"/>
-      <c r="H2" s="5" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="I2" s="4" t="n"/>
-      <c r="J2" s="4" t="n"/>
-      <c r="K2" s="4" t="n"/>
-      <c r="L2" s="5" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-      <c r="M2" s="4" t="n"/>
-      <c r="N2" s="4" t="n"/>
-      <c r="O2" s="4" t="n"/>
-      <c r="P2" s="4" t="n"/>
-      <c r="Q2" s="5" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="n"/>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
       <c r="R2" s="1" t="n"/>
       <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
@@ -665,64 +643,24 @@
       <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>20/May - 26/May</t>
+          <t>20/Dec - 26/Dec</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>27/May - 02/Jun</t>
+          <t>27/Dec - 02/Jan</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
-        <is>
-          <t>03/Jun - 09/Jun</t>
-        </is>
-      </c>
-      <c r="I3" s="5" t="inlineStr">
-        <is>
-          <t>10/Jun - 16/Jun</t>
-        </is>
-      </c>
-      <c r="J3" s="5" t="inlineStr">
-        <is>
-          <t>17/Jun - 23/Jun</t>
-        </is>
-      </c>
-      <c r="K3" s="5" t="inlineStr">
-        <is>
-          <t>24/Jun - 30/Jun</t>
-        </is>
-      </c>
-      <c r="L3" s="5" t="inlineStr">
-        <is>
-          <t>01/Jul - 07/Jul</t>
-        </is>
-      </c>
-      <c r="M3" s="5" t="inlineStr">
-        <is>
-          <t>08/Jul - 14/Jul</t>
-        </is>
-      </c>
-      <c r="N3" s="5" t="inlineStr">
-        <is>
-          <t>15/Jul - 21/Jul</t>
-        </is>
-      </c>
-      <c r="O3" s="5" t="inlineStr">
-        <is>
-          <t>22/Jul - 28/Jul</t>
-        </is>
-      </c>
-      <c r="P3" s="5" t="inlineStr">
-        <is>
-          <t>29/Jul - 04/Aug</t>
-        </is>
-      </c>
-      <c r="Q3" s="5" t="inlineStr">
-        <is>
-          <t>05/Aug - 11/Aug</t>
-        </is>
-      </c>
+      <c r="H3" s="1" t="n"/>
+      <c r="I3" s="1" t="n"/>
+      <c r="J3" s="1" t="n"/>
+      <c r="K3" s="1" t="n"/>
+      <c r="L3" s="1" t="n"/>
+      <c r="M3" s="1" t="n"/>
+      <c r="N3" s="1" t="n"/>
+      <c r="O3" s="1" t="n"/>
+      <c r="P3" s="1" t="n"/>
+      <c r="Q3" s="1" t="n"/>
       <c r="R3" s="1" t="n"/>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="n"/>
@@ -818,17 +756,17 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Requirements Gathering</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>20-May</t>
+          <t>20-Dec</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>02-Jun</t>
+          <t>02-Jan</t>
         </is>
       </c>
       <c r="F5" s="9" t="n"/>
@@ -886,17 +824,17 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>Initial Meeting</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D6" s="11" t="inlineStr">
         <is>
-          <t>20-May</t>
+          <t>20-Dec</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
-          <t>26-May</t>
+          <t>26-Dec</t>
         </is>
       </c>
       <c r="F6" s="12" t="n"/>
@@ -954,21 +892,21 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>Stakeholder Interviews</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D7" s="11" t="inlineStr">
         <is>
-          <t>20-May</t>
+          <t>27-Dec</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
         <is>
-          <t>26-May</t>
+          <t>02-Jan</t>
         </is>
       </c>
-      <c r="F7" s="12" t="n"/>
-      <c r="G7" s="1" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="12" t="n"/>
       <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n"/>
       <c r="J7" s="1" t="n"/>
@@ -1015,28 +953,12 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="10" t="inlineStr">
-        <is>
-          <t>1.3</t>
-        </is>
-      </c>
-      <c r="C8" s="10" t="inlineStr">
-        <is>
-          <t>Requirements Documentation</t>
-        </is>
-      </c>
-      <c r="D8" s="11" t="inlineStr">
-        <is>
-          <t>20-May</t>
-        </is>
-      </c>
-      <c r="E8" s="11" t="inlineStr">
-        <is>
-          <t>02-Jun</t>
-        </is>
-      </c>
-      <c r="F8" s="12" t="n"/>
-      <c r="G8" s="12" t="n"/>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="6" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
       <c r="H8" s="1" t="n"/>
       <c r="I8" s="1" t="n"/>
       <c r="J8" s="1" t="n"/>
@@ -1083,30 +1005,14 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>Task 2</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="inlineStr">
-        <is>
-          <t>Design</t>
-        </is>
-      </c>
-      <c r="D9" s="8" t="inlineStr">
-        <is>
-          <t>03-Jun</t>
-        </is>
-      </c>
-      <c r="E9" s="8" t="inlineStr">
-        <is>
-          <t>16-Jun</t>
-        </is>
-      </c>
+      <c r="B9" s="6" t="n"/>
+      <c r="C9" s="6" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
       <c r="F9" s="1" t="n"/>
       <c r="G9" s="1" t="n"/>
-      <c r="H9" s="9" t="n"/>
-      <c r="I9" s="9" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="1" t="n"/>
       <c r="J9" s="1" t="n"/>
       <c r="K9" s="1" t="n"/>
       <c r="L9" s="1" t="n"/>
@@ -1151,29 +1057,13 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="10" t="inlineStr">
-        <is>
-          <t>2.1</t>
-        </is>
-      </c>
-      <c r="C10" s="10" t="inlineStr">
-        <is>
-          <t>System Architecture Design</t>
-        </is>
-      </c>
-      <c r="D10" s="11" t="inlineStr">
-        <is>
-          <t>03-Jun</t>
-        </is>
-      </c>
-      <c r="E10" s="11" t="inlineStr">
-        <is>
-          <t>09-Jun</t>
-        </is>
-      </c>
+      <c r="B10" s="6" t="n"/>
+      <c r="C10" s="6" t="n"/>
+      <c r="D10" s="1" t="n"/>
+      <c r="E10" s="1" t="n"/>
       <c r="F10" s="1" t="n"/>
       <c r="G10" s="1" t="n"/>
-      <c r="H10" s="12" t="n"/>
+      <c r="H10" s="1" t="n"/>
       <c r="I10" s="1" t="n"/>
       <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
@@ -1219,30 +1109,14 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="10" t="inlineStr">
-        <is>
-          <t>2.2</t>
-        </is>
-      </c>
-      <c r="C11" s="10" t="inlineStr">
-        <is>
-          <t>Database Schema Design</t>
-        </is>
-      </c>
-      <c r="D11" s="11" t="inlineStr">
-        <is>
-          <t>03-Jun</t>
-        </is>
-      </c>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>16-Jun</t>
-        </is>
-      </c>
+      <c r="B11" s="6" t="n"/>
+      <c r="C11" s="6" t="n"/>
+      <c r="D11" s="1" t="n"/>
+      <c r="E11" s="1" t="n"/>
       <c r="F11" s="1" t="n"/>
       <c r="G11" s="1" t="n"/>
-      <c r="H11" s="12" t="n"/>
-      <c r="I11" s="12" t="n"/>
+      <c r="H11" s="1" t="n"/>
+      <c r="I11" s="1" t="n"/>
       <c r="J11" s="1" t="n"/>
       <c r="K11" s="1" t="n"/>
       <c r="L11" s="1" t="n"/>
@@ -1287,30 +1161,14 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="10" t="inlineStr">
-        <is>
-          <t>2.3</t>
-        </is>
-      </c>
-      <c r="C12" s="10" t="inlineStr">
-        <is>
-          <t>UI/UX Design</t>
-        </is>
-      </c>
-      <c r="D12" s="11" t="inlineStr">
-        <is>
-          <t>10-Jun</t>
-        </is>
-      </c>
-      <c r="E12" s="11" t="inlineStr">
-        <is>
-          <t>16-Jun</t>
-        </is>
-      </c>
+      <c r="B12" s="6" t="n"/>
+      <c r="C12" s="6" t="n"/>
+      <c r="D12" s="1" t="n"/>
+      <c r="E12" s="1" t="n"/>
       <c r="F12" s="1" t="n"/>
       <c r="G12" s="1" t="n"/>
       <c r="H12" s="1" t="n"/>
-      <c r="I12" s="12" t="n"/>
+      <c r="I12" s="1" t="n"/>
       <c r="J12" s="1" t="n"/>
       <c r="K12" s="1" t="n"/>
       <c r="L12" s="1" t="n"/>
@@ -1355,33 +1213,17 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>Task 3</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="D13" s="8" t="inlineStr">
-        <is>
-          <t>17-Jun</t>
-        </is>
-      </c>
-      <c r="E13" s="8" t="inlineStr">
-        <is>
-          <t>07-Jul</t>
-        </is>
-      </c>
+      <c r="B13" s="6" t="n"/>
+      <c r="C13" s="6" t="n"/>
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
       <c r="F13" s="1" t="n"/>
       <c r="G13" s="1" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
-      <c r="J13" s="9" t="n"/>
-      <c r="K13" s="9" t="n"/>
-      <c r="L13" s="9" t="n"/>
+      <c r="J13" s="1" t="n"/>
+      <c r="K13" s="1" t="n"/>
+      <c r="L13" s="1" t="n"/>
       <c r="M13" s="1" t="n"/>
       <c r="N13" s="1" t="n"/>
       <c r="O13" s="1" t="n"/>
@@ -1423,31 +1265,15 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="10" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
-        <is>
-          <t>Frontend Development</t>
-        </is>
-      </c>
-      <c r="D14" s="11" t="inlineStr">
-        <is>
-          <t>17-Jun</t>
-        </is>
-      </c>
-      <c r="E14" s="11" t="inlineStr">
-        <is>
-          <t>23-Jun</t>
-        </is>
-      </c>
+      <c r="B14" s="6" t="n"/>
+      <c r="C14" s="6" t="n"/>
+      <c r="D14" s="1" t="n"/>
+      <c r="E14" s="1" t="n"/>
       <c r="F14" s="1" t="n"/>
       <c r="G14" s="1" t="n"/>
       <c r="H14" s="1" t="n"/>
       <c r="I14" s="1" t="n"/>
-      <c r="J14" s="12" t="n"/>
+      <c r="J14" s="1" t="n"/>
       <c r="K14" s="1" t="n"/>
       <c r="L14" s="1" t="n"/>
       <c r="M14" s="1" t="n"/>
@@ -1491,33 +1317,17 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="10" t="inlineStr">
-        <is>
-          <t>3.2</t>
-        </is>
-      </c>
-      <c r="C15" s="10" t="inlineStr">
-        <is>
-          <t>Backend Development</t>
-        </is>
-      </c>
-      <c r="D15" s="11" t="inlineStr">
-        <is>
-          <t>24-Jun</t>
-        </is>
-      </c>
-      <c r="E15" s="11" t="inlineStr">
-        <is>
-          <t>07-Jul</t>
-        </is>
-      </c>
+      <c r="B15" s="6" t="n"/>
+      <c r="C15" s="6" t="n"/>
+      <c r="D15" s="1" t="n"/>
+      <c r="E15" s="1" t="n"/>
       <c r="F15" s="1" t="n"/>
       <c r="G15" s="1" t="n"/>
       <c r="H15" s="1" t="n"/>
       <c r="I15" s="1" t="n"/>
       <c r="J15" s="1" t="n"/>
-      <c r="K15" s="12" t="n"/>
-      <c r="L15" s="12" t="n"/>
+      <c r="K15" s="1" t="n"/>
+      <c r="L15" s="1" t="n"/>
       <c r="M15" s="1" t="n"/>
       <c r="N15" s="1" t="n"/>
       <c r="O15" s="1" t="n"/>
@@ -1559,33 +1369,17 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
-      <c r="B16" s="10" t="inlineStr">
-        <is>
-          <t>3.3</t>
-        </is>
-      </c>
-      <c r="C16" s="10" t="inlineStr">
-        <is>
-          <t>Integration</t>
-        </is>
-      </c>
-      <c r="D16" s="11" t="inlineStr">
-        <is>
-          <t>01-Jul</t>
-        </is>
-      </c>
-      <c r="E16" s="11" t="inlineStr">
-        <is>
-          <t>07-Jul</t>
-        </is>
-      </c>
+      <c r="B16" s="6" t="n"/>
+      <c r="C16" s="6" t="n"/>
+      <c r="D16" s="1" t="n"/>
+      <c r="E16" s="1" t="n"/>
       <c r="F16" s="1" t="n"/>
       <c r="G16" s="1" t="n"/>
       <c r="H16" s="1" t="n"/>
       <c r="I16" s="1" t="n"/>
       <c r="J16" s="1" t="n"/>
       <c r="K16" s="1" t="n"/>
-      <c r="L16" s="12" t="n"/>
+      <c r="L16" s="1" t="n"/>
       <c r="M16" s="1" t="n"/>
       <c r="N16" s="1" t="n"/>
       <c r="O16" s="1" t="n"/>
@@ -1627,26 +1421,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="7" t="inlineStr">
-        <is>
-          <t>Task 4</t>
-        </is>
-      </c>
-      <c r="C17" s="7" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="D17" s="8" t="inlineStr">
-        <is>
-          <t>08-Jul</t>
-        </is>
-      </c>
-      <c r="E17" s="8" t="inlineStr">
-        <is>
-          <t>21-Jul</t>
-        </is>
-      </c>
+      <c r="B17" s="6" t="n"/>
+      <c r="C17" s="6" t="n"/>
+      <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n"/>
       <c r="F17" s="1" t="n"/>
       <c r="G17" s="1" t="n"/>
       <c r="H17" s="1" t="n"/>
@@ -1654,8 +1432,8 @@
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
       <c r="L17" s="1" t="n"/>
-      <c r="M17" s="9" t="n"/>
-      <c r="N17" s="9" t="n"/>
+      <c r="M17" s="1" t="n"/>
+      <c r="N17" s="1" t="n"/>
       <c r="O17" s="1" t="n"/>
       <c r="P17" s="1" t="n"/>
       <c r="Q17" s="1" t="n"/>
@@ -1695,26 +1473,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="10" t="inlineStr">
-        <is>
-          <t>4.1</t>
-        </is>
-      </c>
-      <c r="C18" s="10" t="inlineStr">
-        <is>
-          <t>Unit Testing</t>
-        </is>
-      </c>
-      <c r="D18" s="11" t="inlineStr">
-        <is>
-          <t>08-Jul</t>
-        </is>
-      </c>
-      <c r="E18" s="11" t="inlineStr">
-        <is>
-          <t>14-Jul</t>
-        </is>
-      </c>
+      <c r="B18" s="6" t="n"/>
+      <c r="C18" s="6" t="n"/>
+      <c r="D18" s="1" t="n"/>
+      <c r="E18" s="1" t="n"/>
       <c r="F18" s="1" t="n"/>
       <c r="G18" s="1" t="n"/>
       <c r="H18" s="1" t="n"/>
@@ -1722,7 +1484,7 @@
       <c r="J18" s="1" t="n"/>
       <c r="K18" s="1" t="n"/>
       <c r="L18" s="1" t="n"/>
-      <c r="M18" s="12" t="n"/>
+      <c r="M18" s="1" t="n"/>
       <c r="N18" s="1" t="n"/>
       <c r="O18" s="1" t="n"/>
       <c r="P18" s="1" t="n"/>
@@ -1763,26 +1525,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="10" t="inlineStr">
-        <is>
-          <t>4.2</t>
-        </is>
-      </c>
-      <c r="C19" s="10" t="inlineStr">
-        <is>
-          <t>Integration Testing</t>
-        </is>
-      </c>
-      <c r="D19" s="11" t="inlineStr">
-        <is>
-          <t>08-Jul</t>
-        </is>
-      </c>
-      <c r="E19" s="11" t="inlineStr">
-        <is>
-          <t>21-Jul</t>
-        </is>
-      </c>
+      <c r="B19" s="6" t="n"/>
+      <c r="C19" s="6" t="n"/>
+      <c r="D19" s="1" t="n"/>
+      <c r="E19" s="1" t="n"/>
       <c r="F19" s="1" t="n"/>
       <c r="G19" s="1" t="n"/>
       <c r="H19" s="1" t="n"/>
@@ -1790,8 +1536,8 @@
       <c r="J19" s="1" t="n"/>
       <c r="K19" s="1" t="n"/>
       <c r="L19" s="1" t="n"/>
-      <c r="M19" s="12" t="n"/>
-      <c r="N19" s="12" t="n"/>
+      <c r="M19" s="1" t="n"/>
+      <c r="N19" s="1" t="n"/>
       <c r="O19" s="1" t="n"/>
       <c r="P19" s="1" t="n"/>
       <c r="Q19" s="1" t="n"/>
@@ -1831,26 +1577,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="10" t="inlineStr">
-        <is>
-          <t>4.3</t>
-        </is>
-      </c>
-      <c r="C20" s="10" t="inlineStr">
-        <is>
-          <t>User Acceptance Testing</t>
-        </is>
-      </c>
-      <c r="D20" s="11" t="inlineStr">
-        <is>
-          <t>15-Jul</t>
-        </is>
-      </c>
-      <c r="E20" s="11" t="inlineStr">
-        <is>
-          <t>21-Jul</t>
-        </is>
-      </c>
+      <c r="B20" s="6" t="n"/>
+      <c r="C20" s="6" t="n"/>
+      <c r="D20" s="1" t="n"/>
+      <c r="E20" s="1" t="n"/>
       <c r="F20" s="1" t="n"/>
       <c r="G20" s="1" t="n"/>
       <c r="H20" s="1" t="n"/>
@@ -1859,7 +1589,7 @@
       <c r="K20" s="1" t="n"/>
       <c r="L20" s="1" t="n"/>
       <c r="M20" s="1" t="n"/>
-      <c r="N20" s="12" t="n"/>
+      <c r="N20" s="1" t="n"/>
       <c r="O20" s="1" t="n"/>
       <c r="P20" s="1" t="n"/>
       <c r="Q20" s="1" t="n"/>
@@ -1899,26 +1629,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="7" t="inlineStr">
-        <is>
-          <t>Task 5</t>
-        </is>
-      </c>
-      <c r="C21" s="7" t="inlineStr">
-        <is>
-          <t>Deployment</t>
-        </is>
-      </c>
-      <c r="D21" s="8" t="inlineStr">
-        <is>
-          <t>22-Jul</t>
-        </is>
-      </c>
-      <c r="E21" s="8" t="inlineStr">
-        <is>
-          <t>28-Jul</t>
-        </is>
-      </c>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n"/>
       <c r="F21" s="1" t="n"/>
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
@@ -1928,7 +1642,7 @@
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n"/>
       <c r="N21" s="1" t="n"/>
-      <c r="O21" s="9" t="n"/>
+      <c r="O21" s="1" t="n"/>
       <c r="P21" s="1" t="n"/>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
@@ -1967,26 +1681,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="10" t="inlineStr">
-        <is>
-          <t>5.1</t>
-        </is>
-      </c>
-      <c r="C22" s="10" t="inlineStr">
-        <is>
-          <t>Prepare Deployment Environment</t>
-        </is>
-      </c>
-      <c r="D22" s="11" t="inlineStr">
-        <is>
-          <t>22-Jul</t>
-        </is>
-      </c>
-      <c r="E22" s="11" t="inlineStr">
-        <is>
-          <t>28-Jul</t>
-        </is>
-      </c>
+      <c r="B22" s="6" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="1" t="n"/>
+      <c r="E22" s="1" t="n"/>
       <c r="F22" s="1" t="n"/>
       <c r="G22" s="1" t="n"/>
       <c r="H22" s="1" t="n"/>
@@ -1996,7 +1694,7 @@
       <c r="L22" s="1" t="n"/>
       <c r="M22" s="1" t="n"/>
       <c r="N22" s="1" t="n"/>
-      <c r="O22" s="12" t="n"/>
+      <c r="O22" s="1" t="n"/>
       <c r="P22" s="1" t="n"/>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
@@ -2035,26 +1733,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="10" t="inlineStr">
-        <is>
-          <t>5.2</t>
-        </is>
-      </c>
-      <c r="C23" s="10" t="inlineStr">
-        <is>
-          <t>Deployment</t>
-        </is>
-      </c>
-      <c r="D23" s="11" t="inlineStr">
-        <is>
-          <t>22-Jul</t>
-        </is>
-      </c>
-      <c r="E23" s="11" t="inlineStr">
-        <is>
-          <t>28-Jul</t>
-        </is>
-      </c>
+      <c r="B23" s="6" t="n"/>
+      <c r="C23" s="6" t="n"/>
+      <c r="D23" s="1" t="n"/>
+      <c r="E23" s="1" t="n"/>
       <c r="F23" s="1" t="n"/>
       <c r="G23" s="1" t="n"/>
       <c r="H23" s="1" t="n"/>
@@ -2064,7 +1746,7 @@
       <c r="L23" s="1" t="n"/>
       <c r="M23" s="1" t="n"/>
       <c r="N23" s="1" t="n"/>
-      <c r="O23" s="12" t="n"/>
+      <c r="O23" s="1" t="n"/>
       <c r="P23" s="1" t="n"/>
       <c r="Q23" s="1" t="n"/>
       <c r="R23" s="1" t="n"/>
@@ -2103,26 +1785,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="10" t="inlineStr">
-        <is>
-          <t>5.3</t>
-        </is>
-      </c>
-      <c r="C24" s="10" t="inlineStr">
-        <is>
-          <t>Post-Deployment Verification</t>
-        </is>
-      </c>
-      <c r="D24" s="11" t="inlineStr">
-        <is>
-          <t>22-Jul</t>
-        </is>
-      </c>
-      <c r="E24" s="11" t="inlineStr">
-        <is>
-          <t>28-Jul</t>
-        </is>
-      </c>
+      <c r="B24" s="6" t="n"/>
+      <c r="C24" s="6" t="n"/>
+      <c r="D24" s="1" t="n"/>
+      <c r="E24" s="1" t="n"/>
       <c r="F24" s="1" t="n"/>
       <c r="G24" s="1" t="n"/>
       <c r="H24" s="1" t="n"/>
@@ -2132,7 +1798,7 @@
       <c r="L24" s="1" t="n"/>
       <c r="M24" s="1" t="n"/>
       <c r="N24" s="1" t="n"/>
-      <c r="O24" s="12" t="n"/>
+      <c r="O24" s="1" t="n"/>
       <c r="P24" s="1" t="n"/>
       <c r="Q24" s="1" t="n"/>
       <c r="R24" s="1" t="n"/>
@@ -2171,26 +1837,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="7" t="inlineStr">
-        <is>
-          <t>Task 6</t>
-        </is>
-      </c>
-      <c r="C25" s="7" t="inlineStr">
-        <is>
-          <t>Maintenance</t>
-        </is>
-      </c>
-      <c r="D25" s="8" t="inlineStr">
-        <is>
-          <t>29-Jul</t>
-        </is>
-      </c>
-      <c r="E25" s="8" t="inlineStr">
-        <is>
-          <t>11-Aug</t>
-        </is>
-      </c>
+      <c r="B25" s="6" t="n"/>
+      <c r="C25" s="6" t="n"/>
+      <c r="D25" s="1" t="n"/>
+      <c r="E25" s="1" t="n"/>
       <c r="F25" s="1" t="n"/>
       <c r="G25" s="1" t="n"/>
       <c r="H25" s="1" t="n"/>
@@ -2201,8 +1851,8 @@
       <c r="M25" s="1" t="n"/>
       <c r="N25" s="1" t="n"/>
       <c r="O25" s="1" t="n"/>
-      <c r="P25" s="9" t="n"/>
-      <c r="Q25" s="9" t="n"/>
+      <c r="P25" s="1" t="n"/>
+      <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
       <c r="S25" s="1" t="n"/>
       <c r="T25" s="1" t="n"/>
@@ -2239,26 +1889,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="10" t="inlineStr">
-        <is>
-          <t>6.1</t>
-        </is>
-      </c>
-      <c r="C26" s="10" t="inlineStr">
-        <is>
-          <t>Bug Fixing</t>
-        </is>
-      </c>
-      <c r="D26" s="11" t="inlineStr">
-        <is>
-          <t>29-Jul</t>
-        </is>
-      </c>
-      <c r="E26" s="11" t="inlineStr">
-        <is>
-          <t>04-Aug</t>
-        </is>
-      </c>
+      <c r="B26" s="6" t="n"/>
+      <c r="C26" s="6" t="n"/>
+      <c r="D26" s="1" t="n"/>
+      <c r="E26" s="1" t="n"/>
       <c r="F26" s="1" t="n"/>
       <c r="G26" s="1" t="n"/>
       <c r="H26" s="1" t="n"/>
@@ -2269,7 +1903,7 @@
       <c r="M26" s="1" t="n"/>
       <c r="N26" s="1" t="n"/>
       <c r="O26" s="1" t="n"/>
-      <c r="P26" s="12" t="n"/>
+      <c r="P26" s="1" t="n"/>
       <c r="Q26" s="1" t="n"/>
       <c r="R26" s="1" t="n"/>
       <c r="S26" s="1" t="n"/>
@@ -2307,26 +1941,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="10" t="inlineStr">
-        <is>
-          <t>6.2</t>
-        </is>
-      </c>
-      <c r="C27" s="10" t="inlineStr">
-        <is>
-          <t>Performance Tuning</t>
-        </is>
-      </c>
-      <c r="D27" s="11" t="inlineStr">
-        <is>
-          <t>29-Jul</t>
-        </is>
-      </c>
-      <c r="E27" s="11" t="inlineStr">
-        <is>
-          <t>04-Aug</t>
-        </is>
-      </c>
+      <c r="B27" s="6" t="n"/>
+      <c r="C27" s="6" t="n"/>
+      <c r="D27" s="1" t="n"/>
+      <c r="E27" s="1" t="n"/>
       <c r="F27" s="1" t="n"/>
       <c r="G27" s="1" t="n"/>
       <c r="H27" s="1" t="n"/>
@@ -2337,7 +1955,7 @@
       <c r="M27" s="1" t="n"/>
       <c r="N27" s="1" t="n"/>
       <c r="O27" s="1" t="n"/>
-      <c r="P27" s="12" t="n"/>
+      <c r="P27" s="1" t="n"/>
       <c r="Q27" s="1" t="n"/>
       <c r="R27" s="1" t="n"/>
       <c r="S27" s="1" t="n"/>
@@ -2375,26 +1993,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="10" t="inlineStr">
-        <is>
-          <t>6.3</t>
-        </is>
-      </c>
-      <c r="C28" s="10" t="inlineStr">
-        <is>
-          <t>User Training</t>
-        </is>
-      </c>
-      <c r="D28" s="11" t="inlineStr">
-        <is>
-          <t>29-Jul</t>
-        </is>
-      </c>
-      <c r="E28" s="11" t="inlineStr">
-        <is>
-          <t>11-Aug</t>
-        </is>
-      </c>
+      <c r="B28" s="6" t="n"/>
+      <c r="C28" s="6" t="n"/>
+      <c r="D28" s="1" t="n"/>
+      <c r="E28" s="1" t="n"/>
       <c r="F28" s="1" t="n"/>
       <c r="G28" s="1" t="n"/>
       <c r="H28" s="1" t="n"/>
@@ -2405,8 +2007,8 @@
       <c r="M28" s="1" t="n"/>
       <c r="N28" s="1" t="n"/>
       <c r="O28" s="1" t="n"/>
-      <c r="P28" s="12" t="n"/>
-      <c r="Q28" s="12" t="n"/>
+      <c r="P28" s="1" t="n"/>
+      <c r="Q28" s="1" t="n"/>
       <c r="R28" s="1" t="n"/>
       <c r="S28" s="1" t="n"/>
       <c r="T28" s="1" t="n"/>
@@ -6186,28 +5788,15 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="B9"/>
-    <mergeCell ref="C17"/>
-    <mergeCell ref="Q2"/>
+  <mergeCells count="8">
     <mergeCell ref="B5"/>
-    <mergeCell ref="C13"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="D1:D3"/>
-    <mergeCell ref="B25"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="C5"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B21"/>
-    <mergeCell ref="C25"/>
-    <mergeCell ref="F1:Q1"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="C9"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B17"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="B13"/>
-    <mergeCell ref="C21"/>
-    <mergeCell ref="H2:K2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6233,16 +5822,6 @@
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6273,16 +5852,16 @@
         </is>
       </c>
       <c r="G1" s="4" t="n"/>
-      <c r="H1" s="4" t="n"/>
-      <c r="I1" s="4" t="n"/>
-      <c r="J1" s="4" t="n"/>
-      <c r="K1" s="4" t="n"/>
-      <c r="L1" s="4" t="n"/>
-      <c r="M1" s="4" t="n"/>
-      <c r="N1" s="4" t="n"/>
-      <c r="O1" s="4" t="n"/>
-      <c r="P1" s="4" t="n"/>
-      <c r="Q1" s="4" t="n"/>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
       <c r="R1" s="1" t="n"/>
       <c r="S1" s="1" t="n"/>
       <c r="T1" s="1" t="n"/>
@@ -6325,32 +5904,20 @@
       <c r="E2" s="4" t="n"/>
       <c r="F2" s="5" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>December</t>
         </is>
       </c>
       <c r="G2" s="4" t="n"/>
-      <c r="H2" s="5" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="I2" s="4" t="n"/>
-      <c r="J2" s="4" t="n"/>
-      <c r="K2" s="4" t="n"/>
-      <c r="L2" s="5" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-      <c r="M2" s="4" t="n"/>
-      <c r="N2" s="4" t="n"/>
-      <c r="O2" s="4" t="n"/>
-      <c r="P2" s="4" t="n"/>
-      <c r="Q2" s="5" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="n"/>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
       <c r="R2" s="1" t="n"/>
       <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
@@ -6393,64 +5960,24 @@
       <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>20/May - 26/May</t>
+          <t>20/Dec - 26/Dec</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>27/May - 02/Jun</t>
+          <t>27/Dec - 02/Jan</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
-        <is>
-          <t>03/Jun - 09/Jun</t>
-        </is>
-      </c>
-      <c r="I3" s="5" t="inlineStr">
-        <is>
-          <t>10/Jun - 16/Jun</t>
-        </is>
-      </c>
-      <c r="J3" s="5" t="inlineStr">
-        <is>
-          <t>17/Jun - 23/Jun</t>
-        </is>
-      </c>
-      <c r="K3" s="5" t="inlineStr">
-        <is>
-          <t>24/Jun - 30/Jun</t>
-        </is>
-      </c>
-      <c r="L3" s="5" t="inlineStr">
-        <is>
-          <t>01/Jul - 07/Jul</t>
-        </is>
-      </c>
-      <c r="M3" s="5" t="inlineStr">
-        <is>
-          <t>08/Jul - 14/Jul</t>
-        </is>
-      </c>
-      <c r="N3" s="5" t="inlineStr">
-        <is>
-          <t>15/Jul - 21/Jul</t>
-        </is>
-      </c>
-      <c r="O3" s="5" t="inlineStr">
-        <is>
-          <t>22/Jul - 28/Jul</t>
-        </is>
-      </c>
-      <c r="P3" s="5" t="inlineStr">
-        <is>
-          <t>29/Jul - 04/Aug</t>
-        </is>
-      </c>
-      <c r="Q3" s="5" t="inlineStr">
-        <is>
-          <t>05/Aug - 11/Aug</t>
-        </is>
-      </c>
+      <c r="H3" s="1" t="n"/>
+      <c r="I3" s="1" t="n"/>
+      <c r="J3" s="1" t="n"/>
+      <c r="K3" s="1" t="n"/>
+      <c r="L3" s="1" t="n"/>
+      <c r="M3" s="1" t="n"/>
+      <c r="N3" s="1" t="n"/>
+      <c r="O3" s="1" t="n"/>
+      <c r="P3" s="1" t="n"/>
+      <c r="Q3" s="1" t="n"/>
       <c r="R3" s="1" t="n"/>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="n"/>
@@ -6546,17 +6073,17 @@
       </c>
       <c r="C5" s="13" t="inlineStr">
         <is>
-          <t>Requirements Gathering</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>20-May</t>
+          <t>20-Dec</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>02-Jun</t>
+          <t>02-Jan</t>
         </is>
       </c>
       <c r="F5" s="9" t="n"/>
@@ -6763,30 +6290,14 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="13" t="inlineStr">
-        <is>
-          <t>Task 2</t>
-        </is>
-      </c>
-      <c r="C9" s="13" t="inlineStr">
-        <is>
-          <t>Design</t>
-        </is>
-      </c>
-      <c r="D9" s="8" t="inlineStr">
-        <is>
-          <t>03-Jun</t>
-        </is>
-      </c>
-      <c r="E9" s="8" t="inlineStr">
-        <is>
-          <t>16-Jun</t>
-        </is>
-      </c>
+      <c r="B9" s="6" t="n"/>
+      <c r="C9" s="6" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
       <c r="F9" s="1" t="n"/>
       <c r="G9" s="1" t="n"/>
-      <c r="H9" s="9" t="n"/>
-      <c r="I9" s="9" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="1" t="n"/>
       <c r="J9" s="1" t="n"/>
       <c r="K9" s="1" t="n"/>
       <c r="L9" s="1" t="n"/>
@@ -6987,33 +6498,17 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="13" t="inlineStr">
-        <is>
-          <t>Task 3</t>
-        </is>
-      </c>
-      <c r="C13" s="13" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="D13" s="8" t="inlineStr">
-        <is>
-          <t>17-Jun</t>
-        </is>
-      </c>
-      <c r="E13" s="8" t="inlineStr">
-        <is>
-          <t>07-Jul</t>
-        </is>
-      </c>
+      <c r="B13" s="6" t="n"/>
+      <c r="C13" s="6" t="n"/>
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
       <c r="F13" s="1" t="n"/>
       <c r="G13" s="1" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
-      <c r="J13" s="9" t="n"/>
-      <c r="K13" s="9" t="n"/>
-      <c r="L13" s="9" t="n"/>
+      <c r="J13" s="1" t="n"/>
+      <c r="K13" s="1" t="n"/>
+      <c r="L13" s="1" t="n"/>
       <c r="M13" s="1" t="n"/>
       <c r="N13" s="1" t="n"/>
       <c r="O13" s="1" t="n"/>
@@ -7211,26 +6706,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="13" t="inlineStr">
-        <is>
-          <t>Task 4</t>
-        </is>
-      </c>
-      <c r="C17" s="13" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="D17" s="8" t="inlineStr">
-        <is>
-          <t>08-Jul</t>
-        </is>
-      </c>
-      <c r="E17" s="8" t="inlineStr">
-        <is>
-          <t>21-Jul</t>
-        </is>
-      </c>
+      <c r="B17" s="6" t="n"/>
+      <c r="C17" s="6" t="n"/>
+      <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n"/>
       <c r="F17" s="1" t="n"/>
       <c r="G17" s="1" t="n"/>
       <c r="H17" s="1" t="n"/>
@@ -7238,8 +6717,8 @@
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
       <c r="L17" s="1" t="n"/>
-      <c r="M17" s="9" t="n"/>
-      <c r="N17" s="9" t="n"/>
+      <c r="M17" s="1" t="n"/>
+      <c r="N17" s="1" t="n"/>
       <c r="O17" s="1" t="n"/>
       <c r="P17" s="1" t="n"/>
       <c r="Q17" s="1" t="n"/>
@@ -7435,26 +6914,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="13" t="inlineStr">
-        <is>
-          <t>Task 5</t>
-        </is>
-      </c>
-      <c r="C21" s="13" t="inlineStr">
-        <is>
-          <t>Deployment</t>
-        </is>
-      </c>
-      <c r="D21" s="8" t="inlineStr">
-        <is>
-          <t>22-Jul</t>
-        </is>
-      </c>
-      <c r="E21" s="8" t="inlineStr">
-        <is>
-          <t>28-Jul</t>
-        </is>
-      </c>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n"/>
       <c r="F21" s="1" t="n"/>
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
@@ -7464,7 +6927,7 @@
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n"/>
       <c r="N21" s="1" t="n"/>
-      <c r="O21" s="9" t="n"/>
+      <c r="O21" s="1" t="n"/>
       <c r="P21" s="1" t="n"/>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
@@ -7659,26 +7122,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="13" t="inlineStr">
-        <is>
-          <t>Task 6</t>
-        </is>
-      </c>
-      <c r="C25" s="13" t="inlineStr">
-        <is>
-          <t>Maintenance</t>
-        </is>
-      </c>
-      <c r="D25" s="8" t="inlineStr">
-        <is>
-          <t>29-Jul</t>
-        </is>
-      </c>
-      <c r="E25" s="8" t="inlineStr">
-        <is>
-          <t>11-Aug</t>
-        </is>
-      </c>
+      <c r="B25" s="6" t="n"/>
+      <c r="C25" s="6" t="n"/>
+      <c r="D25" s="1" t="n"/>
+      <c r="E25" s="1" t="n"/>
       <c r="F25" s="1" t="n"/>
       <c r="G25" s="1" t="n"/>
       <c r="H25" s="1" t="n"/>
@@ -7689,8 +7136,8 @@
       <c r="M25" s="1" t="n"/>
       <c r="N25" s="1" t="n"/>
       <c r="O25" s="1" t="n"/>
-      <c r="P25" s="9" t="n"/>
-      <c r="Q25" s="9" t="n"/>
+      <c r="P25" s="1" t="n"/>
+      <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
       <c r="S25" s="1" t="n"/>
       <c r="T25" s="1" t="n"/>
@@ -11626,16 +11073,13 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="6">
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="L2:P2"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="F1:Q1"/>
-    <mergeCell ref="Q2"/>
     <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Colored cells borders when no start date
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -41,7 +41,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -64,12 +64,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFA500"/>
         <bgColor rgb="00FFA500"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0032a852"/>
-        <bgColor rgb="0032a852"/>
       </patternFill>
     </fill>
   </fills>
@@ -97,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -116,16 +110,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -587,7 +579,7 @@
       <c r="E2" s="4" t="n"/>
       <c r="F2" s="5" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>Month 1</t>
         </is>
       </c>
       <c r="G2" s="4" t="n"/>
@@ -643,12 +635,12 @@
       <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>20/Dec - 26/Dec</t>
+          <t>Week 1</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>27/Dec - 02/Jan</t>
+          <t>Week 2</t>
         </is>
       </c>
       <c r="H3" s="1" t="n"/>
@@ -759,18 +751,10 @@
           <t>M1</t>
         </is>
       </c>
-      <c r="D5" s="8" t="inlineStr">
-        <is>
-          <t>20-Dec</t>
-        </is>
-      </c>
-      <c r="E5" s="8" t="inlineStr">
-        <is>
-          <t>02-Jan</t>
-        </is>
-      </c>
-      <c r="F5" s="9" t="n"/>
-      <c r="G5" s="9" t="n"/>
+      <c r="D5" s="1" t="n"/>
+      <c r="E5" s="1" t="n"/>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
       <c r="H5" s="1" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
@@ -817,27 +801,19 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>1.1</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="8" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
-        <is>
-          <t>20-Dec</t>
-        </is>
-      </c>
-      <c r="E6" s="11" t="inlineStr">
-        <is>
-          <t>26-Dec</t>
-        </is>
-      </c>
-      <c r="F6" s="12" t="n"/>
+      <c r="D6" s="1" t="n"/>
+      <c r="E6" s="1" t="n"/>
+      <c r="F6" s="9" t="n"/>
       <c r="G6" s="1" t="n"/>
       <c r="H6" s="1" t="n"/>
       <c r="I6" s="1" t="n"/>
@@ -885,28 +861,20 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="10" t="inlineStr">
+      <c r="B7" s="8" t="inlineStr">
         <is>
           <t>1.2</t>
         </is>
       </c>
-      <c r="C7" s="10" t="inlineStr">
+      <c r="C7" s="8" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D7" s="11" t="inlineStr">
-        <is>
-          <t>27-Dec</t>
-        </is>
-      </c>
-      <c r="E7" s="11" t="inlineStr">
-        <is>
-          <t>02-Jan</t>
-        </is>
-      </c>
+      <c r="D7" s="1" t="n"/>
+      <c r="E7" s="1" t="n"/>
       <c r="F7" s="1" t="n"/>
-      <c r="G7" s="12" t="n"/>
+      <c r="G7" s="9" t="n"/>
       <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n"/>
       <c r="J7" s="1" t="n"/>
@@ -5904,7 +5872,7 @@
       <c r="E2" s="4" t="n"/>
       <c r="F2" s="5" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>Month 1</t>
         </is>
       </c>
       <c r="G2" s="4" t="n"/>
@@ -5960,12 +5928,12 @@
       <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>20/Dec - 26/Dec</t>
+          <t>Week 1</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>27/Dec - 02/Jan</t>
+          <t>Week 2</t>
         </is>
       </c>
       <c r="H3" s="1" t="n"/>
@@ -6066,28 +6034,20 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="13" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>Task 1</t>
         </is>
       </c>
-      <c r="C5" s="13" t="inlineStr">
+      <c r="C5" s="10" t="inlineStr">
         <is>
           <t>M1</t>
         </is>
       </c>
-      <c r="D5" s="8" t="inlineStr">
-        <is>
-          <t>20-Dec</t>
-        </is>
-      </c>
-      <c r="E5" s="8" t="inlineStr">
-        <is>
-          <t>02-Jan</t>
-        </is>
-      </c>
-      <c r="F5" s="9" t="n"/>
-      <c r="G5" s="9" t="n"/>
+      <c r="D5" s="11" t="n"/>
+      <c r="E5" s="11" t="n"/>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
       <c r="H5" s="1" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>

</xml_diff>

<commit_message>
Add borders to statuses
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -42,7 +42,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -73,6 +73,18 @@
         <bgColor rgb="0032a852"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0032CD32"/>
+        <bgColor rgb="0032CD32"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -98,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -124,6 +136,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -633,12 +647,12 @@
       <c r="G2" s="4" t="n"/>
       <c r="H2" s="4" t="n"/>
       <c r="I2" s="4" t="n"/>
-      <c r="J2" s="4" t="n"/>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="1" t="n"/>
       <c r="M2" s="1" t="n"/>
       <c r="N2" s="1" t="n"/>
@@ -687,32 +701,32 @@
       <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>01/May - 07/May</t>
+          <t>10/May - 16/May</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>08/May - 14/May</t>
+          <t>17/May - 23/May</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
-          <t>15/May - 21/May</t>
+          <t>24/May - 30/May</t>
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr">
         <is>
-          <t>22/May - 28/May</t>
+          <t>31/May - 06/Jun</t>
         </is>
       </c>
       <c r="J3" s="5" t="inlineStr">
         <is>
-          <t>29/May - 04/Jun</t>
+          <t>07/Jun - 13/Jun</t>
         </is>
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>05/Jun - 11/Jun</t>
+          <t>14/Jun - 20/Jun</t>
         </is>
       </c>
       <c r="L3" s="1" t="n"/>
@@ -821,12 +835,12 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>01-May-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>21-May-2024</t>
+          <t>30-May-2024</t>
         </is>
       </c>
       <c r="F5" s="9" t="n"/>
@@ -889,12 +903,12 @@
       </c>
       <c r="D6" s="11" t="inlineStr">
         <is>
-          <t>01-May-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
-          <t>07-May-2024</t>
+          <t>16-May-2024</t>
         </is>
       </c>
       <c r="F6" s="12" t="n"/>
@@ -957,12 +971,12 @@
       </c>
       <c r="D7" s="11" t="inlineStr">
         <is>
-          <t>08-May-2024</t>
+          <t>17-May-2024</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
         <is>
-          <t>14-May-2024</t>
+          <t>23-May-2024</t>
         </is>
       </c>
       <c r="F7" s="1" t="n"/>
@@ -1025,12 +1039,12 @@
       </c>
       <c r="D8" s="11" t="inlineStr">
         <is>
-          <t>15-May-2024</t>
+          <t>24-May-2024</t>
         </is>
       </c>
       <c r="E8" s="11" t="inlineStr">
         <is>
-          <t>21-May-2024</t>
+          <t>30-May-2024</t>
         </is>
       </c>
       <c r="F8" s="1" t="n"/>
@@ -1093,12 +1107,12 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>22-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
         <is>
-          <t>11-Jun-2024</t>
+          <t>20-Jun-2024</t>
         </is>
       </c>
       <c r="F9" s="1" t="n"/>
@@ -1161,12 +1175,12 @@
       </c>
       <c r="D10" s="11" t="inlineStr">
         <is>
-          <t>22-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
         <is>
-          <t>28-May-2024</t>
+          <t>06-Jun-2024</t>
         </is>
       </c>
       <c r="F10" s="1" t="n"/>
@@ -1229,12 +1243,12 @@
       </c>
       <c r="D11" s="11" t="inlineStr">
         <is>
-          <t>29-May-2024</t>
+          <t>07-Jun-2024</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
         <is>
-          <t>04-Jun-2024</t>
+          <t>13-Jun-2024</t>
         </is>
       </c>
       <c r="F11" s="1" t="n"/>
@@ -1297,12 +1311,12 @@
       </c>
       <c r="D12" s="11" t="inlineStr">
         <is>
-          <t>05-Jun-2024</t>
+          <t>14-Jun-2024</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
-          <t>11-Jun-2024</t>
+          <t>20-Jun-2024</t>
         </is>
       </c>
       <c r="F12" s="1" t="n"/>
@@ -5934,12 +5948,12 @@
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="B9"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="K2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="F1:K1"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="C5"/>
     <mergeCell ref="C9"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6057,12 +6071,12 @@
       <c r="G2" s="4" t="n"/>
       <c r="H2" s="4" t="n"/>
       <c r="I2" s="4" t="n"/>
-      <c r="J2" s="4" t="n"/>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="1" t="n"/>
       <c r="M2" s="1" t="n"/>
       <c r="N2" s="1" t="n"/>
@@ -6111,32 +6125,32 @@
       <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>01/May - 07/May</t>
+          <t>10/May - 16/May</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>08/May - 14/May</t>
+          <t>17/May - 23/May</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
-          <t>15/May - 21/May</t>
+          <t>24/May - 30/May</t>
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr">
         <is>
-          <t>22/May - 28/May</t>
+          <t>31/May - 06/Jun</t>
         </is>
       </c>
       <c r="J3" s="5" t="inlineStr">
         <is>
-          <t>29/May - 04/Jun</t>
+          <t>07/Jun - 13/Jun</t>
         </is>
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>05/Jun - 11/Jun</t>
+          <t>14/Jun - 20/Jun</t>
         </is>
       </c>
       <c r="L3" s="1" t="n"/>
@@ -6245,12 +6259,12 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>01-May-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>21-May-2024</t>
+          <t>30-May-2024</t>
         </is>
       </c>
       <c r="F5" s="9" t="n"/>
@@ -6469,12 +6483,12 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>22-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
         <is>
-          <t>11-Jun-2024</t>
+          <t>20-Jun-2024</t>
         </is>
       </c>
       <c r="F9" s="1" t="n"/>
@@ -11262,12 +11276,12 @@
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="B9"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="K2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="F1:K1"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="C5"/>
     <mergeCell ref="C9"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -11541,17 +11555,17 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>01-May-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>21-May-2024</t>
+          <t>30-May-2024</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" s="13" t="inlineStr">
         <is>
-          <t>Ongoing</t>
+          <t>At Risk</t>
         </is>
       </c>
       <c r="G5" s="1" t="n"/>
@@ -11613,15 +11627,15 @@
       </c>
       <c r="D6" s="11" t="inlineStr">
         <is>
-          <t>01-May-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
-          <t>07-May-2024</t>
+          <t>16-May-2024</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="11" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
@@ -11685,17 +11699,17 @@
       </c>
       <c r="D7" s="11" t="inlineStr">
         <is>
-          <t>08-May-2024</t>
+          <t>17-May-2024</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
         <is>
-          <t>14-May-2024</t>
+          <t>23-May-2024</t>
         </is>
       </c>
-      <c r="F7" s="1" t="inlineStr">
+      <c r="F7" s="11" t="inlineStr">
         <is>
-          <t>Delayed</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="G7" s="1" t="n"/>
@@ -11757,15 +11771,15 @@
       </c>
       <c r="D8" s="11" t="inlineStr">
         <is>
-          <t>15-May-2024</t>
+          <t>24-May-2024</t>
         </is>
       </c>
       <c r="E8" s="11" t="inlineStr">
         <is>
-          <t>21-May-2024</t>
+          <t>30-May-2024</t>
         </is>
       </c>
-      <c r="F8" s="1" t="inlineStr">
+      <c r="F8" s="11" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
@@ -11829,15 +11843,15 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>22-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
         <is>
-          <t>11-Jun-2024</t>
+          <t>20-Jun-2024</t>
         </is>
       </c>
-      <c r="F9" s="1" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
@@ -11901,15 +11915,15 @@
       </c>
       <c r="D10" s="11" t="inlineStr">
         <is>
-          <t>22-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
         <is>
-          <t>28-May-2024</t>
+          <t>06-Jun-2024</t>
         </is>
       </c>
-      <c r="F10" s="1" t="inlineStr">
+      <c r="F10" s="11" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
@@ -11973,15 +11987,15 @@
       </c>
       <c r="D11" s="11" t="inlineStr">
         <is>
-          <t>29-May-2024</t>
+          <t>07-Jun-2024</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
         <is>
-          <t>04-Jun-2024</t>
+          <t>13-Jun-2024</t>
         </is>
       </c>
-      <c r="F11" s="1" t="inlineStr">
+      <c r="F11" s="11" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
@@ -12045,15 +12059,15 @@
       </c>
       <c r="D12" s="11" t="inlineStr">
         <is>
-          <t>05-Jun-2024</t>
+          <t>14-Jun-2024</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
-          <t>11-Jun-2024</t>
+          <t>20-Jun-2024</t>
         </is>
       </c>
-      <c r="F12" s="1" t="inlineStr">
+      <c r="F12" s="11" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>

</xml_diff>

<commit_message>
Fixed at Risk and Delayed Milestones
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -42,7 +42,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -71,6 +71,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="0032a852"/>
         <bgColor rgb="0032a852"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -110,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -136,8 +142,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -562,9 +569,6 @@
     <col width="20" customWidth="1" min="12" max="12"/>
     <col width="20" customWidth="1" min="13" max="13"/>
     <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -602,9 +606,9 @@
       <c r="L1" s="4" t="n"/>
       <c r="M1" s="4" t="n"/>
       <c r="N1" s="4" t="n"/>
-      <c r="O1" s="4" t="n"/>
-      <c r="P1" s="4" t="n"/>
-      <c r="Q1" s="4" t="n"/>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
       <c r="R1" s="1" t="n"/>
       <c r="S1" s="1" t="n"/>
       <c r="T1" s="1" t="n"/>
@@ -651,24 +655,24 @@
         </is>
       </c>
       <c r="G2" s="4" t="n"/>
-      <c r="H2" s="4" t="n"/>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>May</t>
         </is>
       </c>
+      <c r="I2" s="4" t="n"/>
       <c r="J2" s="4" t="n"/>
       <c r="K2" s="4" t="n"/>
-      <c r="L2" s="4" t="n"/>
-      <c r="M2" s="4" t="n"/>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="O2" s="4" t="n"/>
-      <c r="P2" s="4" t="n"/>
-      <c r="Q2" s="4" t="n"/>
+      <c r="M2" s="4" t="n"/>
+      <c r="N2" s="4" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
       <c r="R2" s="1" t="n"/>
       <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
@@ -711,64 +715,52 @@
       <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>10/Apr - 16/Apr</t>
+          <t>20/Apr - 26/Apr</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>17/Apr - 23/Apr</t>
+          <t>27/Apr - 03/May</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
-          <t>24/Apr - 30/Apr</t>
+          <t>04/May - 10/May</t>
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr">
         <is>
-          <t>01/May - 07/May</t>
+          <t>11/May - 17/May</t>
         </is>
       </c>
       <c r="J3" s="5" t="inlineStr">
         <is>
-          <t>08/May - 14/May</t>
+          <t>18/May - 24/May</t>
         </is>
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>15/May - 21/May</t>
+          <t>25/May - 31/May</t>
         </is>
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
-          <t>22/May - 28/May</t>
+          <t>01/Jun - 07/Jun</t>
         </is>
       </c>
       <c r="M3" s="5" t="inlineStr">
         <is>
-          <t>29/May - 04/Jun</t>
+          <t>08/Jun - 14/Jun</t>
         </is>
       </c>
       <c r="N3" s="5" t="inlineStr">
         <is>
-          <t>05/Jun - 11/Jun</t>
+          <t>15/Jun - 21/Jun</t>
         </is>
       </c>
-      <c r="O3" s="5" t="inlineStr">
-        <is>
-          <t>12/Jun - 18/Jun</t>
-        </is>
-      </c>
-      <c r="P3" s="5" t="inlineStr">
-        <is>
-          <t>19/Jun - 25/Jun</t>
-        </is>
-      </c>
-      <c r="Q3" s="5" t="inlineStr">
-        <is>
-          <t>26/Jun - 02/Jul</t>
-        </is>
-      </c>
+      <c r="O3" s="1" t="n"/>
+      <c r="P3" s="1" t="n"/>
+      <c r="Q3" s="1" t="n"/>
       <c r="R3" s="1" t="n"/>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="n"/>
@@ -864,22 +856,22 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Requirements Gathering</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>10-Apr-2024</t>
+          <t>20-Apr-2024</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>23-Apr-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
       <c r="F5" s="9" t="n"/>
       <c r="G5" s="9" t="n"/>
-      <c r="H5" s="1" t="n"/>
+      <c r="H5" s="9" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
       <c r="K5" s="1" t="n"/>
@@ -932,17 +924,17 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>Initial Meeting</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D6" s="11" t="inlineStr">
         <is>
-          <t>10-Apr-2024</t>
+          <t>20-Apr-2024</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
-          <t>16-Apr-2024</t>
+          <t>26-Apr-2024</t>
         </is>
       </c>
       <c r="F6" s="12" t="n"/>
@@ -1000,21 +992,21 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>Stakeholder Interviews</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D7" s="11" t="inlineStr">
         <is>
-          <t>10-Apr-2024</t>
+          <t>27-Apr-2024</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
         <is>
-          <t>16-Apr-2024</t>
+          <t>03-May-2024</t>
         </is>
       </c>
-      <c r="F7" s="12" t="n"/>
-      <c r="G7" s="1" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="12" t="n"/>
       <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n"/>
       <c r="J7" s="1" t="n"/>
@@ -1068,22 +1060,22 @@
       </c>
       <c r="C8" s="10" t="inlineStr">
         <is>
-          <t>Requirements Documentation</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D8" s="11" t="inlineStr">
         <is>
-          <t>10-Apr-2024</t>
+          <t>04-May-2024</t>
         </is>
       </c>
       <c r="E8" s="11" t="inlineStr">
         <is>
-          <t>23-Apr-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
-      <c r="F8" s="12" t="n"/>
-      <c r="G8" s="12" t="n"/>
-      <c r="H8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="12" t="n"/>
       <c r="I8" s="1" t="n"/>
       <c r="J8" s="1" t="n"/>
       <c r="K8" s="1" t="n"/>
@@ -1136,25 +1128,25 @@
       </c>
       <c r="C9" s="7" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>24-Apr-2024</t>
+          <t>11-May-2024</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
         <is>
-          <t>07-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
       <c r="F9" s="1" t="n"/>
       <c r="G9" s="1" t="n"/>
-      <c r="H9" s="9" t="n"/>
+      <c r="H9" s="1" t="n"/>
       <c r="I9" s="9" t="n"/>
-      <c r="J9" s="1" t="n"/>
-      <c r="K9" s="1" t="n"/>
+      <c r="J9" s="9" t="n"/>
+      <c r="K9" s="9" t="n"/>
       <c r="L9" s="1" t="n"/>
       <c r="M9" s="1" t="n"/>
       <c r="N9" s="1" t="n"/>
@@ -1204,23 +1196,23 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>System Architecture Design</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D10" s="11" t="inlineStr">
         <is>
-          <t>24-Apr-2024</t>
+          <t>11-May-2024</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
         <is>
-          <t>30-Apr-2024</t>
+          <t>17-May-2024</t>
         </is>
       </c>
       <c r="F10" s="1" t="n"/>
       <c r="G10" s="1" t="n"/>
-      <c r="H10" s="12" t="n"/>
-      <c r="I10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
+      <c r="I10" s="12" t="n"/>
       <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
       <c r="L10" s="1" t="n"/>
@@ -1272,24 +1264,24 @@
       </c>
       <c r="C11" s="10" t="inlineStr">
         <is>
-          <t>Database Schema Design</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D11" s="11" t="inlineStr">
         <is>
-          <t>24-Apr-2024</t>
+          <t>18-May-2024</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
         <is>
-          <t>07-May-2024</t>
+          <t>24-May-2024</t>
         </is>
       </c>
       <c r="F11" s="1" t="n"/>
       <c r="G11" s="1" t="n"/>
-      <c r="H11" s="12" t="n"/>
-      <c r="I11" s="12" t="n"/>
-      <c r="J11" s="1" t="n"/>
+      <c r="H11" s="1" t="n"/>
+      <c r="I11" s="1" t="n"/>
+      <c r="J11" s="12" t="n"/>
       <c r="K11" s="1" t="n"/>
       <c r="L11" s="1" t="n"/>
       <c r="M11" s="1" t="n"/>
@@ -1340,25 +1332,25 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>UI/UX Design</t>
+          <t>F</t>
         </is>
       </c>
       <c r="D12" s="11" t="inlineStr">
         <is>
-          <t>01-May-2024</t>
+          <t>25-May-2024</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
-          <t>07-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
       <c r="F12" s="1" t="n"/>
       <c r="G12" s="1" t="n"/>
       <c r="H12" s="1" t="n"/>
-      <c r="I12" s="12" t="n"/>
+      <c r="I12" s="1" t="n"/>
       <c r="J12" s="1" t="n"/>
-      <c r="K12" s="1" t="n"/>
+      <c r="K12" s="12" t="n"/>
       <c r="L12" s="1" t="n"/>
       <c r="M12" s="1" t="n"/>
       <c r="N12" s="1" t="n"/>
@@ -1408,28 +1400,28 @@
       </c>
       <c r="C13" s="7" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>08-May-2024</t>
+          <t>01-Jun-2024</t>
         </is>
       </c>
       <c r="E13" s="8" t="inlineStr">
         <is>
-          <t>28-May-2024</t>
+          <t>21-Jun-2024</t>
         </is>
       </c>
       <c r="F13" s="1" t="n"/>
       <c r="G13" s="1" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
-      <c r="J13" s="9" t="n"/>
-      <c r="K13" s="9" t="n"/>
+      <c r="J13" s="1" t="n"/>
+      <c r="K13" s="1" t="n"/>
       <c r="L13" s="9" t="n"/>
-      <c r="M13" s="1" t="n"/>
-      <c r="N13" s="1" t="n"/>
+      <c r="M13" s="9" t="n"/>
+      <c r="N13" s="9" t="n"/>
       <c r="O13" s="1" t="n"/>
       <c r="P13" s="1" t="n"/>
       <c r="Q13" s="1" t="n"/>
@@ -1476,26 +1468,26 @@
       </c>
       <c r="C14" s="10" t="inlineStr">
         <is>
-          <t>Frontend Development</t>
+          <t>G</t>
         </is>
       </c>
       <c r="D14" s="11" t="inlineStr">
         <is>
-          <t>08-May-2024</t>
+          <t>01-Jun-2024</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
         <is>
-          <t>14-May-2024</t>
+          <t>07-Jun-2024</t>
         </is>
       </c>
       <c r="F14" s="1" t="n"/>
       <c r="G14" s="1" t="n"/>
       <c r="H14" s="1" t="n"/>
       <c r="I14" s="1" t="n"/>
-      <c r="J14" s="12" t="n"/>
+      <c r="J14" s="1" t="n"/>
       <c r="K14" s="1" t="n"/>
-      <c r="L14" s="1" t="n"/>
+      <c r="L14" s="12" t="n"/>
       <c r="M14" s="1" t="n"/>
       <c r="N14" s="1" t="n"/>
       <c r="O14" s="1" t="n"/>
@@ -1544,17 +1536,17 @@
       </c>
       <c r="C15" s="10" t="inlineStr">
         <is>
-          <t>Backend Development</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D15" s="11" t="inlineStr">
         <is>
-          <t>15-May-2024</t>
+          <t>08-Jun-2024</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
         <is>
-          <t>28-May-2024</t>
+          <t>14-Jun-2024</t>
         </is>
       </c>
       <c r="F15" s="1" t="n"/>
@@ -1562,9 +1554,9 @@
       <c r="H15" s="1" t="n"/>
       <c r="I15" s="1" t="n"/>
       <c r="J15" s="1" t="n"/>
-      <c r="K15" s="12" t="n"/>
-      <c r="L15" s="12" t="n"/>
-      <c r="M15" s="1" t="n"/>
+      <c r="K15" s="1" t="n"/>
+      <c r="L15" s="1" t="n"/>
+      <c r="M15" s="12" t="n"/>
       <c r="N15" s="1" t="n"/>
       <c r="O15" s="1" t="n"/>
       <c r="P15" s="1" t="n"/>
@@ -1612,17 +1604,17 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>Integration</t>
+          <t>I</t>
         </is>
       </c>
       <c r="D16" s="11" t="inlineStr">
         <is>
-          <t>22-May-2024</t>
+          <t>15-Jun-2024</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
         <is>
-          <t>28-May-2024</t>
+          <t>21-Jun-2024</t>
         </is>
       </c>
       <c r="F16" s="1" t="n"/>
@@ -1631,9 +1623,9 @@
       <c r="I16" s="1" t="n"/>
       <c r="J16" s="1" t="n"/>
       <c r="K16" s="1" t="n"/>
-      <c r="L16" s="12" t="n"/>
+      <c r="L16" s="1" t="n"/>
       <c r="M16" s="1" t="n"/>
-      <c r="N16" s="1" t="n"/>
+      <c r="N16" s="12" t="n"/>
       <c r="O16" s="1" t="n"/>
       <c r="P16" s="1" t="n"/>
       <c r="Q16" s="1" t="n"/>
@@ -1673,26 +1665,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="7" t="inlineStr">
-        <is>
-          <t>Task 4</t>
-        </is>
-      </c>
-      <c r="C17" s="7" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="D17" s="8" t="inlineStr">
-        <is>
-          <t>29-May-2024</t>
-        </is>
-      </c>
-      <c r="E17" s="8" t="inlineStr">
-        <is>
-          <t>11-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B17" s="6" t="n"/>
+      <c r="C17" s="6" t="n"/>
+      <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n"/>
       <c r="F17" s="1" t="n"/>
       <c r="G17" s="1" t="n"/>
       <c r="H17" s="1" t="n"/>
@@ -1700,8 +1676,8 @@
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
       <c r="L17" s="1" t="n"/>
-      <c r="M17" s="9" t="n"/>
-      <c r="N17" s="9" t="n"/>
+      <c r="M17" s="1" t="n"/>
+      <c r="N17" s="1" t="n"/>
       <c r="O17" s="1" t="n"/>
       <c r="P17" s="1" t="n"/>
       <c r="Q17" s="1" t="n"/>
@@ -1741,26 +1717,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="10" t="inlineStr">
-        <is>
-          <t>4.1</t>
-        </is>
-      </c>
-      <c r="C18" s="10" t="inlineStr">
-        <is>
-          <t>Unit Testing</t>
-        </is>
-      </c>
-      <c r="D18" s="11" t="inlineStr">
-        <is>
-          <t>29-May-2024</t>
-        </is>
-      </c>
-      <c r="E18" s="11" t="inlineStr">
-        <is>
-          <t>04-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B18" s="6" t="n"/>
+      <c r="C18" s="6" t="n"/>
+      <c r="D18" s="1" t="n"/>
+      <c r="E18" s="1" t="n"/>
       <c r="F18" s="1" t="n"/>
       <c r="G18" s="1" t="n"/>
       <c r="H18" s="1" t="n"/>
@@ -1768,7 +1728,7 @@
       <c r="J18" s="1" t="n"/>
       <c r="K18" s="1" t="n"/>
       <c r="L18" s="1" t="n"/>
-      <c r="M18" s="12" t="n"/>
+      <c r="M18" s="1" t="n"/>
       <c r="N18" s="1" t="n"/>
       <c r="O18" s="1" t="n"/>
       <c r="P18" s="1" t="n"/>
@@ -1809,26 +1769,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="10" t="inlineStr">
-        <is>
-          <t>4.2</t>
-        </is>
-      </c>
-      <c r="C19" s="10" t="inlineStr">
-        <is>
-          <t>Integration Testing</t>
-        </is>
-      </c>
-      <c r="D19" s="11" t="inlineStr">
-        <is>
-          <t>29-May-2024</t>
-        </is>
-      </c>
-      <c r="E19" s="11" t="inlineStr">
-        <is>
-          <t>11-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B19" s="6" t="n"/>
+      <c r="C19" s="6" t="n"/>
+      <c r="D19" s="1" t="n"/>
+      <c r="E19" s="1" t="n"/>
       <c r="F19" s="1" t="n"/>
       <c r="G19" s="1" t="n"/>
       <c r="H19" s="1" t="n"/>
@@ -1836,8 +1780,8 @@
       <c r="J19" s="1" t="n"/>
       <c r="K19" s="1" t="n"/>
       <c r="L19" s="1" t="n"/>
-      <c r="M19" s="12" t="n"/>
-      <c r="N19" s="12" t="n"/>
+      <c r="M19" s="1" t="n"/>
+      <c r="N19" s="1" t="n"/>
       <c r="O19" s="1" t="n"/>
       <c r="P19" s="1" t="n"/>
       <c r="Q19" s="1" t="n"/>
@@ -1877,26 +1821,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="10" t="inlineStr">
-        <is>
-          <t>4.3</t>
-        </is>
-      </c>
-      <c r="C20" s="10" t="inlineStr">
-        <is>
-          <t>User Acceptance Testing</t>
-        </is>
-      </c>
-      <c r="D20" s="11" t="inlineStr">
-        <is>
-          <t>05-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E20" s="11" t="inlineStr">
-        <is>
-          <t>11-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B20" s="6" t="n"/>
+      <c r="C20" s="6" t="n"/>
+      <c r="D20" s="1" t="n"/>
+      <c r="E20" s="1" t="n"/>
       <c r="F20" s="1" t="n"/>
       <c r="G20" s="1" t="n"/>
       <c r="H20" s="1" t="n"/>
@@ -1905,7 +1833,7 @@
       <c r="K20" s="1" t="n"/>
       <c r="L20" s="1" t="n"/>
       <c r="M20" s="1" t="n"/>
-      <c r="N20" s="12" t="n"/>
+      <c r="N20" s="1" t="n"/>
       <c r="O20" s="1" t="n"/>
       <c r="P20" s="1" t="n"/>
       <c r="Q20" s="1" t="n"/>
@@ -1945,26 +1873,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="7" t="inlineStr">
-        <is>
-          <t>Task 5</t>
-        </is>
-      </c>
-      <c r="C21" s="7" t="inlineStr">
-        <is>
-          <t>Deployment</t>
-        </is>
-      </c>
-      <c r="D21" s="8" t="inlineStr">
-        <is>
-          <t>12-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E21" s="8" t="inlineStr">
-        <is>
-          <t>18-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n"/>
       <c r="F21" s="1" t="n"/>
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
@@ -1974,7 +1886,7 @@
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n"/>
       <c r="N21" s="1" t="n"/>
-      <c r="O21" s="9" t="n"/>
+      <c r="O21" s="1" t="n"/>
       <c r="P21" s="1" t="n"/>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
@@ -2013,26 +1925,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="10" t="inlineStr">
-        <is>
-          <t>5.1</t>
-        </is>
-      </c>
-      <c r="C22" s="10" t="inlineStr">
-        <is>
-          <t>Prepare Deployment Environment</t>
-        </is>
-      </c>
-      <c r="D22" s="11" t="inlineStr">
-        <is>
-          <t>12-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E22" s="11" t="inlineStr">
-        <is>
-          <t>18-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B22" s="6" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="1" t="n"/>
+      <c r="E22" s="1" t="n"/>
       <c r="F22" s="1" t="n"/>
       <c r="G22" s="1" t="n"/>
       <c r="H22" s="1" t="n"/>
@@ -2042,7 +1938,7 @@
       <c r="L22" s="1" t="n"/>
       <c r="M22" s="1" t="n"/>
       <c r="N22" s="1" t="n"/>
-      <c r="O22" s="12" t="n"/>
+      <c r="O22" s="1" t="n"/>
       <c r="P22" s="1" t="n"/>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
@@ -2081,26 +1977,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="10" t="inlineStr">
-        <is>
-          <t>5.2</t>
-        </is>
-      </c>
-      <c r="C23" s="10" t="inlineStr">
-        <is>
-          <t>Deployment</t>
-        </is>
-      </c>
-      <c r="D23" s="11" t="inlineStr">
-        <is>
-          <t>12-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E23" s="11" t="inlineStr">
-        <is>
-          <t>18-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B23" s="6" t="n"/>
+      <c r="C23" s="6" t="n"/>
+      <c r="D23" s="1" t="n"/>
+      <c r="E23" s="1" t="n"/>
       <c r="F23" s="1" t="n"/>
       <c r="G23" s="1" t="n"/>
       <c r="H23" s="1" t="n"/>
@@ -2110,7 +1990,7 @@
       <c r="L23" s="1" t="n"/>
       <c r="M23" s="1" t="n"/>
       <c r="N23" s="1" t="n"/>
-      <c r="O23" s="12" t="n"/>
+      <c r="O23" s="1" t="n"/>
       <c r="P23" s="1" t="n"/>
       <c r="Q23" s="1" t="n"/>
       <c r="R23" s="1" t="n"/>
@@ -2149,26 +2029,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="10" t="inlineStr">
-        <is>
-          <t>5.3</t>
-        </is>
-      </c>
-      <c r="C24" s="10" t="inlineStr">
-        <is>
-          <t>Post-Deployment Verification</t>
-        </is>
-      </c>
-      <c r="D24" s="11" t="inlineStr">
-        <is>
-          <t>12-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E24" s="11" t="inlineStr">
-        <is>
-          <t>18-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B24" s="6" t="n"/>
+      <c r="C24" s="6" t="n"/>
+      <c r="D24" s="1" t="n"/>
+      <c r="E24" s="1" t="n"/>
       <c r="F24" s="1" t="n"/>
       <c r="G24" s="1" t="n"/>
       <c r="H24" s="1" t="n"/>
@@ -2178,7 +2042,7 @@
       <c r="L24" s="1" t="n"/>
       <c r="M24" s="1" t="n"/>
       <c r="N24" s="1" t="n"/>
-      <c r="O24" s="12" t="n"/>
+      <c r="O24" s="1" t="n"/>
       <c r="P24" s="1" t="n"/>
       <c r="Q24" s="1" t="n"/>
       <c r="R24" s="1" t="n"/>
@@ -2217,26 +2081,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="7" t="inlineStr">
-        <is>
-          <t>Task 6</t>
-        </is>
-      </c>
-      <c r="C25" s="7" t="inlineStr">
-        <is>
-          <t>Maintenance</t>
-        </is>
-      </c>
-      <c r="D25" s="8" t="inlineStr">
-        <is>
-          <t>19-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E25" s="8" t="inlineStr">
-        <is>
-          <t>02-Jul-2024</t>
-        </is>
-      </c>
+      <c r="B25" s="6" t="n"/>
+      <c r="C25" s="6" t="n"/>
+      <c r="D25" s="1" t="n"/>
+      <c r="E25" s="1" t="n"/>
       <c r="F25" s="1" t="n"/>
       <c r="G25" s="1" t="n"/>
       <c r="H25" s="1" t="n"/>
@@ -2247,8 +2095,8 @@
       <c r="M25" s="1" t="n"/>
       <c r="N25" s="1" t="n"/>
       <c r="O25" s="1" t="n"/>
-      <c r="P25" s="9" t="n"/>
-      <c r="Q25" s="9" t="n"/>
+      <c r="P25" s="1" t="n"/>
+      <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
       <c r="S25" s="1" t="n"/>
       <c r="T25" s="1" t="n"/>
@@ -2285,26 +2133,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="10" t="inlineStr">
-        <is>
-          <t>6.1</t>
-        </is>
-      </c>
-      <c r="C26" s="10" t="inlineStr">
-        <is>
-          <t>Bug Fixing</t>
-        </is>
-      </c>
-      <c r="D26" s="11" t="inlineStr">
-        <is>
-          <t>19-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E26" s="11" t="inlineStr">
-        <is>
-          <t>25-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B26" s="6" t="n"/>
+      <c r="C26" s="6" t="n"/>
+      <c r="D26" s="1" t="n"/>
+      <c r="E26" s="1" t="n"/>
       <c r="F26" s="1" t="n"/>
       <c r="G26" s="1" t="n"/>
       <c r="H26" s="1" t="n"/>
@@ -2315,7 +2147,7 @@
       <c r="M26" s="1" t="n"/>
       <c r="N26" s="1" t="n"/>
       <c r="O26" s="1" t="n"/>
-      <c r="P26" s="12" t="n"/>
+      <c r="P26" s="1" t="n"/>
       <c r="Q26" s="1" t="n"/>
       <c r="R26" s="1" t="n"/>
       <c r="S26" s="1" t="n"/>
@@ -2353,26 +2185,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="10" t="inlineStr">
-        <is>
-          <t>6.2</t>
-        </is>
-      </c>
-      <c r="C27" s="10" t="inlineStr">
-        <is>
-          <t>Performance Tuning</t>
-        </is>
-      </c>
-      <c r="D27" s="11" t="inlineStr">
-        <is>
-          <t>19-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E27" s="11" t="inlineStr">
-        <is>
-          <t>25-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B27" s="6" t="n"/>
+      <c r="C27" s="6" t="n"/>
+      <c r="D27" s="1" t="n"/>
+      <c r="E27" s="1" t="n"/>
       <c r="F27" s="1" t="n"/>
       <c r="G27" s="1" t="n"/>
       <c r="H27" s="1" t="n"/>
@@ -2383,7 +2199,7 @@
       <c r="M27" s="1" t="n"/>
       <c r="N27" s="1" t="n"/>
       <c r="O27" s="1" t="n"/>
-      <c r="P27" s="12" t="n"/>
+      <c r="P27" s="1" t="n"/>
       <c r="Q27" s="1" t="n"/>
       <c r="R27" s="1" t="n"/>
       <c r="S27" s="1" t="n"/>
@@ -2421,26 +2237,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="10" t="inlineStr">
-        <is>
-          <t>6.3</t>
-        </is>
-      </c>
-      <c r="C28" s="10" t="inlineStr">
-        <is>
-          <t>User Training</t>
-        </is>
-      </c>
-      <c r="D28" s="11" t="inlineStr">
-        <is>
-          <t>19-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E28" s="11" t="inlineStr">
-        <is>
-          <t>02-Jul-2024</t>
-        </is>
-      </c>
+      <c r="B28" s="6" t="n"/>
+      <c r="C28" s="6" t="n"/>
+      <c r="D28" s="1" t="n"/>
+      <c r="E28" s="1" t="n"/>
       <c r="F28" s="1" t="n"/>
       <c r="G28" s="1" t="n"/>
       <c r="H28" s="1" t="n"/>
@@ -2451,8 +2251,8 @@
       <c r="M28" s="1" t="n"/>
       <c r="N28" s="1" t="n"/>
       <c r="O28" s="1" t="n"/>
-      <c r="P28" s="12" t="n"/>
-      <c r="Q28" s="12" t="n"/>
+      <c r="P28" s="1" t="n"/>
+      <c r="Q28" s="1" t="n"/>
       <c r="R28" s="1" t="n"/>
       <c r="S28" s="1" t="n"/>
       <c r="T28" s="1" t="n"/>
@@ -6232,27 +6032,21 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="14">
+    <mergeCell ref="B5"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="B1:B3"/>
     <mergeCell ref="B9"/>
-    <mergeCell ref="C17"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B5"/>
-    <mergeCell ref="C13"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="B25"/>
-    <mergeCell ref="C5"/>
-    <mergeCell ref="B21"/>
-    <mergeCell ref="C25"/>
-    <mergeCell ref="F1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="C9"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B17"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="B13"/>
-    <mergeCell ref="C21"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C13"/>
+    <mergeCell ref="F1:N1"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="C5"/>
+    <mergeCell ref="C9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6285,9 +6079,6 @@
     <col width="20" customWidth="1" min="12" max="12"/>
     <col width="20" customWidth="1" min="13" max="13"/>
     <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6325,9 +6116,9 @@
       <c r="L1" s="4" t="n"/>
       <c r="M1" s="4" t="n"/>
       <c r="N1" s="4" t="n"/>
-      <c r="O1" s="4" t="n"/>
-      <c r="P1" s="4" t="n"/>
-      <c r="Q1" s="4" t="n"/>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
       <c r="R1" s="1" t="n"/>
       <c r="S1" s="1" t="n"/>
       <c r="T1" s="1" t="n"/>
@@ -6374,24 +6165,24 @@
         </is>
       </c>
       <c r="G2" s="4" t="n"/>
-      <c r="H2" s="4" t="n"/>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>May</t>
         </is>
       </c>
+      <c r="I2" s="4" t="n"/>
       <c r="J2" s="4" t="n"/>
       <c r="K2" s="4" t="n"/>
-      <c r="L2" s="4" t="n"/>
-      <c r="M2" s="4" t="n"/>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="O2" s="4" t="n"/>
-      <c r="P2" s="4" t="n"/>
-      <c r="Q2" s="4" t="n"/>
+      <c r="M2" s="4" t="n"/>
+      <c r="N2" s="4" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
       <c r="R2" s="1" t="n"/>
       <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
@@ -6434,64 +6225,52 @@
       <c r="E3" s="4" t="n"/>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>10/Apr - 16/Apr</t>
+          <t>20/Apr - 26/Apr</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>17/Apr - 23/Apr</t>
+          <t>27/Apr - 03/May</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
-          <t>24/Apr - 30/Apr</t>
+          <t>04/May - 10/May</t>
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr">
         <is>
-          <t>01/May - 07/May</t>
+          <t>11/May - 17/May</t>
         </is>
       </c>
       <c r="J3" s="5" t="inlineStr">
         <is>
-          <t>08/May - 14/May</t>
+          <t>18/May - 24/May</t>
         </is>
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>15/May - 21/May</t>
+          <t>25/May - 31/May</t>
         </is>
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
-          <t>22/May - 28/May</t>
+          <t>01/Jun - 07/Jun</t>
         </is>
       </c>
       <c r="M3" s="5" t="inlineStr">
         <is>
-          <t>29/May - 04/Jun</t>
+          <t>08/Jun - 14/Jun</t>
         </is>
       </c>
       <c r="N3" s="5" t="inlineStr">
         <is>
-          <t>05/Jun - 11/Jun</t>
+          <t>15/Jun - 21/Jun</t>
         </is>
       </c>
-      <c r="O3" s="5" t="inlineStr">
-        <is>
-          <t>12/Jun - 18/Jun</t>
-        </is>
-      </c>
-      <c r="P3" s="5" t="inlineStr">
-        <is>
-          <t>19/Jun - 25/Jun</t>
-        </is>
-      </c>
-      <c r="Q3" s="5" t="inlineStr">
-        <is>
-          <t>26/Jun - 02/Jul</t>
-        </is>
-      </c>
+      <c r="O3" s="1" t="n"/>
+      <c r="P3" s="1" t="n"/>
+      <c r="Q3" s="1" t="n"/>
       <c r="R3" s="1" t="n"/>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="n"/>
@@ -6587,22 +6366,22 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Requirements Gathering</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>10-Apr-2024</t>
+          <t>20-Apr-2024</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>23-Apr-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
       <c r="F5" s="9" t="n"/>
       <c r="G5" s="9" t="n"/>
-      <c r="H5" s="1" t="n"/>
+      <c r="H5" s="9" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
       <c r="K5" s="1" t="n"/>
@@ -6811,25 +6590,25 @@
       </c>
       <c r="C9" s="7" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>24-Apr-2024</t>
+          <t>11-May-2024</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
         <is>
-          <t>07-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
       <c r="F9" s="1" t="n"/>
       <c r="G9" s="1" t="n"/>
-      <c r="H9" s="9" t="n"/>
+      <c r="H9" s="1" t="n"/>
       <c r="I9" s="9" t="n"/>
-      <c r="J9" s="1" t="n"/>
-      <c r="K9" s="1" t="n"/>
+      <c r="J9" s="9" t="n"/>
+      <c r="K9" s="9" t="n"/>
       <c r="L9" s="1" t="n"/>
       <c r="M9" s="1" t="n"/>
       <c r="N9" s="1" t="n"/>
@@ -7035,28 +6814,28 @@
       </c>
       <c r="C13" s="7" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>08-May-2024</t>
+          <t>01-Jun-2024</t>
         </is>
       </c>
       <c r="E13" s="8" t="inlineStr">
         <is>
-          <t>28-May-2024</t>
+          <t>21-Jun-2024</t>
         </is>
       </c>
       <c r="F13" s="1" t="n"/>
       <c r="G13" s="1" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
-      <c r="J13" s="9" t="n"/>
-      <c r="K13" s="9" t="n"/>
+      <c r="J13" s="1" t="n"/>
+      <c r="K13" s="1" t="n"/>
       <c r="L13" s="9" t="n"/>
-      <c r="M13" s="1" t="n"/>
-      <c r="N13" s="1" t="n"/>
+      <c r="M13" s="9" t="n"/>
+      <c r="N13" s="9" t="n"/>
       <c r="O13" s="1" t="n"/>
       <c r="P13" s="1" t="n"/>
       <c r="Q13" s="1" t="n"/>
@@ -7252,26 +7031,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="7" t="inlineStr">
-        <is>
-          <t>Task 4</t>
-        </is>
-      </c>
-      <c r="C17" s="7" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="D17" s="8" t="inlineStr">
-        <is>
-          <t>29-May-2024</t>
-        </is>
-      </c>
-      <c r="E17" s="8" t="inlineStr">
-        <is>
-          <t>11-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B17" s="6" t="n"/>
+      <c r="C17" s="6" t="n"/>
+      <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n"/>
       <c r="F17" s="1" t="n"/>
       <c r="G17" s="1" t="n"/>
       <c r="H17" s="1" t="n"/>
@@ -7279,8 +7042,8 @@
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
       <c r="L17" s="1" t="n"/>
-      <c r="M17" s="9" t="n"/>
-      <c r="N17" s="9" t="n"/>
+      <c r="M17" s="1" t="n"/>
+      <c r="N17" s="1" t="n"/>
       <c r="O17" s="1" t="n"/>
       <c r="P17" s="1" t="n"/>
       <c r="Q17" s="1" t="n"/>
@@ -7476,26 +7239,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="7" t="inlineStr">
-        <is>
-          <t>Task 5</t>
-        </is>
-      </c>
-      <c r="C21" s="7" t="inlineStr">
-        <is>
-          <t>Deployment</t>
-        </is>
-      </c>
-      <c r="D21" s="8" t="inlineStr">
-        <is>
-          <t>12-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E21" s="8" t="inlineStr">
-        <is>
-          <t>18-Jun-2024</t>
-        </is>
-      </c>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n"/>
       <c r="F21" s="1" t="n"/>
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
@@ -7505,7 +7252,7 @@
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n"/>
       <c r="N21" s="1" t="n"/>
-      <c r="O21" s="9" t="n"/>
+      <c r="O21" s="1" t="n"/>
       <c r="P21" s="1" t="n"/>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
@@ -7700,26 +7447,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="7" t="inlineStr">
-        <is>
-          <t>Task 6</t>
-        </is>
-      </c>
-      <c r="C25" s="7" t="inlineStr">
-        <is>
-          <t>Maintenance</t>
-        </is>
-      </c>
-      <c r="D25" s="8" t="inlineStr">
-        <is>
-          <t>19-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E25" s="8" t="inlineStr">
-        <is>
-          <t>02-Jul-2024</t>
-        </is>
-      </c>
+      <c r="B25" s="6" t="n"/>
+      <c r="C25" s="6" t="n"/>
+      <c r="D25" s="1" t="n"/>
+      <c r="E25" s="1" t="n"/>
       <c r="F25" s="1" t="n"/>
       <c r="G25" s="1" t="n"/>
       <c r="H25" s="1" t="n"/>
@@ -7730,8 +7461,8 @@
       <c r="M25" s="1" t="n"/>
       <c r="N25" s="1" t="n"/>
       <c r="O25" s="1" t="n"/>
-      <c r="P25" s="9" t="n"/>
-      <c r="Q25" s="9" t="n"/>
+      <c r="P25" s="1" t="n"/>
+      <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
       <c r="S25" s="1" t="n"/>
       <c r="T25" s="1" t="n"/>
@@ -11667,27 +11398,21 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="14">
+    <mergeCell ref="B5"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="B1:B3"/>
     <mergeCell ref="B9"/>
-    <mergeCell ref="C17"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B5"/>
-    <mergeCell ref="C13"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="B25"/>
-    <mergeCell ref="C5"/>
-    <mergeCell ref="B21"/>
-    <mergeCell ref="C25"/>
-    <mergeCell ref="F1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="C9"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B17"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="B13"/>
-    <mergeCell ref="C21"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C13"/>
+    <mergeCell ref="F1:N1"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="C5"/>
+    <mergeCell ref="C9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -11720,9 +11445,6 @@
     <col width="20" customWidth="1" min="12" max="12"/>
     <col width="20" customWidth="1" min="13" max="13"/>
     <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -11962,22 +11684,22 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Requirements Gathering</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>10-Apr-2024</t>
+          <t>20-Apr-2024</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>23-Apr-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
       <c r="F5" s="13" t="inlineStr">
         <is>
-          <t>At Risk</t>
+          <t>Delayed</t>
         </is>
       </c>
       <c r="G5" s="1" t="n"/>
@@ -12034,17 +11756,17 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>Initial Meeting</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D6" s="11" t="inlineStr">
         <is>
-          <t>10-Apr-2024</t>
+          <t>20-Apr-2024</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
-          <t>16-Apr-2024</t>
+          <t>26-Apr-2024</t>
         </is>
       </c>
       <c r="F6" s="11" t="inlineStr">
@@ -12106,17 +11828,17 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>Stakeholder Interviews</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D7" s="11" t="inlineStr">
         <is>
-          <t>10-Apr-2024</t>
+          <t>27-Apr-2024</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
         <is>
-          <t>16-Apr-2024</t>
+          <t>03-May-2024</t>
         </is>
       </c>
       <c r="F7" s="11" t="inlineStr">
@@ -12178,17 +11900,17 @@
       </c>
       <c r="C8" s="10" t="inlineStr">
         <is>
-          <t>Requirements Documentation</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D8" s="11" t="inlineStr">
         <is>
-          <t>10-Apr-2024</t>
+          <t>04-May-2024</t>
         </is>
       </c>
       <c r="E8" s="11" t="inlineStr">
         <is>
-          <t>23-Apr-2024</t>
+          <t>10-May-2024</t>
         </is>
       </c>
       <c r="F8" s="11" t="inlineStr">
@@ -12250,20 +11972,20 @@
       </c>
       <c r="C9" s="7" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>24-Apr-2024</t>
+          <t>11-May-2024</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
         <is>
-          <t>07-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
-      <c r="F9" s="13" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>At Risk</t>
         </is>
@@ -12322,17 +12044,17 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>System Architecture Design</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D10" s="11" t="inlineStr">
         <is>
-          <t>24-Apr-2024</t>
+          <t>11-May-2024</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
         <is>
-          <t>30-Apr-2024</t>
+          <t>17-May-2024</t>
         </is>
       </c>
       <c r="F10" s="11" t="inlineStr">
@@ -12394,22 +12116,22 @@
       </c>
       <c r="C11" s="10" t="inlineStr">
         <is>
-          <t>Database Schema Design</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D11" s="11" t="inlineStr">
         <is>
-          <t>24-Apr-2024</t>
+          <t>18-May-2024</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
         <is>
-          <t>07-May-2024</t>
+          <t>24-May-2024</t>
         </is>
       </c>
       <c r="F11" s="11" t="inlineStr">
         <is>
-          <t>Delayed</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="G11" s="1" t="n"/>
@@ -12466,22 +12188,22 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>UI/UX Design</t>
+          <t>F</t>
         </is>
       </c>
       <c r="D12" s="11" t="inlineStr">
         <is>
-          <t>01-May-2024</t>
+          <t>25-May-2024</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
-          <t>07-May-2024</t>
+          <t>31-May-2024</t>
         </is>
       </c>
       <c r="F12" s="11" t="inlineStr">
         <is>
-          <t>Delayed</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="G12" s="1" t="n"/>
@@ -12538,22 +12260,22 @@
       </c>
       <c r="C13" s="7" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>08-May-2024</t>
+          <t>01-Jun-2024</t>
         </is>
       </c>
       <c r="E13" s="8" t="inlineStr">
         <is>
-          <t>28-May-2024</t>
+          <t>21-Jun-2024</t>
         </is>
       </c>
-      <c r="F13" s="13" t="inlineStr">
+      <c r="F13" s="15" t="inlineStr">
         <is>
-          <t>At Risk</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="G13" s="1" t="n"/>
@@ -12610,22 +12332,22 @@
       </c>
       <c r="C14" s="10" t="inlineStr">
         <is>
-          <t>Frontend Development</t>
+          <t>G</t>
         </is>
       </c>
       <c r="D14" s="11" t="inlineStr">
         <is>
-          <t>08-May-2024</t>
+          <t>01-Jun-2024</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
         <is>
-          <t>14-May-2024</t>
+          <t>07-Jun-2024</t>
         </is>
       </c>
       <c r="F14" s="11" t="inlineStr">
         <is>
-          <t>Delayed</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="G14" s="1" t="n"/>
@@ -12682,17 +12404,17 @@
       </c>
       <c r="C15" s="10" t="inlineStr">
         <is>
-          <t>Backend Development</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D15" s="11" t="inlineStr">
         <is>
-          <t>15-May-2024</t>
+          <t>08-Jun-2024</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
         <is>
-          <t>28-May-2024</t>
+          <t>14-Jun-2024</t>
         </is>
       </c>
       <c r="F15" s="11" t="inlineStr">
@@ -12754,17 +12476,17 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>Integration</t>
+          <t>I</t>
         </is>
       </c>
       <c r="D16" s="11" t="inlineStr">
         <is>
-          <t>22-May-2024</t>
+          <t>15-Jun-2024</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
         <is>
-          <t>28-May-2024</t>
+          <t>21-Jun-2024</t>
         </is>
       </c>
       <c r="F16" s="11" t="inlineStr">
@@ -12819,31 +12541,11 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="7" t="inlineStr">
-        <is>
-          <t>Task 4</t>
-        </is>
-      </c>
-      <c r="C17" s="7" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="D17" s="8" t="inlineStr">
-        <is>
-          <t>29-May-2024</t>
-        </is>
-      </c>
-      <c r="E17" s="8" t="inlineStr">
-        <is>
-          <t>11-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F17" s="14" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B17" s="6" t="n"/>
+      <c r="C17" s="6" t="n"/>
+      <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n"/>
+      <c r="F17" s="1" t="n"/>
       <c r="G17" s="1" t="n"/>
       <c r="H17" s="1" t="n"/>
       <c r="I17" s="1" t="n"/>
@@ -12891,31 +12593,11 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="10" t="inlineStr">
-        <is>
-          <t>4.1</t>
-        </is>
-      </c>
-      <c r="C18" s="10" t="inlineStr">
-        <is>
-          <t>Unit Testing</t>
-        </is>
-      </c>
-      <c r="D18" s="11" t="inlineStr">
-        <is>
-          <t>29-May-2024</t>
-        </is>
-      </c>
-      <c r="E18" s="11" t="inlineStr">
-        <is>
-          <t>04-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F18" s="11" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B18" s="6" t="n"/>
+      <c r="C18" s="6" t="n"/>
+      <c r="D18" s="1" t="n"/>
+      <c r="E18" s="1" t="n"/>
+      <c r="F18" s="1" t="n"/>
       <c r="G18" s="1" t="n"/>
       <c r="H18" s="1" t="n"/>
       <c r="I18" s="1" t="n"/>
@@ -12963,31 +12645,11 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="10" t="inlineStr">
-        <is>
-          <t>4.2</t>
-        </is>
-      </c>
-      <c r="C19" s="10" t="inlineStr">
-        <is>
-          <t>Integration Testing</t>
-        </is>
-      </c>
-      <c r="D19" s="11" t="inlineStr">
-        <is>
-          <t>29-May-2024</t>
-        </is>
-      </c>
-      <c r="E19" s="11" t="inlineStr">
-        <is>
-          <t>11-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F19" s="11" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B19" s="6" t="n"/>
+      <c r="C19" s="6" t="n"/>
+      <c r="D19" s="1" t="n"/>
+      <c r="E19" s="1" t="n"/>
+      <c r="F19" s="1" t="n"/>
       <c r="G19" s="1" t="n"/>
       <c r="H19" s="1" t="n"/>
       <c r="I19" s="1" t="n"/>
@@ -13035,31 +12697,11 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="10" t="inlineStr">
-        <is>
-          <t>4.3</t>
-        </is>
-      </c>
-      <c r="C20" s="10" t="inlineStr">
-        <is>
-          <t>User Acceptance Testing</t>
-        </is>
-      </c>
-      <c r="D20" s="11" t="inlineStr">
-        <is>
-          <t>05-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E20" s="11" t="inlineStr">
-        <is>
-          <t>11-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F20" s="11" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B20" s="6" t="n"/>
+      <c r="C20" s="6" t="n"/>
+      <c r="D20" s="1" t="n"/>
+      <c r="E20" s="1" t="n"/>
+      <c r="F20" s="1" t="n"/>
       <c r="G20" s="1" t="n"/>
       <c r="H20" s="1" t="n"/>
       <c r="I20" s="1" t="n"/>
@@ -13107,31 +12749,11 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="7" t="inlineStr">
-        <is>
-          <t>Task 5</t>
-        </is>
-      </c>
-      <c r="C21" s="7" t="inlineStr">
-        <is>
-          <t>Deployment</t>
-        </is>
-      </c>
-      <c r="D21" s="8" t="inlineStr">
-        <is>
-          <t>12-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E21" s="8" t="inlineStr">
-        <is>
-          <t>18-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F21" s="14" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n"/>
+      <c r="F21" s="1" t="n"/>
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
       <c r="I21" s="1" t="n"/>
@@ -13179,31 +12801,11 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="10" t="inlineStr">
-        <is>
-          <t>5.1</t>
-        </is>
-      </c>
-      <c r="C22" s="10" t="inlineStr">
-        <is>
-          <t>Prepare Deployment Environment</t>
-        </is>
-      </c>
-      <c r="D22" s="11" t="inlineStr">
-        <is>
-          <t>12-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E22" s="11" t="inlineStr">
-        <is>
-          <t>18-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F22" s="11" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B22" s="6" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="1" t="n"/>
+      <c r="E22" s="1" t="n"/>
+      <c r="F22" s="1" t="n"/>
       <c r="G22" s="1" t="n"/>
       <c r="H22" s="1" t="n"/>
       <c r="I22" s="1" t="n"/>
@@ -13251,31 +12853,11 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="10" t="inlineStr">
-        <is>
-          <t>5.2</t>
-        </is>
-      </c>
-      <c r="C23" s="10" t="inlineStr">
-        <is>
-          <t>Deployment</t>
-        </is>
-      </c>
-      <c r="D23" s="11" t="inlineStr">
-        <is>
-          <t>12-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E23" s="11" t="inlineStr">
-        <is>
-          <t>18-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F23" s="11" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B23" s="6" t="n"/>
+      <c r="C23" s="6" t="n"/>
+      <c r="D23" s="1" t="n"/>
+      <c r="E23" s="1" t="n"/>
+      <c r="F23" s="1" t="n"/>
       <c r="G23" s="1" t="n"/>
       <c r="H23" s="1" t="n"/>
       <c r="I23" s="1" t="n"/>
@@ -13323,31 +12905,11 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="10" t="inlineStr">
-        <is>
-          <t>5.3</t>
-        </is>
-      </c>
-      <c r="C24" s="10" t="inlineStr">
-        <is>
-          <t>Post-Deployment Verification</t>
-        </is>
-      </c>
-      <c r="D24" s="11" t="inlineStr">
-        <is>
-          <t>12-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E24" s="11" t="inlineStr">
-        <is>
-          <t>18-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F24" s="11" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B24" s="6" t="n"/>
+      <c r="C24" s="6" t="n"/>
+      <c r="D24" s="1" t="n"/>
+      <c r="E24" s="1" t="n"/>
+      <c r="F24" s="1" t="n"/>
       <c r="G24" s="1" t="n"/>
       <c r="H24" s="1" t="n"/>
       <c r="I24" s="1" t="n"/>
@@ -13395,31 +12957,11 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="7" t="inlineStr">
-        <is>
-          <t>Task 6</t>
-        </is>
-      </c>
-      <c r="C25" s="7" t="inlineStr">
-        <is>
-          <t>Maintenance</t>
-        </is>
-      </c>
-      <c r="D25" s="8" t="inlineStr">
-        <is>
-          <t>19-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E25" s="8" t="inlineStr">
-        <is>
-          <t>02-Jul-2024</t>
-        </is>
-      </c>
-      <c r="F25" s="14" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B25" s="6" t="n"/>
+      <c r="C25" s="6" t="n"/>
+      <c r="D25" s="1" t="n"/>
+      <c r="E25" s="1" t="n"/>
+      <c r="F25" s="1" t="n"/>
       <c r="G25" s="1" t="n"/>
       <c r="H25" s="1" t="n"/>
       <c r="I25" s="1" t="n"/>
@@ -13467,31 +13009,11 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="10" t="inlineStr">
-        <is>
-          <t>6.1</t>
-        </is>
-      </c>
-      <c r="C26" s="10" t="inlineStr">
-        <is>
-          <t>Bug Fixing</t>
-        </is>
-      </c>
-      <c r="D26" s="11" t="inlineStr">
-        <is>
-          <t>19-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E26" s="11" t="inlineStr">
-        <is>
-          <t>25-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F26" s="11" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B26" s="6" t="n"/>
+      <c r="C26" s="6" t="n"/>
+      <c r="D26" s="1" t="n"/>
+      <c r="E26" s="1" t="n"/>
+      <c r="F26" s="1" t="n"/>
       <c r="G26" s="1" t="n"/>
       <c r="H26" s="1" t="n"/>
       <c r="I26" s="1" t="n"/>
@@ -13539,31 +13061,11 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="10" t="inlineStr">
-        <is>
-          <t>6.2</t>
-        </is>
-      </c>
-      <c r="C27" s="10" t="inlineStr">
-        <is>
-          <t>Performance Tuning</t>
-        </is>
-      </c>
-      <c r="D27" s="11" t="inlineStr">
-        <is>
-          <t>19-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E27" s="11" t="inlineStr">
-        <is>
-          <t>25-Jun-2024</t>
-        </is>
-      </c>
-      <c r="F27" s="11" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B27" s="6" t="n"/>
+      <c r="C27" s="6" t="n"/>
+      <c r="D27" s="1" t="n"/>
+      <c r="E27" s="1" t="n"/>
+      <c r="F27" s="1" t="n"/>
       <c r="G27" s="1" t="n"/>
       <c r="H27" s="1" t="n"/>
       <c r="I27" s="1" t="n"/>
@@ -13611,31 +13113,11 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="10" t="inlineStr">
-        <is>
-          <t>6.3</t>
-        </is>
-      </c>
-      <c r="C28" s="10" t="inlineStr">
-        <is>
-          <t>User Training</t>
-        </is>
-      </c>
-      <c r="D28" s="11" t="inlineStr">
-        <is>
-          <t>19-Jun-2024</t>
-        </is>
-      </c>
-      <c r="E28" s="11" t="inlineStr">
-        <is>
-          <t>02-Jul-2024</t>
-        </is>
-      </c>
-      <c r="F28" s="11" t="inlineStr">
-        <is>
-          <t>Ongoing</t>
-        </is>
-      </c>
+      <c r="B28" s="6" t="n"/>
+      <c r="C28" s="6" t="n"/>
+      <c r="D28" s="1" t="n"/>
+      <c r="E28" s="1" t="n"/>
+      <c r="F28" s="1" t="n"/>
       <c r="G28" s="1" t="n"/>
       <c r="H28" s="1" t="n"/>
       <c r="I28" s="1" t="n"/>
@@ -17426,7 +16908,7 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="11">
     <mergeCell ref="B5"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
@@ -17434,18 +16916,12 @@
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="B13"/>
-    <mergeCell ref="B17"/>
-    <mergeCell ref="C17"/>
-    <mergeCell ref="B21"/>
-    <mergeCell ref="C21"/>
-    <mergeCell ref="B25"/>
     <mergeCell ref="C13"/>
-    <mergeCell ref="C25"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="C5"/>
     <mergeCell ref="C9"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:F28">
+  <conditionalFormatting sqref="F5:F16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Ongoing"</formula>
     </cfRule>
@@ -17457,7 +16933,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation sqref="F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25 F26 F27 F28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid entry, please select from the list" type="list">
+    <dataValidation sqref="F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid entry, please select from the list" type="list">
       <formula1>"Ongoing,At Risk,Delayed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added Priority and Completeness
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -43,7 +43,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill/>
     </fill>
@@ -70,8 +70,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0032a852"/>
-        <bgColor rgb="0032a852"/>
+        <fgColor rgb="001FD5C4"/>
+        <bgColor rgb="001FD5C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D2DDDC"/>
+        <bgColor rgb="00D2DDDC"/>
       </patternFill>
     </fill>
     <fill>
@@ -117,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -137,15 +143,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -154,7 +166,7 @@
     <dxf>
       <font>
         <b val="1"/>
-        <color rgb="00000000"/>
+        <color rgb="00FFFFFF"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -585,7 +597,7 @@
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
@@ -597,6 +609,7 @@
     <col width="20" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
     <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -621,12 +634,16 @@
           <t>End Date</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="G1" s="4" t="n"/>
       <c r="H1" s="4" t="n"/>
       <c r="I1" s="4" t="n"/>
       <c r="J1" s="4" t="n"/>
@@ -637,7 +654,7 @@
       <c r="O1" s="4" t="n"/>
       <c r="P1" s="4" t="n"/>
       <c r="Q1" s="4" t="n"/>
-      <c r="R1" s="1" t="n"/>
+      <c r="R1" s="4" t="n"/>
       <c r="S1" s="1" t="n"/>
       <c r="T1" s="1" t="n"/>
       <c r="U1" s="1" t="n"/>
@@ -677,31 +694,31 @@
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="4" t="n"/>
       <c r="E2" s="4" t="n"/>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="4" t="n"/>
+      <c r="G2" s="5" t="inlineStr">
         <is>
           <t>April</t>
         </is>
       </c>
-      <c r="G2" s="4" t="n"/>
       <c r="H2" s="4" t="n"/>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="I2" s="4" t="n"/>
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>May</t>
         </is>
       </c>
-      <c r="J2" s="4" t="n"/>
       <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="4" t="n"/>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="N2" s="4" t="n"/>
+      <c r="O2" s="5" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="O2" s="4" t="n"/>
       <c r="P2" s="4" t="n"/>
       <c r="Q2" s="4" t="n"/>
-      <c r="R2" s="1" t="n"/>
+      <c r="R2" s="4" t="n"/>
       <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
       <c r="U2" s="1" t="n"/>
@@ -741,67 +758,67 @@
       <c r="C3" s="4" t="n"/>
       <c r="D3" s="4" t="n"/>
       <c r="E3" s="4" t="n"/>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="5" t="inlineStr">
         <is>
           <t>10/Apr - 16/Apr</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="H3" s="5" t="inlineStr">
         <is>
           <t>17/Apr - 23/Apr</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="I3" s="5" t="inlineStr">
         <is>
           <t>24/Apr - 30/Apr</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="J3" s="5" t="inlineStr">
         <is>
           <t>01/May - 07/May</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="K3" s="5" t="inlineStr">
         <is>
           <t>08/May - 14/May</t>
         </is>
       </c>
-      <c r="K3" s="5" t="inlineStr">
+      <c r="L3" s="5" t="inlineStr">
         <is>
           <t>15/May - 21/May</t>
         </is>
       </c>
-      <c r="L3" s="5" t="inlineStr">
+      <c r="M3" s="5" t="inlineStr">
         <is>
           <t>22/May - 28/May</t>
         </is>
       </c>
-      <c r="M3" s="5" t="inlineStr">
+      <c r="N3" s="5" t="inlineStr">
         <is>
           <t>29/May - 04/Jun</t>
         </is>
       </c>
-      <c r="N3" s="5" t="inlineStr">
+      <c r="O3" s="5" t="inlineStr">
         <is>
           <t>05/Jun - 11/Jun</t>
         </is>
       </c>
-      <c r="O3" s="5" t="inlineStr">
+      <c r="P3" s="5" t="inlineStr">
         <is>
           <t>12/Jun - 18/Jun</t>
         </is>
       </c>
-      <c r="P3" s="5" t="inlineStr">
+      <c r="Q3" s="5" t="inlineStr">
         <is>
           <t>19/Jun - 25/Jun</t>
         </is>
       </c>
-      <c r="Q3" s="5" t="inlineStr">
+      <c r="R3" s="5" t="inlineStr">
         <is>
           <t>26/Jun - 02/Jul</t>
         </is>
       </c>
-      <c r="R3" s="1" t="n"/>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="n"/>
       <c r="U3" s="1" t="n"/>
@@ -909,9 +926,13 @@
           <t>23-Apr-2024</t>
         </is>
       </c>
-      <c r="F5" s="9" t="n"/>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="1" t="n"/>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="n"/>
+      <c r="H5" s="10" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
       <c r="K5" s="1" t="n"/>
@@ -957,28 +978,32 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="11" t="inlineStr">
         <is>
           <t>1.1</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>Initial Meeting</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
+      <c r="D6" s="12" t="inlineStr">
         <is>
           <t>10-Apr-2024</t>
         </is>
       </c>
-      <c r="E6" s="11" t="inlineStr">
+      <c r="E6" s="12" t="inlineStr">
         <is>
           <t>16-Apr-2024</t>
         </is>
       </c>
-      <c r="F6" s="12" t="n"/>
-      <c r="G6" s="1" t="n"/>
+      <c r="F6" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="G6" s="13" t="n"/>
       <c r="H6" s="1" t="n"/>
       <c r="I6" s="1" t="n"/>
       <c r="J6" s="1" t="n"/>
@@ -1025,28 +1050,32 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="10" t="inlineStr">
+      <c r="B7" s="11" t="inlineStr">
         <is>
           <t>1.2</t>
         </is>
       </c>
-      <c r="C7" s="10" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>Stakeholder Interviews</t>
         </is>
       </c>
-      <c r="D7" s="11" t="inlineStr">
+      <c r="D7" s="12" t="inlineStr">
         <is>
           <t>10-Apr-2024</t>
         </is>
       </c>
-      <c r="E7" s="11" t="inlineStr">
+      <c r="E7" s="12" t="inlineStr">
         <is>
           <t>16-Apr-2024</t>
         </is>
       </c>
-      <c r="F7" s="12" t="n"/>
-      <c r="G7" s="1" t="n"/>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="G7" s="13" t="n"/>
       <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n"/>
       <c r="J7" s="1" t="n"/>
@@ -1093,29 +1122,33 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="11" t="inlineStr">
         <is>
           <t>1.3</t>
         </is>
       </c>
-      <c r="C8" s="10" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>Requirements Documentation</t>
         </is>
       </c>
-      <c r="D8" s="11" t="inlineStr">
+      <c r="D8" s="12" t="inlineStr">
         <is>
           <t>10-Apr-2024</t>
         </is>
       </c>
-      <c r="E8" s="11" t="inlineStr">
+      <c r="E8" s="12" t="inlineStr">
         <is>
           <t>23-Apr-2024</t>
         </is>
       </c>
-      <c r="F8" s="12" t="n"/>
-      <c r="G8" s="12" t="n"/>
-      <c r="H8" s="1" t="n"/>
+      <c r="F8" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="G8" s="13" t="n"/>
+      <c r="H8" s="13" t="n"/>
       <c r="I8" s="1" t="n"/>
       <c r="J8" s="1" t="n"/>
       <c r="K8" s="1" t="n"/>
@@ -1181,11 +1214,15 @@
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F9" s="1" t="n"/>
+      <c r="F9" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G9" s="1" t="n"/>
-      <c r="H9" s="9" t="n"/>
-      <c r="I9" s="9" t="n"/>
-      <c r="J9" s="1" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="10" t="n"/>
+      <c r="J9" s="10" t="n"/>
       <c r="K9" s="1" t="n"/>
       <c r="L9" s="1" t="n"/>
       <c r="M9" s="1" t="n"/>
@@ -1229,30 +1266,34 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="11" t="inlineStr">
         <is>
           <t>2.1</t>
         </is>
       </c>
-      <c r="C10" s="10" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>System Architecture Design</t>
         </is>
       </c>
-      <c r="D10" s="11" t="inlineStr">
+      <c r="D10" s="12" t="inlineStr">
         <is>
           <t>24-Apr-2024</t>
         </is>
       </c>
-      <c r="E10" s="11" t="inlineStr">
+      <c r="E10" s="12" t="inlineStr">
         <is>
           <t>30-Apr-2024</t>
         </is>
       </c>
-      <c r="F10" s="1" t="n"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G10" s="1" t="n"/>
-      <c r="H10" s="12" t="n"/>
-      <c r="I10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
+      <c r="I10" s="13" t="n"/>
       <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
       <c r="L10" s="1" t="n"/>
@@ -1297,31 +1338,35 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="10" t="inlineStr">
+      <c r="B11" s="11" t="inlineStr">
         <is>
           <t>2.2</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="11" t="inlineStr">
         <is>
           <t>Database Schema Design</t>
         </is>
       </c>
-      <c r="D11" s="11" t="inlineStr">
+      <c r="D11" s="12" t="inlineStr">
         <is>
           <t>24-Apr-2024</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
+      <c r="E11" s="12" t="inlineStr">
         <is>
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F11" s="1" t="n"/>
+      <c r="F11" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G11" s="1" t="n"/>
-      <c r="H11" s="12" t="n"/>
-      <c r="I11" s="12" t="n"/>
-      <c r="J11" s="1" t="n"/>
+      <c r="H11" s="1" t="n"/>
+      <c r="I11" s="13" t="n"/>
+      <c r="J11" s="13" t="n"/>
       <c r="K11" s="1" t="n"/>
       <c r="L11" s="1" t="n"/>
       <c r="M11" s="1" t="n"/>
@@ -1365,31 +1410,35 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="11" t="inlineStr">
         <is>
           <t>2.3</t>
         </is>
       </c>
-      <c r="C12" s="10" t="inlineStr">
+      <c r="C12" s="11" t="inlineStr">
         <is>
           <t>UI/UX Design</t>
         </is>
       </c>
-      <c r="D12" s="11" t="inlineStr">
+      <c r="D12" s="12" t="inlineStr">
         <is>
           <t>01-May-2024</t>
         </is>
       </c>
-      <c r="E12" s="11" t="inlineStr">
+      <c r="E12" s="12" t="inlineStr">
         <is>
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F12" s="1" t="n"/>
+      <c r="F12" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G12" s="1" t="n"/>
       <c r="H12" s="1" t="n"/>
-      <c r="I12" s="12" t="n"/>
-      <c r="J12" s="1" t="n"/>
+      <c r="I12" s="1" t="n"/>
+      <c r="J12" s="13" t="n"/>
       <c r="K12" s="1" t="n"/>
       <c r="L12" s="1" t="n"/>
       <c r="M12" s="1" t="n"/>
@@ -1453,14 +1502,18 @@
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F13" s="1" t="n"/>
+      <c r="F13" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G13" s="1" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
-      <c r="J13" s="9" t="n"/>
-      <c r="K13" s="9" t="n"/>
-      <c r="L13" s="9" t="n"/>
-      <c r="M13" s="1" t="n"/>
+      <c r="J13" s="1" t="n"/>
+      <c r="K13" s="10" t="n"/>
+      <c r="L13" s="10" t="n"/>
+      <c r="M13" s="10" t="n"/>
       <c r="N13" s="1" t="n"/>
       <c r="O13" s="1" t="n"/>
       <c r="P13" s="1" t="n"/>
@@ -1501,32 +1554,36 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="10" t="inlineStr">
+      <c r="B14" s="11" t="inlineStr">
         <is>
           <t>3.1</t>
         </is>
       </c>
-      <c r="C14" s="10" t="inlineStr">
+      <c r="C14" s="11" t="inlineStr">
         <is>
           <t>Frontend Development</t>
         </is>
       </c>
-      <c r="D14" s="11" t="inlineStr">
+      <c r="D14" s="12" t="inlineStr">
         <is>
           <t>08-May-2024</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="E14" s="12" t="inlineStr">
         <is>
           <t>14-May-2024</t>
         </is>
       </c>
-      <c r="F14" s="1" t="n"/>
+      <c r="F14" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G14" s="1" t="n"/>
       <c r="H14" s="1" t="n"/>
       <c r="I14" s="1" t="n"/>
-      <c r="J14" s="12" t="n"/>
-      <c r="K14" s="1" t="n"/>
+      <c r="J14" s="1" t="n"/>
+      <c r="K14" s="13" t="n"/>
       <c r="L14" s="1" t="n"/>
       <c r="M14" s="1" t="n"/>
       <c r="N14" s="1" t="n"/>
@@ -1569,34 +1626,38 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="10" t="inlineStr">
+      <c r="B15" s="11" t="inlineStr">
         <is>
           <t>3.2</t>
         </is>
       </c>
-      <c r="C15" s="10" t="inlineStr">
+      <c r="C15" s="11" t="inlineStr">
         <is>
           <t>Backend Development</t>
         </is>
       </c>
-      <c r="D15" s="11" t="inlineStr">
+      <c r="D15" s="12" t="inlineStr">
         <is>
           <t>15-May-2024</t>
         </is>
       </c>
-      <c r="E15" s="11" t="inlineStr">
+      <c r="E15" s="12" t="inlineStr">
         <is>
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F15" s="1" t="n"/>
+      <c r="F15" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G15" s="1" t="n"/>
       <c r="H15" s="1" t="n"/>
       <c r="I15" s="1" t="n"/>
       <c r="J15" s="1" t="n"/>
-      <c r="K15" s="12" t="n"/>
-      <c r="L15" s="12" t="n"/>
-      <c r="M15" s="1" t="n"/>
+      <c r="K15" s="1" t="n"/>
+      <c r="L15" s="13" t="n"/>
+      <c r="M15" s="13" t="n"/>
       <c r="N15" s="1" t="n"/>
       <c r="O15" s="1" t="n"/>
       <c r="P15" s="1" t="n"/>
@@ -1637,34 +1698,38 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
-      <c r="B16" s="10" t="inlineStr">
+      <c r="B16" s="11" t="inlineStr">
         <is>
           <t>3.3</t>
         </is>
       </c>
-      <c r="C16" s="10" t="inlineStr">
+      <c r="C16" s="11" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="D16" s="11" t="inlineStr">
+      <c r="D16" s="12" t="inlineStr">
         <is>
           <t>22-May-2024</t>
         </is>
       </c>
-      <c r="E16" s="11" t="inlineStr">
+      <c r="E16" s="12" t="inlineStr">
         <is>
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F16" s="1" t="n"/>
+      <c r="F16" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G16" s="1" t="n"/>
       <c r="H16" s="1" t="n"/>
       <c r="I16" s="1" t="n"/>
       <c r="J16" s="1" t="n"/>
       <c r="K16" s="1" t="n"/>
-      <c r="L16" s="12" t="n"/>
-      <c r="M16" s="1" t="n"/>
+      <c r="L16" s="1" t="n"/>
+      <c r="M16" s="13" t="n"/>
       <c r="N16" s="1" t="n"/>
       <c r="O16" s="1" t="n"/>
       <c r="P16" s="1" t="n"/>
@@ -1725,16 +1790,20 @@
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F17" s="1" t="n"/>
+      <c r="F17" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G17" s="1" t="n"/>
       <c r="H17" s="1" t="n"/>
       <c r="I17" s="1" t="n"/>
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
       <c r="L17" s="1" t="n"/>
-      <c r="M17" s="9" t="n"/>
-      <c r="N17" s="9" t="n"/>
-      <c r="O17" s="1" t="n"/>
+      <c r="M17" s="1" t="n"/>
+      <c r="N17" s="10" t="n"/>
+      <c r="O17" s="10" t="n"/>
       <c r="P17" s="1" t="n"/>
       <c r="Q17" s="1" t="n"/>
       <c r="R17" s="1" t="n"/>
@@ -1773,35 +1842,39 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="10" t="inlineStr">
+      <c r="B18" s="11" t="inlineStr">
         <is>
           <t>4.1</t>
         </is>
       </c>
-      <c r="C18" s="10" t="inlineStr">
+      <c r="C18" s="11" t="inlineStr">
         <is>
           <t>Unit Testing</t>
         </is>
       </c>
-      <c r="D18" s="11" t="inlineStr">
+      <c r="D18" s="12" t="inlineStr">
         <is>
           <t>29-May-2024</t>
         </is>
       </c>
-      <c r="E18" s="11" t="inlineStr">
+      <c r="E18" s="12" t="inlineStr">
         <is>
           <t>04-Jun-2024</t>
         </is>
       </c>
-      <c r="F18" s="1" t="n"/>
+      <c r="F18" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G18" s="1" t="n"/>
       <c r="H18" s="1" t="n"/>
       <c r="I18" s="1" t="n"/>
       <c r="J18" s="1" t="n"/>
       <c r="K18" s="1" t="n"/>
       <c r="L18" s="1" t="n"/>
-      <c r="M18" s="12" t="n"/>
-      <c r="N18" s="1" t="n"/>
+      <c r="M18" s="1" t="n"/>
+      <c r="N18" s="13" t="n"/>
       <c r="O18" s="1" t="n"/>
       <c r="P18" s="1" t="n"/>
       <c r="Q18" s="1" t="n"/>
@@ -1841,36 +1914,40 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="10" t="inlineStr">
+      <c r="B19" s="11" t="inlineStr">
         <is>
           <t>4.2</t>
         </is>
       </c>
-      <c r="C19" s="10" t="inlineStr">
+      <c r="C19" s="11" t="inlineStr">
         <is>
           <t>Integration Testing</t>
         </is>
       </c>
-      <c r="D19" s="11" t="inlineStr">
+      <c r="D19" s="12" t="inlineStr">
         <is>
           <t>29-May-2024</t>
         </is>
       </c>
-      <c r="E19" s="11" t="inlineStr">
+      <c r="E19" s="12" t="inlineStr">
         <is>
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F19" s="1" t="n"/>
+      <c r="F19" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G19" s="1" t="n"/>
       <c r="H19" s="1" t="n"/>
       <c r="I19" s="1" t="n"/>
       <c r="J19" s="1" t="n"/>
       <c r="K19" s="1" t="n"/>
       <c r="L19" s="1" t="n"/>
-      <c r="M19" s="12" t="n"/>
-      <c r="N19" s="12" t="n"/>
-      <c r="O19" s="1" t="n"/>
+      <c r="M19" s="1" t="n"/>
+      <c r="N19" s="13" t="n"/>
+      <c r="O19" s="13" t="n"/>
       <c r="P19" s="1" t="n"/>
       <c r="Q19" s="1" t="n"/>
       <c r="R19" s="1" t="n"/>
@@ -1909,27 +1986,31 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="10" t="inlineStr">
+      <c r="B20" s="11" t="inlineStr">
         <is>
           <t>4.3</t>
         </is>
       </c>
-      <c r="C20" s="10" t="inlineStr">
+      <c r="C20" s="11" t="inlineStr">
         <is>
           <t>User Acceptance Testing</t>
         </is>
       </c>
-      <c r="D20" s="11" t="inlineStr">
+      <c r="D20" s="12" t="inlineStr">
         <is>
           <t>05-Jun-2024</t>
         </is>
       </c>
-      <c r="E20" s="11" t="inlineStr">
+      <c r="E20" s="12" t="inlineStr">
         <is>
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F20" s="1" t="n"/>
+      <c r="F20" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G20" s="1" t="n"/>
       <c r="H20" s="1" t="n"/>
       <c r="I20" s="1" t="n"/>
@@ -1937,8 +2018,8 @@
       <c r="K20" s="1" t="n"/>
       <c r="L20" s="1" t="n"/>
       <c r="M20" s="1" t="n"/>
-      <c r="N20" s="12" t="n"/>
-      <c r="O20" s="1" t="n"/>
+      <c r="N20" s="1" t="n"/>
+      <c r="O20" s="13" t="n"/>
       <c r="P20" s="1" t="n"/>
       <c r="Q20" s="1" t="n"/>
       <c r="R20" s="1" t="n"/>
@@ -1997,7 +2078,11 @@
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F21" s="1" t="n"/>
+      <c r="F21" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
       <c r="I21" s="1" t="n"/>
@@ -2006,8 +2091,8 @@
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n"/>
       <c r="N21" s="1" t="n"/>
-      <c r="O21" s="9" t="n"/>
-      <c r="P21" s="1" t="n"/>
+      <c r="O21" s="1" t="n"/>
+      <c r="P21" s="10" t="n"/>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
       <c r="S21" s="1" t="n"/>
@@ -2045,27 +2130,31 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="10" t="inlineStr">
+      <c r="B22" s="11" t="inlineStr">
         <is>
           <t>5.1</t>
         </is>
       </c>
-      <c r="C22" s="10" t="inlineStr">
+      <c r="C22" s="11" t="inlineStr">
         <is>
           <t>Prepare Deployment Environment</t>
         </is>
       </c>
-      <c r="D22" s="11" t="inlineStr">
+      <c r="D22" s="12" t="inlineStr">
         <is>
           <t>12-Jun-2024</t>
         </is>
       </c>
-      <c r="E22" s="11" t="inlineStr">
+      <c r="E22" s="12" t="inlineStr">
         <is>
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F22" s="1" t="n"/>
+      <c r="F22" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G22" s="1" t="n"/>
       <c r="H22" s="1" t="n"/>
       <c r="I22" s="1" t="n"/>
@@ -2074,8 +2163,8 @@
       <c r="L22" s="1" t="n"/>
       <c r="M22" s="1" t="n"/>
       <c r="N22" s="1" t="n"/>
-      <c r="O22" s="12" t="n"/>
-      <c r="P22" s="1" t="n"/>
+      <c r="O22" s="1" t="n"/>
+      <c r="P22" s="13" t="n"/>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
       <c r="S22" s="1" t="n"/>
@@ -2113,27 +2202,31 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="10" t="inlineStr">
+      <c r="B23" s="11" t="inlineStr">
         <is>
           <t>5.2</t>
         </is>
       </c>
-      <c r="C23" s="10" t="inlineStr">
+      <c r="C23" s="11" t="inlineStr">
         <is>
           <t>Deployment</t>
         </is>
       </c>
-      <c r="D23" s="11" t="inlineStr">
+      <c r="D23" s="12" t="inlineStr">
         <is>
           <t>12-Jun-2024</t>
         </is>
       </c>
-      <c r="E23" s="11" t="inlineStr">
+      <c r="E23" s="12" t="inlineStr">
         <is>
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F23" s="1" t="n"/>
+      <c r="F23" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G23" s="1" t="n"/>
       <c r="H23" s="1" t="n"/>
       <c r="I23" s="1" t="n"/>
@@ -2142,8 +2235,8 @@
       <c r="L23" s="1" t="n"/>
       <c r="M23" s="1" t="n"/>
       <c r="N23" s="1" t="n"/>
-      <c r="O23" s="12" t="n"/>
-      <c r="P23" s="1" t="n"/>
+      <c r="O23" s="1" t="n"/>
+      <c r="P23" s="13" t="n"/>
       <c r="Q23" s="1" t="n"/>
       <c r="R23" s="1" t="n"/>
       <c r="S23" s="1" t="n"/>
@@ -2181,27 +2274,31 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="10" t="inlineStr">
+      <c r="B24" s="11" t="inlineStr">
         <is>
           <t>5.3</t>
         </is>
       </c>
-      <c r="C24" s="10" t="inlineStr">
+      <c r="C24" s="11" t="inlineStr">
         <is>
           <t>Post-Deployment Verification</t>
         </is>
       </c>
-      <c r="D24" s="11" t="inlineStr">
+      <c r="D24" s="12" t="inlineStr">
         <is>
           <t>12-Jun-2024</t>
         </is>
       </c>
-      <c r="E24" s="11" t="inlineStr">
+      <c r="E24" s="12" t="inlineStr">
         <is>
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F24" s="1" t="n"/>
+      <c r="F24" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G24" s="1" t="n"/>
       <c r="H24" s="1" t="n"/>
       <c r="I24" s="1" t="n"/>
@@ -2210,8 +2307,8 @@
       <c r="L24" s="1" t="n"/>
       <c r="M24" s="1" t="n"/>
       <c r="N24" s="1" t="n"/>
-      <c r="O24" s="12" t="n"/>
-      <c r="P24" s="1" t="n"/>
+      <c r="O24" s="1" t="n"/>
+      <c r="P24" s="13" t="n"/>
       <c r="Q24" s="1" t="n"/>
       <c r="R24" s="1" t="n"/>
       <c r="S24" s="1" t="n"/>
@@ -2269,7 +2366,11 @@
           <t>02-Jul-2024</t>
         </is>
       </c>
-      <c r="F25" s="1" t="n"/>
+      <c r="F25" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G25" s="1" t="n"/>
       <c r="H25" s="1" t="n"/>
       <c r="I25" s="1" t="n"/>
@@ -2279,9 +2380,9 @@
       <c r="M25" s="1" t="n"/>
       <c r="N25" s="1" t="n"/>
       <c r="O25" s="1" t="n"/>
-      <c r="P25" s="9" t="n"/>
-      <c r="Q25" s="9" t="n"/>
-      <c r="R25" s="1" t="n"/>
+      <c r="P25" s="1" t="n"/>
+      <c r="Q25" s="10" t="n"/>
+      <c r="R25" s="10" t="n"/>
       <c r="S25" s="1" t="n"/>
       <c r="T25" s="1" t="n"/>
       <c r="U25" s="1" t="n"/>
@@ -2317,27 +2418,31 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="10" t="inlineStr">
+      <c r="B26" s="11" t="inlineStr">
         <is>
           <t>6.1</t>
         </is>
       </c>
-      <c r="C26" s="10" t="inlineStr">
+      <c r="C26" s="11" t="inlineStr">
         <is>
           <t>Bug Fixing</t>
         </is>
       </c>
-      <c r="D26" s="11" t="inlineStr">
+      <c r="D26" s="12" t="inlineStr">
         <is>
           <t>19-Jun-2024</t>
         </is>
       </c>
-      <c r="E26" s="11" t="inlineStr">
+      <c r="E26" s="12" t="inlineStr">
         <is>
           <t>25-Jun-2024</t>
         </is>
       </c>
-      <c r="F26" s="1" t="n"/>
+      <c r="F26" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G26" s="1" t="n"/>
       <c r="H26" s="1" t="n"/>
       <c r="I26" s="1" t="n"/>
@@ -2347,8 +2452,8 @@
       <c r="M26" s="1" t="n"/>
       <c r="N26" s="1" t="n"/>
       <c r="O26" s="1" t="n"/>
-      <c r="P26" s="12" t="n"/>
-      <c r="Q26" s="1" t="n"/>
+      <c r="P26" s="1" t="n"/>
+      <c r="Q26" s="13" t="n"/>
       <c r="R26" s="1" t="n"/>
       <c r="S26" s="1" t="n"/>
       <c r="T26" s="1" t="n"/>
@@ -2385,27 +2490,31 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="10" t="inlineStr">
+      <c r="B27" s="11" t="inlineStr">
         <is>
           <t>6.2</t>
         </is>
       </c>
-      <c r="C27" s="10" t="inlineStr">
+      <c r="C27" s="11" t="inlineStr">
         <is>
           <t>Performance Tuning</t>
         </is>
       </c>
-      <c r="D27" s="11" t="inlineStr">
+      <c r="D27" s="12" t="inlineStr">
         <is>
           <t>19-Jun-2024</t>
         </is>
       </c>
-      <c r="E27" s="11" t="inlineStr">
+      <c r="E27" s="12" t="inlineStr">
         <is>
           <t>25-Jun-2024</t>
         </is>
       </c>
-      <c r="F27" s="1" t="n"/>
+      <c r="F27" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G27" s="1" t="n"/>
       <c r="H27" s="1" t="n"/>
       <c r="I27" s="1" t="n"/>
@@ -2415,8 +2524,8 @@
       <c r="M27" s="1" t="n"/>
       <c r="N27" s="1" t="n"/>
       <c r="O27" s="1" t="n"/>
-      <c r="P27" s="12" t="n"/>
-      <c r="Q27" s="1" t="n"/>
+      <c r="P27" s="1" t="n"/>
+      <c r="Q27" s="13" t="n"/>
       <c r="R27" s="1" t="n"/>
       <c r="S27" s="1" t="n"/>
       <c r="T27" s="1" t="n"/>
@@ -2453,27 +2562,31 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="10" t="inlineStr">
+      <c r="B28" s="11" t="inlineStr">
         <is>
           <t>6.3</t>
         </is>
       </c>
-      <c r="C28" s="10" t="inlineStr">
+      <c r="C28" s="11" t="inlineStr">
         <is>
           <t>User Training</t>
         </is>
       </c>
-      <c r="D28" s="11" t="inlineStr">
+      <c r="D28" s="12" t="inlineStr">
         <is>
           <t>19-Jun-2024</t>
         </is>
       </c>
-      <c r="E28" s="11" t="inlineStr">
+      <c r="E28" s="12" t="inlineStr">
         <is>
           <t>02-Jul-2024</t>
         </is>
       </c>
-      <c r="F28" s="1" t="n"/>
+      <c r="F28" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G28" s="1" t="n"/>
       <c r="H28" s="1" t="n"/>
       <c r="I28" s="1" t="n"/>
@@ -2483,9 +2596,9 @@
       <c r="M28" s="1" t="n"/>
       <c r="N28" s="1" t="n"/>
       <c r="O28" s="1" t="n"/>
-      <c r="P28" s="12" t="n"/>
-      <c r="Q28" s="12" t="n"/>
-      <c r="R28" s="1" t="n"/>
+      <c r="P28" s="1" t="n"/>
+      <c r="Q28" s="13" t="n"/>
+      <c r="R28" s="13" t="n"/>
       <c r="S28" s="1" t="n"/>
       <c r="T28" s="1" t="n"/>
       <c r="U28" s="1" t="n"/>
@@ -6264,28 +6377,45 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
     <mergeCell ref="B9"/>
     <mergeCell ref="C17"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="O2:R2"/>
     <mergeCell ref="B5"/>
     <mergeCell ref="C13"/>
     <mergeCell ref="D1:D3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="B25"/>
     <mergeCell ref="C5"/>
+    <mergeCell ref="G1:R1"/>
     <mergeCell ref="B21"/>
     <mergeCell ref="C25"/>
-    <mergeCell ref="F1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="C9"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="B17"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="B13"/>
     <mergeCell ref="C21"/>
+    <mergeCell ref="J2:N2"/>
   </mergeCells>
+  <conditionalFormatting sqref="F5:F28">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>"Low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>"High"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation sqref="F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25 F26 F27 F28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid entry, please select from the list" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -6308,7 +6438,7 @@
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
@@ -6320,6 +6450,7 @@
     <col width="20" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
     <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6344,12 +6475,16 @@
           <t>End Date</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="G1" s="4" t="n"/>
       <c r="H1" s="4" t="n"/>
       <c r="I1" s="4" t="n"/>
       <c r="J1" s="4" t="n"/>
@@ -6360,7 +6495,7 @@
       <c r="O1" s="4" t="n"/>
       <c r="P1" s="4" t="n"/>
       <c r="Q1" s="4" t="n"/>
-      <c r="R1" s="1" t="n"/>
+      <c r="R1" s="4" t="n"/>
       <c r="S1" s="1" t="n"/>
       <c r="T1" s="1" t="n"/>
       <c r="U1" s="1" t="n"/>
@@ -6400,31 +6535,31 @@
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="4" t="n"/>
       <c r="E2" s="4" t="n"/>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="4" t="n"/>
+      <c r="G2" s="5" t="inlineStr">
         <is>
           <t>April</t>
         </is>
       </c>
-      <c r="G2" s="4" t="n"/>
       <c r="H2" s="4" t="n"/>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="I2" s="4" t="n"/>
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>May</t>
         </is>
       </c>
-      <c r="J2" s="4" t="n"/>
       <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="4" t="n"/>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="N2" s="4" t="n"/>
+      <c r="O2" s="5" t="inlineStr">
         <is>
           <t>June</t>
         </is>
       </c>
-      <c r="O2" s="4" t="n"/>
       <c r="P2" s="4" t="n"/>
       <c r="Q2" s="4" t="n"/>
-      <c r="R2" s="1" t="n"/>
+      <c r="R2" s="4" t="n"/>
       <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
       <c r="U2" s="1" t="n"/>
@@ -6464,67 +6599,67 @@
       <c r="C3" s="4" t="n"/>
       <c r="D3" s="4" t="n"/>
       <c r="E3" s="4" t="n"/>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="5" t="inlineStr">
         <is>
           <t>10/Apr - 16/Apr</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="H3" s="5" t="inlineStr">
         <is>
           <t>17/Apr - 23/Apr</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="I3" s="5" t="inlineStr">
         <is>
           <t>24/Apr - 30/Apr</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="J3" s="5" t="inlineStr">
         <is>
           <t>01/May - 07/May</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="K3" s="5" t="inlineStr">
         <is>
           <t>08/May - 14/May</t>
         </is>
       </c>
-      <c r="K3" s="5" t="inlineStr">
+      <c r="L3" s="5" t="inlineStr">
         <is>
           <t>15/May - 21/May</t>
         </is>
       </c>
-      <c r="L3" s="5" t="inlineStr">
+      <c r="M3" s="5" t="inlineStr">
         <is>
           <t>22/May - 28/May</t>
         </is>
       </c>
-      <c r="M3" s="5" t="inlineStr">
+      <c r="N3" s="5" t="inlineStr">
         <is>
           <t>29/May - 04/Jun</t>
         </is>
       </c>
-      <c r="N3" s="5" t="inlineStr">
+      <c r="O3" s="5" t="inlineStr">
         <is>
           <t>05/Jun - 11/Jun</t>
         </is>
       </c>
-      <c r="O3" s="5" t="inlineStr">
+      <c r="P3" s="5" t="inlineStr">
         <is>
           <t>12/Jun - 18/Jun</t>
         </is>
       </c>
-      <c r="P3" s="5" t="inlineStr">
+      <c r="Q3" s="5" t="inlineStr">
         <is>
           <t>19/Jun - 25/Jun</t>
         </is>
       </c>
-      <c r="Q3" s="5" t="inlineStr">
+      <c r="R3" s="5" t="inlineStr">
         <is>
           <t>26/Jun - 02/Jul</t>
         </is>
       </c>
-      <c r="R3" s="1" t="n"/>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="n"/>
       <c r="U3" s="1" t="n"/>
@@ -6632,9 +6767,13 @@
           <t>23-Apr-2024</t>
         </is>
       </c>
-      <c r="F5" s="9" t="n"/>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="1" t="n"/>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="n"/>
+      <c r="H5" s="10" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
       <c r="K5" s="1" t="n"/>
@@ -6856,11 +6995,15 @@
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F9" s="1" t="n"/>
+      <c r="F9" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G9" s="1" t="n"/>
-      <c r="H9" s="9" t="n"/>
-      <c r="I9" s="9" t="n"/>
-      <c r="J9" s="1" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="10" t="n"/>
+      <c r="J9" s="10" t="n"/>
       <c r="K9" s="1" t="n"/>
       <c r="L9" s="1" t="n"/>
       <c r="M9" s="1" t="n"/>
@@ -7080,14 +7223,18 @@
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F13" s="1" t="n"/>
+      <c r="F13" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G13" s="1" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
-      <c r="J13" s="9" t="n"/>
-      <c r="K13" s="9" t="n"/>
-      <c r="L13" s="9" t="n"/>
-      <c r="M13" s="1" t="n"/>
+      <c r="J13" s="1" t="n"/>
+      <c r="K13" s="10" t="n"/>
+      <c r="L13" s="10" t="n"/>
+      <c r="M13" s="10" t="n"/>
       <c r="N13" s="1" t="n"/>
       <c r="O13" s="1" t="n"/>
       <c r="P13" s="1" t="n"/>
@@ -7304,16 +7451,20 @@
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F17" s="1" t="n"/>
+      <c r="F17" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G17" s="1" t="n"/>
       <c r="H17" s="1" t="n"/>
       <c r="I17" s="1" t="n"/>
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
       <c r="L17" s="1" t="n"/>
-      <c r="M17" s="9" t="n"/>
-      <c r="N17" s="9" t="n"/>
-      <c r="O17" s="1" t="n"/>
+      <c r="M17" s="1" t="n"/>
+      <c r="N17" s="10" t="n"/>
+      <c r="O17" s="10" t="n"/>
       <c r="P17" s="1" t="n"/>
       <c r="Q17" s="1" t="n"/>
       <c r="R17" s="1" t="n"/>
@@ -7528,7 +7679,11 @@
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F21" s="1" t="n"/>
+      <c r="F21" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
       <c r="I21" s="1" t="n"/>
@@ -7537,8 +7692,8 @@
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n"/>
       <c r="N21" s="1" t="n"/>
-      <c r="O21" s="9" t="n"/>
-      <c r="P21" s="1" t="n"/>
+      <c r="O21" s="1" t="n"/>
+      <c r="P21" s="10" t="n"/>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
       <c r="S21" s="1" t="n"/>
@@ -7752,7 +7907,11 @@
           <t>02-Jul-2024</t>
         </is>
       </c>
-      <c r="F25" s="1" t="n"/>
+      <c r="F25" s="9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
       <c r="G25" s="1" t="n"/>
       <c r="H25" s="1" t="n"/>
       <c r="I25" s="1" t="n"/>
@@ -7762,9 +7921,9 @@
       <c r="M25" s="1" t="n"/>
       <c r="N25" s="1" t="n"/>
       <c r="O25" s="1" t="n"/>
-      <c r="P25" s="9" t="n"/>
-      <c r="Q25" s="9" t="n"/>
-      <c r="R25" s="1" t="n"/>
+      <c r="P25" s="1" t="n"/>
+      <c r="Q25" s="10" t="n"/>
+      <c r="R25" s="10" t="n"/>
       <c r="S25" s="1" t="n"/>
       <c r="T25" s="1" t="n"/>
       <c r="U25" s="1" t="n"/>
@@ -11699,28 +11858,45 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
     <mergeCell ref="B9"/>
     <mergeCell ref="C17"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="O2:R2"/>
     <mergeCell ref="B5"/>
     <mergeCell ref="C13"/>
     <mergeCell ref="D1:D3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="B25"/>
     <mergeCell ref="C5"/>
+    <mergeCell ref="G1:R1"/>
     <mergeCell ref="B21"/>
     <mergeCell ref="C25"/>
-    <mergeCell ref="F1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="C9"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="B17"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="B13"/>
     <mergeCell ref="C21"/>
+    <mergeCell ref="J2:N2"/>
   </mergeCells>
+  <conditionalFormatting sqref="F5:F28">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>"Low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>"High"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation sqref="F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25 F26 F27 F28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid entry, please select from the list" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -11743,7 +11919,7 @@
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
@@ -11755,6 +11931,7 @@
     <col width="20" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
     <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -11784,7 +11961,11 @@
           <t>Status</t>
         </is>
       </c>
-      <c r="G1" s="1" t="n"/>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="n"/>
@@ -11836,7 +12017,7 @@
       <c r="D2" s="4" t="n"/>
       <c r="E2" s="4" t="n"/>
       <c r="F2" s="4" t="n"/>
-      <c r="G2" s="1" t="n"/>
+      <c r="G2" s="4" t="n"/>
       <c r="H2" s="1" t="n"/>
       <c r="I2" s="1" t="n"/>
       <c r="J2" s="1" t="n"/>
@@ -11888,7 +12069,7 @@
       <c r="D3" s="4" t="n"/>
       <c r="E3" s="4" t="n"/>
       <c r="F3" s="4" t="n"/>
-      <c r="G3" s="1" t="n"/>
+      <c r="G3" s="4" t="n"/>
       <c r="H3" s="1" t="n"/>
       <c r="I3" s="1" t="n"/>
       <c r="J3" s="1" t="n"/>
@@ -12007,12 +12188,16 @@
           <t>23-Apr-2024</t>
         </is>
       </c>
-      <c r="F5" s="13" t="inlineStr">
+      <c r="F5" s="14" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
       </c>
-      <c r="G5" s="1" t="n"/>
+      <c r="G5" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H5" s="1" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
@@ -12059,32 +12244,36 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="11" t="inlineStr">
         <is>
           <t>1.1</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>Initial Meeting</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
+      <c r="D6" s="12" t="inlineStr">
         <is>
           <t>10-Apr-2024</t>
         </is>
       </c>
-      <c r="E6" s="11" t="inlineStr">
+      <c r="E6" s="12" t="inlineStr">
         <is>
           <t>16-Apr-2024</t>
         </is>
       </c>
-      <c r="F6" s="11" t="inlineStr">
+      <c r="F6" s="12" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
       </c>
-      <c r="G6" s="1" t="n"/>
+      <c r="G6" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H6" s="1" t="n"/>
       <c r="I6" s="1" t="n"/>
       <c r="J6" s="1" t="n"/>
@@ -12131,32 +12320,36 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="10" t="inlineStr">
+      <c r="B7" s="11" t="inlineStr">
         <is>
           <t>1.2</t>
         </is>
       </c>
-      <c r="C7" s="10" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>Stakeholder Interviews</t>
         </is>
       </c>
-      <c r="D7" s="11" t="inlineStr">
+      <c r="D7" s="12" t="inlineStr">
         <is>
           <t>10-Apr-2024</t>
         </is>
       </c>
-      <c r="E7" s="11" t="inlineStr">
+      <c r="E7" s="12" t="inlineStr">
         <is>
           <t>16-Apr-2024</t>
         </is>
       </c>
-      <c r="F7" s="11" t="inlineStr">
+      <c r="F7" s="12" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
       </c>
-      <c r="G7" s="1" t="n"/>
+      <c r="G7" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n"/>
       <c r="J7" s="1" t="n"/>
@@ -12203,32 +12396,36 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="11" t="inlineStr">
         <is>
           <t>1.3</t>
         </is>
       </c>
-      <c r="C8" s="10" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>Requirements Documentation</t>
         </is>
       </c>
-      <c r="D8" s="11" t="inlineStr">
+      <c r="D8" s="12" t="inlineStr">
         <is>
           <t>10-Apr-2024</t>
         </is>
       </c>
-      <c r="E8" s="11" t="inlineStr">
+      <c r="E8" s="12" t="inlineStr">
         <is>
           <t>23-Apr-2024</t>
         </is>
       </c>
-      <c r="F8" s="11" t="inlineStr">
+      <c r="F8" s="12" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
       </c>
-      <c r="G8" s="1" t="n"/>
+      <c r="G8" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H8" s="1" t="n"/>
       <c r="I8" s="1" t="n"/>
       <c r="J8" s="1" t="n"/>
@@ -12295,12 +12492,16 @@
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F9" s="13" t="inlineStr">
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
       </c>
-      <c r="G9" s="1" t="n"/>
+      <c r="G9" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H9" s="1" t="n"/>
       <c r="I9" s="1" t="n"/>
       <c r="J9" s="1" t="n"/>
@@ -12347,32 +12548,36 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="11" t="inlineStr">
         <is>
           <t>2.1</t>
         </is>
       </c>
-      <c r="C10" s="10" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>System Architecture Design</t>
         </is>
       </c>
-      <c r="D10" s="11" t="inlineStr">
+      <c r="D10" s="12" t="inlineStr">
         <is>
           <t>24-Apr-2024</t>
         </is>
       </c>
-      <c r="E10" s="11" t="inlineStr">
+      <c r="E10" s="12" t="inlineStr">
         <is>
           <t>30-Apr-2024</t>
         </is>
       </c>
-      <c r="F10" s="11" t="inlineStr">
+      <c r="F10" s="12" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
       </c>
-      <c r="G10" s="1" t="n"/>
+      <c r="G10" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H10" s="1" t="n"/>
       <c r="I10" s="1" t="n"/>
       <c r="J10" s="1" t="n"/>
@@ -12419,32 +12624,36 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="10" t="inlineStr">
+      <c r="B11" s="11" t="inlineStr">
         <is>
           <t>2.2</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="11" t="inlineStr">
         <is>
           <t>Database Schema Design</t>
         </is>
       </c>
-      <c r="D11" s="11" t="inlineStr">
+      <c r="D11" s="12" t="inlineStr">
         <is>
           <t>24-Apr-2024</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
+      <c r="E11" s="12" t="inlineStr">
         <is>
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F11" s="11" t="inlineStr">
+      <c r="F11" s="12" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
       </c>
-      <c r="G11" s="1" t="n"/>
+      <c r="G11" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H11" s="1" t="n"/>
       <c r="I11" s="1" t="n"/>
       <c r="J11" s="1" t="n"/>
@@ -12491,32 +12700,36 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="11" t="inlineStr">
         <is>
           <t>2.3</t>
         </is>
       </c>
-      <c r="C12" s="10" t="inlineStr">
+      <c r="C12" s="11" t="inlineStr">
         <is>
           <t>UI/UX Design</t>
         </is>
       </c>
-      <c r="D12" s="11" t="inlineStr">
+      <c r="D12" s="12" t="inlineStr">
         <is>
           <t>01-May-2024</t>
         </is>
       </c>
-      <c r="E12" s="11" t="inlineStr">
+      <c r="E12" s="12" t="inlineStr">
         <is>
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F12" s="11" t="inlineStr">
+      <c r="F12" s="12" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
       </c>
-      <c r="G12" s="1" t="n"/>
+      <c r="G12" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H12" s="1" t="n"/>
       <c r="I12" s="1" t="n"/>
       <c r="J12" s="1" t="n"/>
@@ -12583,12 +12796,16 @@
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F13" s="14" t="inlineStr">
+      <c r="F13" s="16" t="inlineStr">
         <is>
           <t>At Risk</t>
         </is>
       </c>
-      <c r="G13" s="1" t="n"/>
+      <c r="G13" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
       <c r="J13" s="1" t="n"/>
@@ -12635,32 +12852,36 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="10" t="inlineStr">
+      <c r="B14" s="11" t="inlineStr">
         <is>
           <t>3.1</t>
         </is>
       </c>
-      <c r="C14" s="10" t="inlineStr">
+      <c r="C14" s="11" t="inlineStr">
         <is>
           <t>Frontend Development</t>
         </is>
       </c>
-      <c r="D14" s="11" t="inlineStr">
+      <c r="D14" s="12" t="inlineStr">
         <is>
           <t>08-May-2024</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="E14" s="12" t="inlineStr">
         <is>
           <t>14-May-2024</t>
         </is>
       </c>
-      <c r="F14" s="11" t="inlineStr">
+      <c r="F14" s="12" t="inlineStr">
         <is>
           <t>Delayed</t>
         </is>
       </c>
-      <c r="G14" s="1" t="n"/>
+      <c r="G14" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H14" s="1" t="n"/>
       <c r="I14" s="1" t="n"/>
       <c r="J14" s="1" t="n"/>
@@ -12707,32 +12928,36 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="10" t="inlineStr">
+      <c r="B15" s="11" t="inlineStr">
         <is>
           <t>3.2</t>
         </is>
       </c>
-      <c r="C15" s="10" t="inlineStr">
+      <c r="C15" s="11" t="inlineStr">
         <is>
           <t>Backend Development</t>
         </is>
       </c>
-      <c r="D15" s="11" t="inlineStr">
+      <c r="D15" s="12" t="inlineStr">
         <is>
           <t>15-May-2024</t>
         </is>
       </c>
-      <c r="E15" s="11" t="inlineStr">
+      <c r="E15" s="12" t="inlineStr">
         <is>
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F15" s="11" t="inlineStr">
+      <c r="F15" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G15" s="1" t="n"/>
+      <c r="G15" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H15" s="1" t="n"/>
       <c r="I15" s="1" t="n"/>
       <c r="J15" s="1" t="n"/>
@@ -12779,32 +13004,36 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
-      <c r="B16" s="10" t="inlineStr">
+      <c r="B16" s="11" t="inlineStr">
         <is>
           <t>3.3</t>
         </is>
       </c>
-      <c r="C16" s="10" t="inlineStr">
+      <c r="C16" s="11" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="D16" s="11" t="inlineStr">
+      <c r="D16" s="12" t="inlineStr">
         <is>
           <t>22-May-2024</t>
         </is>
       </c>
-      <c r="E16" s="11" t="inlineStr">
+      <c r="E16" s="12" t="inlineStr">
         <is>
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F16" s="11" t="inlineStr">
+      <c r="F16" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G16" s="1" t="n"/>
+      <c r="G16" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H16" s="1" t="n"/>
       <c r="I16" s="1" t="n"/>
       <c r="J16" s="1" t="n"/>
@@ -12871,12 +13100,16 @@
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F17" s="15" t="inlineStr">
+      <c r="F17" s="17" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G17" s="1" t="n"/>
+      <c r="G17" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H17" s="1" t="n"/>
       <c r="I17" s="1" t="n"/>
       <c r="J17" s="1" t="n"/>
@@ -12923,32 +13156,36 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="10" t="inlineStr">
+      <c r="B18" s="11" t="inlineStr">
         <is>
           <t>4.1</t>
         </is>
       </c>
-      <c r="C18" s="10" t="inlineStr">
+      <c r="C18" s="11" t="inlineStr">
         <is>
           <t>Unit Testing</t>
         </is>
       </c>
-      <c r="D18" s="11" t="inlineStr">
+      <c r="D18" s="12" t="inlineStr">
         <is>
           <t>29-May-2024</t>
         </is>
       </c>
-      <c r="E18" s="11" t="inlineStr">
+      <c r="E18" s="12" t="inlineStr">
         <is>
           <t>04-Jun-2024</t>
         </is>
       </c>
-      <c r="F18" s="11" t="inlineStr">
+      <c r="F18" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G18" s="1" t="n"/>
+      <c r="G18" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H18" s="1" t="n"/>
       <c r="I18" s="1" t="n"/>
       <c r="J18" s="1" t="n"/>
@@ -12995,32 +13232,36 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="10" t="inlineStr">
+      <c r="B19" s="11" t="inlineStr">
         <is>
           <t>4.2</t>
         </is>
       </c>
-      <c r="C19" s="10" t="inlineStr">
+      <c r="C19" s="11" t="inlineStr">
         <is>
           <t>Integration Testing</t>
         </is>
       </c>
-      <c r="D19" s="11" t="inlineStr">
+      <c r="D19" s="12" t="inlineStr">
         <is>
           <t>29-May-2024</t>
         </is>
       </c>
-      <c r="E19" s="11" t="inlineStr">
+      <c r="E19" s="12" t="inlineStr">
         <is>
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F19" s="11" t="inlineStr">
+      <c r="F19" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G19" s="1" t="n"/>
+      <c r="G19" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H19" s="1" t="n"/>
       <c r="I19" s="1" t="n"/>
       <c r="J19" s="1" t="n"/>
@@ -13067,32 +13308,36 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="10" t="inlineStr">
+      <c r="B20" s="11" t="inlineStr">
         <is>
           <t>4.3</t>
         </is>
       </c>
-      <c r="C20" s="10" t="inlineStr">
+      <c r="C20" s="11" t="inlineStr">
         <is>
           <t>User Acceptance Testing</t>
         </is>
       </c>
-      <c r="D20" s="11" t="inlineStr">
+      <c r="D20" s="12" t="inlineStr">
         <is>
           <t>05-Jun-2024</t>
         </is>
       </c>
-      <c r="E20" s="11" t="inlineStr">
+      <c r="E20" s="12" t="inlineStr">
         <is>
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F20" s="11" t="inlineStr">
+      <c r="F20" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G20" s="1" t="n"/>
+      <c r="G20" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H20" s="1" t="n"/>
       <c r="I20" s="1" t="n"/>
       <c r="J20" s="1" t="n"/>
@@ -13159,12 +13404,16 @@
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F21" s="15" t="inlineStr">
+      <c r="F21" s="17" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G21" s="1" t="n"/>
+      <c r="G21" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H21" s="1" t="n"/>
       <c r="I21" s="1" t="n"/>
       <c r="J21" s="1" t="n"/>
@@ -13211,32 +13460,36 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="10" t="inlineStr">
+      <c r="B22" s="11" t="inlineStr">
         <is>
           <t>5.1</t>
         </is>
       </c>
-      <c r="C22" s="10" t="inlineStr">
+      <c r="C22" s="11" t="inlineStr">
         <is>
           <t>Prepare Deployment Environment</t>
         </is>
       </c>
-      <c r="D22" s="11" t="inlineStr">
+      <c r="D22" s="12" t="inlineStr">
         <is>
           <t>12-Jun-2024</t>
         </is>
       </c>
-      <c r="E22" s="11" t="inlineStr">
+      <c r="E22" s="12" t="inlineStr">
         <is>
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F22" s="11" t="inlineStr">
+      <c r="F22" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G22" s="1" t="n"/>
+      <c r="G22" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H22" s="1" t="n"/>
       <c r="I22" s="1" t="n"/>
       <c r="J22" s="1" t="n"/>
@@ -13283,32 +13536,36 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="10" t="inlineStr">
+      <c r="B23" s="11" t="inlineStr">
         <is>
           <t>5.2</t>
         </is>
       </c>
-      <c r="C23" s="10" t="inlineStr">
+      <c r="C23" s="11" t="inlineStr">
         <is>
           <t>Deployment</t>
         </is>
       </c>
-      <c r="D23" s="11" t="inlineStr">
+      <c r="D23" s="12" t="inlineStr">
         <is>
           <t>12-Jun-2024</t>
         </is>
       </c>
-      <c r="E23" s="11" t="inlineStr">
+      <c r="E23" s="12" t="inlineStr">
         <is>
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F23" s="11" t="inlineStr">
+      <c r="F23" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G23" s="1" t="n"/>
+      <c r="G23" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H23" s="1" t="n"/>
       <c r="I23" s="1" t="n"/>
       <c r="J23" s="1" t="n"/>
@@ -13355,32 +13612,36 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="10" t="inlineStr">
+      <c r="B24" s="11" t="inlineStr">
         <is>
           <t>5.3</t>
         </is>
       </c>
-      <c r="C24" s="10" t="inlineStr">
+      <c r="C24" s="11" t="inlineStr">
         <is>
           <t>Post-Deployment Verification</t>
         </is>
       </c>
-      <c r="D24" s="11" t="inlineStr">
+      <c r="D24" s="12" t="inlineStr">
         <is>
           <t>12-Jun-2024</t>
         </is>
       </c>
-      <c r="E24" s="11" t="inlineStr">
+      <c r="E24" s="12" t="inlineStr">
         <is>
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F24" s="11" t="inlineStr">
+      <c r="F24" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G24" s="1" t="n"/>
+      <c r="G24" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H24" s="1" t="n"/>
       <c r="I24" s="1" t="n"/>
       <c r="J24" s="1" t="n"/>
@@ -13447,12 +13708,16 @@
           <t>02-Jul-2024</t>
         </is>
       </c>
-      <c r="F25" s="15" t="inlineStr">
+      <c r="F25" s="17" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G25" s="1" t="n"/>
+      <c r="G25" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H25" s="1" t="n"/>
       <c r="I25" s="1" t="n"/>
       <c r="J25" s="1" t="n"/>
@@ -13499,32 +13764,36 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="10" t="inlineStr">
+      <c r="B26" s="11" t="inlineStr">
         <is>
           <t>6.1</t>
         </is>
       </c>
-      <c r="C26" s="10" t="inlineStr">
+      <c r="C26" s="11" t="inlineStr">
         <is>
           <t>Bug Fixing</t>
         </is>
       </c>
-      <c r="D26" s="11" t="inlineStr">
+      <c r="D26" s="12" t="inlineStr">
         <is>
           <t>19-Jun-2024</t>
         </is>
       </c>
-      <c r="E26" s="11" t="inlineStr">
+      <c r="E26" s="12" t="inlineStr">
         <is>
           <t>25-Jun-2024</t>
         </is>
       </c>
-      <c r="F26" s="11" t="inlineStr">
+      <c r="F26" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G26" s="1" t="n"/>
+      <c r="G26" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H26" s="1" t="n"/>
       <c r="I26" s="1" t="n"/>
       <c r="J26" s="1" t="n"/>
@@ -13571,32 +13840,36 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="10" t="inlineStr">
+      <c r="B27" s="11" t="inlineStr">
         <is>
           <t>6.2</t>
         </is>
       </c>
-      <c r="C27" s="10" t="inlineStr">
+      <c r="C27" s="11" t="inlineStr">
         <is>
           <t>Performance Tuning</t>
         </is>
       </c>
-      <c r="D27" s="11" t="inlineStr">
+      <c r="D27" s="12" t="inlineStr">
         <is>
           <t>19-Jun-2024</t>
         </is>
       </c>
-      <c r="E27" s="11" t="inlineStr">
+      <c r="E27" s="12" t="inlineStr">
         <is>
           <t>25-Jun-2024</t>
         </is>
       </c>
-      <c r="F27" s="11" t="inlineStr">
+      <c r="F27" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G27" s="1" t="n"/>
+      <c r="G27" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H27" s="1" t="n"/>
       <c r="I27" s="1" t="n"/>
       <c r="J27" s="1" t="n"/>
@@ -13643,32 +13916,36 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="10" t="inlineStr">
+      <c r="B28" s="11" t="inlineStr">
         <is>
           <t>6.3</t>
         </is>
       </c>
-      <c r="C28" s="10" t="inlineStr">
+      <c r="C28" s="11" t="inlineStr">
         <is>
           <t>User Training</t>
         </is>
       </c>
-      <c r="D28" s="11" t="inlineStr">
+      <c r="D28" s="12" t="inlineStr">
         <is>
           <t>19-Jun-2024</t>
         </is>
       </c>
-      <c r="E28" s="11" t="inlineStr">
+      <c r="E28" s="12" t="inlineStr">
         <is>
           <t>02-Jul-2024</t>
         </is>
       </c>
-      <c r="F28" s="11" t="inlineStr">
+      <c r="F28" s="12" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="G28" s="1" t="n"/>
+      <c r="G28" s="15" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
       <c r="H28" s="1" t="n"/>
       <c r="I28" s="1" t="n"/>
       <c r="J28" s="1" t="n"/>
@@ -17458,13 +17735,14 @@
       <c r="AX100" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
     <mergeCell ref="B5"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B9"/>
+    <mergeCell ref="G1:G3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="C1:C3"/>
+    <mergeCell ref="B9"/>
     <mergeCell ref="B13"/>
     <mergeCell ref="B17"/>
     <mergeCell ref="C17"/>
@@ -17477,18 +17755,33 @@
     <mergeCell ref="C5"/>
     <mergeCell ref="C9"/>
   </mergeCells>
+  <conditionalFormatting sqref="G5:G28">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="percentile" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="100"/>
+        <color rgb="00D2DDDC"/>
+        <color rgb="0065DBCE"/>
+        <color rgb="0002FCE0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F5:F28">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="0">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1">
       <formula>"At Risk"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="2">
       <formula>"Delayed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation sqref="G5 G6 G7 G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25 G26 G27 G28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid entry, please select from the list" type="list">
+      <formula1>"0%,10%,20%,25%,30%,40%,50%,60%,70%,75%,80%,90%,100%"</formula1>
+    </dataValidation>
     <dataValidation sqref="F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25 F26 F27 F28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid entry, please select from the list" type="list">
       <formula1>"Ongoing,At Risk,Delayed"</formula1>
     </dataValidation>
@@ -17515,7 +17808,7 @@
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
@@ -17527,6 +17820,7 @@
     <col width="20" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
     <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -17811,47 +18105,47 @@
           <t>23-Apr-2024</t>
         </is>
       </c>
-      <c r="F5" s="11" t="inlineStr">
+      <c r="F5" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G5" s="11" t="inlineStr">
+      <c r="G5" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H5" s="11" t="inlineStr">
+      <c r="H5" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I5" s="11" t="inlineStr">
+      <c r="I5" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J5" s="11" t="inlineStr">
+      <c r="J5" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K5" s="11" t="inlineStr">
+      <c r="K5" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L5" s="11" t="inlineStr">
+      <c r="L5" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M5" s="11" t="inlineStr">
+      <c r="M5" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N5" s="11" t="inlineStr">
+      <c r="N5" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -17895,67 +18189,67 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="11" t="inlineStr">
         <is>
           <t>1.1</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>Initial Meeting</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
+      <c r="D6" s="12" t="inlineStr">
         <is>
           <t>10-Apr-2024</t>
         </is>
       </c>
-      <c r="E6" s="11" t="inlineStr">
+      <c r="E6" s="12" t="inlineStr">
         <is>
           <t>16-Apr-2024</t>
         </is>
       </c>
-      <c r="F6" s="11" t="inlineStr">
+      <c r="F6" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G6" s="11" t="inlineStr">
+      <c r="G6" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H6" s="11" t="inlineStr">
+      <c r="H6" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I6" s="11" t="inlineStr">
+      <c r="I6" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J6" s="11" t="inlineStr">
+      <c r="J6" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K6" s="11" t="inlineStr">
+      <c r="K6" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L6" s="11" t="inlineStr">
+      <c r="L6" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M6" s="11" t="inlineStr">
+      <c r="M6" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N6" s="11" t="inlineStr">
+      <c r="N6" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -17999,67 +18293,67 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="10" t="inlineStr">
+      <c r="B7" s="11" t="inlineStr">
         <is>
           <t>1.2</t>
         </is>
       </c>
-      <c r="C7" s="10" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>Stakeholder Interviews</t>
         </is>
       </c>
-      <c r="D7" s="11" t="inlineStr">
+      <c r="D7" s="12" t="inlineStr">
         <is>
           <t>10-Apr-2024</t>
         </is>
       </c>
-      <c r="E7" s="11" t="inlineStr">
+      <c r="E7" s="12" t="inlineStr">
         <is>
           <t>16-Apr-2024</t>
         </is>
       </c>
-      <c r="F7" s="11" t="inlineStr">
+      <c r="F7" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G7" s="11" t="inlineStr">
+      <c r="G7" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H7" s="11" t="inlineStr">
+      <c r="H7" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I7" s="11" t="inlineStr">
+      <c r="I7" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J7" s="11" t="inlineStr">
+      <c r="J7" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K7" s="11" t="inlineStr">
+      <c r="K7" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L7" s="11" t="inlineStr">
+      <c r="L7" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M7" s="11" t="inlineStr">
+      <c r="M7" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N7" s="11" t="inlineStr">
+      <c r="N7" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -18103,67 +18397,67 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="11" t="inlineStr">
         <is>
           <t>1.3</t>
         </is>
       </c>
-      <c r="C8" s="10" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>Requirements Documentation</t>
         </is>
       </c>
-      <c r="D8" s="11" t="inlineStr">
+      <c r="D8" s="12" t="inlineStr">
         <is>
           <t>10-Apr-2024</t>
         </is>
       </c>
-      <c r="E8" s="11" t="inlineStr">
+      <c r="E8" s="12" t="inlineStr">
         <is>
           <t>23-Apr-2024</t>
         </is>
       </c>
-      <c r="F8" s="11" t="inlineStr">
+      <c r="F8" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G8" s="11" t="inlineStr">
+      <c r="G8" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H8" s="11" t="inlineStr">
+      <c r="H8" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I8" s="11" t="inlineStr">
+      <c r="I8" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J8" s="11" t="inlineStr">
+      <c r="J8" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K8" s="11" t="inlineStr">
+      <c r="K8" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L8" s="11" t="inlineStr">
+      <c r="L8" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M8" s="11" t="inlineStr">
+      <c r="M8" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N8" s="11" t="inlineStr">
+      <c r="N8" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -18227,47 +18521,47 @@
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F9" s="11" t="inlineStr">
+      <c r="F9" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G9" s="11" t="inlineStr">
+      <c r="G9" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H9" s="11" t="inlineStr">
+      <c r="H9" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I9" s="11" t="inlineStr">
+      <c r="I9" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J9" s="11" t="inlineStr">
+      <c r="J9" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K9" s="11" t="inlineStr">
+      <c r="K9" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L9" s="11" t="inlineStr">
+      <c r="L9" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M9" s="11" t="inlineStr">
+      <c r="M9" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N9" s="11" t="inlineStr">
+      <c r="N9" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -18311,67 +18605,67 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="11" t="inlineStr">
         <is>
           <t>2.1</t>
         </is>
       </c>
-      <c r="C10" s="10" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>System Architecture Design</t>
         </is>
       </c>
-      <c r="D10" s="11" t="inlineStr">
+      <c r="D10" s="12" t="inlineStr">
         <is>
           <t>24-Apr-2024</t>
         </is>
       </c>
-      <c r="E10" s="11" t="inlineStr">
+      <c r="E10" s="12" t="inlineStr">
         <is>
           <t>30-Apr-2024</t>
         </is>
       </c>
-      <c r="F10" s="11" t="inlineStr">
+      <c r="F10" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G10" s="11" t="inlineStr">
+      <c r="G10" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H10" s="11" t="inlineStr">
+      <c r="H10" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I10" s="11" t="inlineStr">
+      <c r="I10" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J10" s="11" t="inlineStr">
+      <c r="J10" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K10" s="11" t="inlineStr">
+      <c r="K10" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L10" s="11" t="inlineStr">
+      <c r="L10" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M10" s="11" t="inlineStr">
+      <c r="M10" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N10" s="11" t="inlineStr">
+      <c r="N10" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -18415,67 +18709,67 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="10" t="inlineStr">
+      <c r="B11" s="11" t="inlineStr">
         <is>
           <t>2.2</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="11" t="inlineStr">
         <is>
           <t>Database Schema Design</t>
         </is>
       </c>
-      <c r="D11" s="11" t="inlineStr">
+      <c r="D11" s="12" t="inlineStr">
         <is>
           <t>24-Apr-2024</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
+      <c r="E11" s="12" t="inlineStr">
         <is>
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F11" s="11" t="inlineStr">
+      <c r="F11" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G11" s="11" t="inlineStr">
+      <c r="G11" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H11" s="11" t="inlineStr">
+      <c r="H11" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I11" s="11" t="inlineStr">
+      <c r="I11" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J11" s="11" t="inlineStr">
+      <c r="J11" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K11" s="11" t="inlineStr">
+      <c r="K11" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L11" s="11" t="inlineStr">
+      <c r="L11" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M11" s="11" t="inlineStr">
+      <c r="M11" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N11" s="11" t="inlineStr">
+      <c r="N11" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -18519,67 +18813,67 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="11" t="inlineStr">
         <is>
           <t>2.3</t>
         </is>
       </c>
-      <c r="C12" s="10" t="inlineStr">
+      <c r="C12" s="11" t="inlineStr">
         <is>
           <t>UI/UX Design</t>
         </is>
       </c>
-      <c r="D12" s="11" t="inlineStr">
+      <c r="D12" s="12" t="inlineStr">
         <is>
           <t>01-May-2024</t>
         </is>
       </c>
-      <c r="E12" s="11" t="inlineStr">
+      <c r="E12" s="12" t="inlineStr">
         <is>
           <t>07-May-2024</t>
         </is>
       </c>
-      <c r="F12" s="11" t="inlineStr">
+      <c r="F12" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G12" s="11" t="inlineStr">
+      <c r="G12" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H12" s="11" t="inlineStr">
+      <c r="H12" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I12" s="11" t="inlineStr">
+      <c r="I12" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J12" s="11" t="inlineStr">
+      <c r="J12" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K12" s="11" t="inlineStr">
+      <c r="K12" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L12" s="11" t="inlineStr">
+      <c r="L12" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M12" s="11" t="inlineStr">
+      <c r="M12" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N12" s="11" t="inlineStr">
+      <c r="N12" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -18643,47 +18937,47 @@
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F13" s="11" t="inlineStr">
+      <c r="F13" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G13" s="11" t="inlineStr">
+      <c r="G13" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H13" s="11" t="inlineStr">
+      <c r="H13" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I13" s="11" t="inlineStr">
+      <c r="I13" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J13" s="11" t="inlineStr">
+      <c r="J13" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K13" s="11" t="inlineStr">
+      <c r="K13" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L13" s="11" t="inlineStr">
+      <c r="L13" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M13" s="11" t="inlineStr">
+      <c r="M13" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N13" s="11" t="inlineStr">
+      <c r="N13" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -18727,67 +19021,67 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="10" t="inlineStr">
+      <c r="B14" s="11" t="inlineStr">
         <is>
           <t>3.1</t>
         </is>
       </c>
-      <c r="C14" s="10" t="inlineStr">
+      <c r="C14" s="11" t="inlineStr">
         <is>
           <t>Frontend Development</t>
         </is>
       </c>
-      <c r="D14" s="11" t="inlineStr">
+      <c r="D14" s="12" t="inlineStr">
         <is>
           <t>08-May-2024</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="E14" s="12" t="inlineStr">
         <is>
           <t>14-May-2024</t>
         </is>
       </c>
-      <c r="F14" s="11" t="inlineStr">
+      <c r="F14" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G14" s="11" t="inlineStr">
+      <c r="G14" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H14" s="11" t="inlineStr">
+      <c r="H14" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I14" s="11" t="inlineStr">
+      <c r="I14" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J14" s="11" t="inlineStr">
+      <c r="J14" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K14" s="11" t="inlineStr">
+      <c r="K14" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L14" s="11" t="inlineStr">
+      <c r="L14" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M14" s="11" t="inlineStr">
+      <c r="M14" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N14" s="11" t="inlineStr">
+      <c r="N14" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -18831,67 +19125,67 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="10" t="inlineStr">
+      <c r="B15" s="11" t="inlineStr">
         <is>
           <t>3.2</t>
         </is>
       </c>
-      <c r="C15" s="10" t="inlineStr">
+      <c r="C15" s="11" t="inlineStr">
         <is>
           <t>Backend Development</t>
         </is>
       </c>
-      <c r="D15" s="11" t="inlineStr">
+      <c r="D15" s="12" t="inlineStr">
         <is>
           <t>15-May-2024</t>
         </is>
       </c>
-      <c r="E15" s="11" t="inlineStr">
+      <c r="E15" s="12" t="inlineStr">
         <is>
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F15" s="11" t="inlineStr">
+      <c r="F15" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G15" s="11" t="inlineStr">
+      <c r="G15" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H15" s="11" t="inlineStr">
+      <c r="H15" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I15" s="11" t="inlineStr">
+      <c r="I15" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J15" s="11" t="inlineStr">
+      <c r="J15" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K15" s="11" t="inlineStr">
+      <c r="K15" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L15" s="11" t="inlineStr">
+      <c r="L15" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M15" s="11" t="inlineStr">
+      <c r="M15" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N15" s="11" t="inlineStr">
+      <c r="N15" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -18935,67 +19229,67 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
-      <c r="B16" s="10" t="inlineStr">
+      <c r="B16" s="11" t="inlineStr">
         <is>
           <t>3.3</t>
         </is>
       </c>
-      <c r="C16" s="10" t="inlineStr">
+      <c r="C16" s="11" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="D16" s="11" t="inlineStr">
+      <c r="D16" s="12" t="inlineStr">
         <is>
           <t>22-May-2024</t>
         </is>
       </c>
-      <c r="E16" s="11" t="inlineStr">
+      <c r="E16" s="12" t="inlineStr">
         <is>
           <t>28-May-2024</t>
         </is>
       </c>
-      <c r="F16" s="11" t="inlineStr">
+      <c r="F16" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G16" s="11" t="inlineStr">
+      <c r="G16" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H16" s="11" t="inlineStr">
+      <c r="H16" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I16" s="11" t="inlineStr">
+      <c r="I16" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J16" s="11" t="inlineStr">
+      <c r="J16" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K16" s="11" t="inlineStr">
+      <c r="K16" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L16" s="11" t="inlineStr">
+      <c r="L16" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M16" s="11" t="inlineStr">
+      <c r="M16" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N16" s="11" t="inlineStr">
+      <c r="N16" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19059,47 +19353,47 @@
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F17" s="11" t="inlineStr">
+      <c r="F17" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G17" s="11" t="inlineStr">
+      <c r="G17" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H17" s="11" t="inlineStr">
+      <c r="H17" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I17" s="11" t="inlineStr">
+      <c r="I17" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J17" s="11" t="inlineStr">
+      <c r="J17" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K17" s="11" t="inlineStr">
+      <c r="K17" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L17" s="11" t="inlineStr">
+      <c r="L17" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M17" s="11" t="inlineStr">
+      <c r="M17" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N17" s="11" t="inlineStr">
+      <c r="N17" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19143,67 +19437,67 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="10" t="inlineStr">
+      <c r="B18" s="11" t="inlineStr">
         <is>
           <t>4.1</t>
         </is>
       </c>
-      <c r="C18" s="10" t="inlineStr">
+      <c r="C18" s="11" t="inlineStr">
         <is>
           <t>Unit Testing</t>
         </is>
       </c>
-      <c r="D18" s="11" t="inlineStr">
+      <c r="D18" s="12" t="inlineStr">
         <is>
           <t>29-May-2024</t>
         </is>
       </c>
-      <c r="E18" s="11" t="inlineStr">
+      <c r="E18" s="12" t="inlineStr">
         <is>
           <t>04-Jun-2024</t>
         </is>
       </c>
-      <c r="F18" s="11" t="inlineStr">
+      <c r="F18" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G18" s="11" t="inlineStr">
+      <c r="G18" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H18" s="11" t="inlineStr">
+      <c r="H18" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I18" s="11" t="inlineStr">
+      <c r="I18" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J18" s="11" t="inlineStr">
+      <c r="J18" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K18" s="11" t="inlineStr">
+      <c r="K18" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L18" s="11" t="inlineStr">
+      <c r="L18" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M18" s="11" t="inlineStr">
+      <c r="M18" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N18" s="11" t="inlineStr">
+      <c r="N18" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19247,67 +19541,67 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="10" t="inlineStr">
+      <c r="B19" s="11" t="inlineStr">
         <is>
           <t>4.2</t>
         </is>
       </c>
-      <c r="C19" s="10" t="inlineStr">
+      <c r="C19" s="11" t="inlineStr">
         <is>
           <t>Integration Testing</t>
         </is>
       </c>
-      <c r="D19" s="11" t="inlineStr">
+      <c r="D19" s="12" t="inlineStr">
         <is>
           <t>29-May-2024</t>
         </is>
       </c>
-      <c r="E19" s="11" t="inlineStr">
+      <c r="E19" s="12" t="inlineStr">
         <is>
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F19" s="11" t="inlineStr">
+      <c r="F19" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G19" s="11" t="inlineStr">
+      <c r="G19" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H19" s="11" t="inlineStr">
+      <c r="H19" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I19" s="11" t="inlineStr">
+      <c r="I19" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J19" s="11" t="inlineStr">
+      <c r="J19" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K19" s="11" t="inlineStr">
+      <c r="K19" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L19" s="11" t="inlineStr">
+      <c r="L19" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M19" s="11" t="inlineStr">
+      <c r="M19" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N19" s="11" t="inlineStr">
+      <c r="N19" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19351,67 +19645,67 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="10" t="inlineStr">
+      <c r="B20" s="11" t="inlineStr">
         <is>
           <t>4.3</t>
         </is>
       </c>
-      <c r="C20" s="10" t="inlineStr">
+      <c r="C20" s="11" t="inlineStr">
         <is>
           <t>User Acceptance Testing</t>
         </is>
       </c>
-      <c r="D20" s="11" t="inlineStr">
+      <c r="D20" s="12" t="inlineStr">
         <is>
           <t>05-Jun-2024</t>
         </is>
       </c>
-      <c r="E20" s="11" t="inlineStr">
+      <c r="E20" s="12" t="inlineStr">
         <is>
           <t>11-Jun-2024</t>
         </is>
       </c>
-      <c r="F20" s="11" t="inlineStr">
+      <c r="F20" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G20" s="11" t="inlineStr">
+      <c r="G20" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H20" s="11" t="inlineStr">
+      <c r="H20" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I20" s="11" t="inlineStr">
+      <c r="I20" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J20" s="11" t="inlineStr">
+      <c r="J20" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K20" s="11" t="inlineStr">
+      <c r="K20" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L20" s="11" t="inlineStr">
+      <c r="L20" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M20" s="11" t="inlineStr">
+      <c r="M20" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N20" s="11" t="inlineStr">
+      <c r="N20" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19475,47 +19769,47 @@
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F21" s="11" t="inlineStr">
+      <c r="F21" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G21" s="11" t="inlineStr">
+      <c r="G21" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H21" s="11" t="inlineStr">
+      <c r="H21" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I21" s="11" t="inlineStr">
+      <c r="I21" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J21" s="11" t="inlineStr">
+      <c r="J21" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K21" s="11" t="inlineStr">
+      <c r="K21" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L21" s="11" t="inlineStr">
+      <c r="L21" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M21" s="11" t="inlineStr">
+      <c r="M21" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N21" s="11" t="inlineStr">
+      <c r="N21" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19559,67 +19853,67 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="10" t="inlineStr">
+      <c r="B22" s="11" t="inlineStr">
         <is>
           <t>5.1</t>
         </is>
       </c>
-      <c r="C22" s="10" t="inlineStr">
+      <c r="C22" s="11" t="inlineStr">
         <is>
           <t>Prepare Deployment Environment</t>
         </is>
       </c>
-      <c r="D22" s="11" t="inlineStr">
+      <c r="D22" s="12" t="inlineStr">
         <is>
           <t>12-Jun-2024</t>
         </is>
       </c>
-      <c r="E22" s="11" t="inlineStr">
+      <c r="E22" s="12" t="inlineStr">
         <is>
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F22" s="11" t="inlineStr">
+      <c r="F22" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G22" s="11" t="inlineStr">
+      <c r="G22" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H22" s="11" t="inlineStr">
+      <c r="H22" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I22" s="11" t="inlineStr">
+      <c r="I22" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J22" s="11" t="inlineStr">
+      <c r="J22" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K22" s="11" t="inlineStr">
+      <c r="K22" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L22" s="11" t="inlineStr">
+      <c r="L22" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M22" s="11" t="inlineStr">
+      <c r="M22" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N22" s="11" t="inlineStr">
+      <c r="N22" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19663,67 +19957,67 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="10" t="inlineStr">
+      <c r="B23" s="11" t="inlineStr">
         <is>
           <t>5.2</t>
         </is>
       </c>
-      <c r="C23" s="10" t="inlineStr">
+      <c r="C23" s="11" t="inlineStr">
         <is>
           <t>Deployment</t>
         </is>
       </c>
-      <c r="D23" s="11" t="inlineStr">
+      <c r="D23" s="12" t="inlineStr">
         <is>
           <t>12-Jun-2024</t>
         </is>
       </c>
-      <c r="E23" s="11" t="inlineStr">
+      <c r="E23" s="12" t="inlineStr">
         <is>
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F23" s="11" t="inlineStr">
+      <c r="F23" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G23" s="11" t="inlineStr">
+      <c r="G23" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H23" s="11" t="inlineStr">
+      <c r="H23" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I23" s="11" t="inlineStr">
+      <c r="I23" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J23" s="11" t="inlineStr">
+      <c r="J23" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K23" s="11" t="inlineStr">
+      <c r="K23" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L23" s="11" t="inlineStr">
+      <c r="L23" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M23" s="11" t="inlineStr">
+      <c r="M23" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N23" s="11" t="inlineStr">
+      <c r="N23" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19767,67 +20061,67 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="10" t="inlineStr">
+      <c r="B24" s="11" t="inlineStr">
         <is>
           <t>5.3</t>
         </is>
       </c>
-      <c r="C24" s="10" t="inlineStr">
+      <c r="C24" s="11" t="inlineStr">
         <is>
           <t>Post-Deployment Verification</t>
         </is>
       </c>
-      <c r="D24" s="11" t="inlineStr">
+      <c r="D24" s="12" t="inlineStr">
         <is>
           <t>12-Jun-2024</t>
         </is>
       </c>
-      <c r="E24" s="11" t="inlineStr">
+      <c r="E24" s="12" t="inlineStr">
         <is>
           <t>18-Jun-2024</t>
         </is>
       </c>
-      <c r="F24" s="11" t="inlineStr">
+      <c r="F24" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G24" s="11" t="inlineStr">
+      <c r="G24" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H24" s="11" t="inlineStr">
+      <c r="H24" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I24" s="11" t="inlineStr">
+      <c r="I24" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J24" s="11" t="inlineStr">
+      <c r="J24" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K24" s="11" t="inlineStr">
+      <c r="K24" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L24" s="11" t="inlineStr">
+      <c r="L24" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M24" s="11" t="inlineStr">
+      <c r="M24" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N24" s="11" t="inlineStr">
+      <c r="N24" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19891,47 +20185,47 @@
           <t>02-Jul-2024</t>
         </is>
       </c>
-      <c r="F25" s="11" t="inlineStr">
+      <c r="F25" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G25" s="11" t="inlineStr">
+      <c r="G25" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H25" s="11" t="inlineStr">
+      <c r="H25" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I25" s="11" t="inlineStr">
+      <c r="I25" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J25" s="11" t="inlineStr">
+      <c r="J25" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K25" s="11" t="inlineStr">
+      <c r="K25" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L25" s="11" t="inlineStr">
+      <c r="L25" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M25" s="11" t="inlineStr">
+      <c r="M25" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N25" s="11" t="inlineStr">
+      <c r="N25" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -19975,67 +20269,67 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="10" t="inlineStr">
+      <c r="B26" s="11" t="inlineStr">
         <is>
           <t>6.1</t>
         </is>
       </c>
-      <c r="C26" s="10" t="inlineStr">
+      <c r="C26" s="11" t="inlineStr">
         <is>
           <t>Bug Fixing</t>
         </is>
       </c>
-      <c r="D26" s="11" t="inlineStr">
+      <c r="D26" s="12" t="inlineStr">
         <is>
           <t>19-Jun-2024</t>
         </is>
       </c>
-      <c r="E26" s="11" t="inlineStr">
+      <c r="E26" s="12" t="inlineStr">
         <is>
           <t>25-Jun-2024</t>
         </is>
       </c>
-      <c r="F26" s="11" t="inlineStr">
+      <c r="F26" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G26" s="11" t="inlineStr">
+      <c r="G26" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H26" s="11" t="inlineStr">
+      <c r="H26" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I26" s="11" t="inlineStr">
+      <c r="I26" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J26" s="11" t="inlineStr">
+      <c r="J26" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K26" s="11" t="inlineStr">
+      <c r="K26" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L26" s="11" t="inlineStr">
+      <c r="L26" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M26" s="11" t="inlineStr">
+      <c r="M26" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N26" s="11" t="inlineStr">
+      <c r="N26" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -20079,67 +20373,67 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="10" t="inlineStr">
+      <c r="B27" s="11" t="inlineStr">
         <is>
           <t>6.2</t>
         </is>
       </c>
-      <c r="C27" s="10" t="inlineStr">
+      <c r="C27" s="11" t="inlineStr">
         <is>
           <t>Performance Tuning</t>
         </is>
       </c>
-      <c r="D27" s="11" t="inlineStr">
+      <c r="D27" s="12" t="inlineStr">
         <is>
           <t>19-Jun-2024</t>
         </is>
       </c>
-      <c r="E27" s="11" t="inlineStr">
+      <c r="E27" s="12" t="inlineStr">
         <is>
           <t>25-Jun-2024</t>
         </is>
       </c>
-      <c r="F27" s="11" t="inlineStr">
+      <c r="F27" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G27" s="11" t="inlineStr">
+      <c r="G27" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H27" s="11" t="inlineStr">
+      <c r="H27" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I27" s="11" t="inlineStr">
+      <c r="I27" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J27" s="11" t="inlineStr">
+      <c r="J27" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K27" s="11" t="inlineStr">
+      <c r="K27" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L27" s="11" t="inlineStr">
+      <c r="L27" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M27" s="11" t="inlineStr">
+      <c r="M27" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N27" s="11" t="inlineStr">
+      <c r="N27" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>
@@ -20183,67 +20477,67 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="10" t="inlineStr">
+      <c r="B28" s="11" t="inlineStr">
         <is>
           <t>6.3</t>
         </is>
       </c>
-      <c r="C28" s="10" t="inlineStr">
+      <c r="C28" s="11" t="inlineStr">
         <is>
           <t>User Training</t>
         </is>
       </c>
-      <c r="D28" s="11" t="inlineStr">
+      <c r="D28" s="12" t="inlineStr">
         <is>
           <t>19-Jun-2024</t>
         </is>
       </c>
-      <c r="E28" s="11" t="inlineStr">
+      <c r="E28" s="12" t="inlineStr">
         <is>
           <t>02-Jul-2024</t>
         </is>
       </c>
-      <c r="F28" s="11" t="inlineStr">
+      <c r="F28" s="12" t="inlineStr">
         <is>
           <t>Accountable</t>
         </is>
       </c>
-      <c r="G28" s="11" t="inlineStr">
+      <c r="G28" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="H28" s="11" t="inlineStr">
+      <c r="H28" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="I28" s="11" t="inlineStr">
+      <c r="I28" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="J28" s="11" t="inlineStr">
+      <c r="J28" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="K28" s="11" t="inlineStr">
+      <c r="K28" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="L28" s="11" t="inlineStr">
+      <c r="L28" s="12" t="inlineStr">
         <is>
           <t>Consulted</t>
         </is>
       </c>
-      <c r="M28" s="11" t="inlineStr">
+      <c r="M28" s="12" t="inlineStr">
         <is>
           <t>Informed</t>
         </is>
       </c>
-      <c r="N28" s="11" t="inlineStr">
+      <c r="N28" s="12" t="inlineStr">
         <is>
           <t>Responsible</t>
         </is>

</xml_diff>

<commit_message>
New test and gif
</commit_message>
<xml_diff>
--- a/chronogram.xlsx
+++ b/chronogram.xlsx
@@ -17856,47 +17856,47 @@
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>Product Owner</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>Jane Doe</t>
+          <t>Business Analyst</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Emily Davis</t>
+          <t>Financial Lead</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>Michael Brown</t>
+          <t>Design Director</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>Olivia Johnson</t>
+          <t>CRM Lead</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>Liam Williams</t>
+          <t>Head of CRM</t>
         </is>
       </c>
       <c r="L1" s="2" t="inlineStr">
         <is>
-          <t>Sophia Martinez</t>
+          <t>Senior Stakeholder*</t>
         </is>
       </c>
       <c r="M1" s="2" t="inlineStr">
         <is>
-          <t>William Garcia</t>
+          <t>Senior Stakeholder**</t>
         </is>
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>Ava Lee</t>
+          <t>AGENCY</t>
         </is>
       </c>
       <c r="O1" s="17" t="n"/>

</xml_diff>